<commit_message>
Conditionally validate the data when updating an existing record
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/3.create-update-and-delete-individual-resources.xlsx
+++ b/me/4.create-a-restful-api/3.create-update-and-delete-individual-resources.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA241380-8104-49C6-927A-04F16EF0362F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD907677-2315-4268-AC68-993F3A3685B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="get request JSON data" sheetId="1" r:id="rId1"/>
     <sheet name="Insert a record 201 status code" sheetId="2" r:id="rId2"/>
     <sheet name="add generic error handler" sheetId="3" r:id="rId3"/>
     <sheet name="Validate data respond 422status" sheetId="4" r:id="rId4"/>
+    <sheet name="validate update existing record" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="252">
   <si>
     <t>構成</t>
   </si>
@@ -871,6 +872,95 @@
   </si>
   <si>
     <t>Trường hợp truyền data ko có vấn đề thì insert bình thường</t>
+  </si>
+  <si>
+    <t>Conditionally validate the data when updating an existing record</t>
+  </si>
+  <si>
+    <t>Cũng giống như trường hợp insert thì đối với trường hợp update thì mình cũng nhận data được truyền đến rồi validate data đó</t>
+  </si>
+  <si>
+    <t>Tuy nhiên khác với trường hợp insert thì đối với trường hợp update thì mình ko cần validate cho trường field là bắt buộc phải được truyền lên</t>
+  </si>
+  <si>
+    <t>                    $data = (array) json_decode(file_get_contents("php://input"), true);</t>
+  </si>
+  <si>
+    <t>                    $errors = $this-&gt;getValidationErrors($data, false);</t>
+  </si>
+  <si>
+    <t>                    if (!empty($errors)) {</t>
+  </si>
+  <si>
+    <t>                        $this-&gt;respondUnprocessableEntity($errors);</t>
+  </si>
+  <si>
+    <t>                        return;</t>
+  </si>
+  <si>
+    <t>                    }</t>
+  </si>
+  <si>
+    <r>
+      <t>    private function getValidationErrors(array $data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, bool $is_new = true</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>): array</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        if (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">$is_new &amp;&amp; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>empty($data["name"])) {</t>
+    </r>
+  </si>
+  <si>
+    <t>hợp update thì ko cần validate required</t>
+  </si>
+  <si>
+    <t>Đối với trường hợp insert thì mới phải validate cho trường name là required, còn đối với trường</t>
+  </si>
+  <si>
+    <t>trường hợp này là update nên ko cần validate required</t>
+  </si>
+  <si>
+    <t>call api để update data, data truyền lên ko cần chứa trường name, response trả về là OK(200)</t>
   </si>
 </sst>
 </file>
@@ -4664,6 +4754,267 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0080E2A6-CAE6-2116-83AC-155CDE9FBF14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1466850" y="26079450"/>
+          <a:ext cx="2609850" cy="666750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B544E564-99B7-2E01-CC3A-4988684EFC41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3829050" y="17497425"/>
+          <a:ext cx="762000" cy="8477250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>408320</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>37558</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D199340B-4E12-EFB7-2A4B-A3B8DDED7182}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="30565725"/>
+          <a:ext cx="10038095" cy="4333333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A753C0D-2E51-C709-9D88-CE87D22CA1D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2190750" y="30470475"/>
+          <a:ext cx="1304925" cy="1457325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4E2B5A1-AA90-0698-73CC-460307AE383D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5686425" y="30432375"/>
+          <a:ext cx="3800475" cy="3086100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -20761,8 +21112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA3CFD4-718E-4844-AF2F-8F8B9DAF029D}">
   <dimension ref="A2:T320"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A316" workbookViewId="0">
-      <selection activeCell="F326" sqref="F326"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:L66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25863,4 +26214,2251 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D565EF0-601C-40DC-B5D3-AD4BBA1DD3AA}">
+  <dimension ref="A2:R185"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="B2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="4"/>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="4"/>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="4"/>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="4"/>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="4"/>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="2:12">
+      <c r="B19" s="4"/>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20" s="4"/>
+      <c r="F20" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="4"/>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="4"/>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="B23" s="4"/>
+      <c r="F23" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="4"/>
+      <c r="F24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="5"/>
+      <c r="K24" t="s">
+        <v>17</v>
+      </c>
+      <c r="L24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" s="4"/>
+      <c r="F25" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" s="4"/>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" s="4"/>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="B28" s="4"/>
+      <c r="E28" t="s">
+        <v>22</v>
+      </c>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="B29" s="4"/>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" s="4"/>
+      <c r="E30" t="s">
+        <v>24</v>
+      </c>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="9"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="B36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="B37" s="4"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="B38" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="B39" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="B40" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="B41" s="4"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="B42" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="B43" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="B44" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="B45" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="B46" s="4"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="B47" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="B48" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" s="4"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="B51" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" s="4"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="B54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" s="4"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="B57" s="4"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="2:10">
+      <c r="B59" s="4"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="2:10">
+      <c r="B60" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="2:10">
+      <c r="B61" s="4"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="2:10">
+      <c r="B62" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="B63" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="B64" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" s="4"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="2:10">
+      <c r="B66" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="2:10">
+      <c r="B67" s="4"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="2:10">
+      <c r="B68" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="2:10">
+      <c r="B69" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="2:10">
+      <c r="B70" s="4"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="2:10">
+      <c r="B71" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="2:10">
+      <c r="B72" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="2:10">
+      <c r="B73" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" spans="2:10">
+      <c r="B74" s="4"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="2:10">
+      <c r="B75" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" spans="2:10">
+      <c r="B76" s="4"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="5"/>
+    </row>
+    <row r="77" spans="2:10">
+      <c r="B77" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="5"/>
+    </row>
+    <row r="78" spans="2:10">
+      <c r="B78" s="4"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="5"/>
+    </row>
+    <row r="79" spans="2:10">
+      <c r="B79" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" spans="2:10">
+      <c r="B80" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="5"/>
+    </row>
+    <row r="81" spans="2:12">
+      <c r="B81" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="5"/>
+    </row>
+    <row r="82" spans="2:12">
+      <c r="B82" s="4"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="5"/>
+    </row>
+    <row r="83" spans="2:12">
+      <c r="B83" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="5"/>
+    </row>
+    <row r="84" spans="2:12">
+      <c r="B84" s="4"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="5"/>
+    </row>
+    <row r="85" spans="2:12">
+      <c r="B85" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="5"/>
+    </row>
+    <row r="86" spans="2:12">
+      <c r="B86" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="5"/>
+    </row>
+    <row r="87" spans="2:12">
+      <c r="B87" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="5"/>
+    </row>
+    <row r="88" spans="2:12">
+      <c r="B88" s="4"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="5"/>
+    </row>
+    <row r="89" spans="2:12">
+      <c r="B89" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="5"/>
+    </row>
+    <row r="90" spans="2:12">
+      <c r="B90" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="5"/>
+    </row>
+    <row r="91" spans="2:12">
+      <c r="B91" s="14"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="5"/>
+    </row>
+    <row r="92" spans="2:12">
+      <c r="B92" s="14" t="s">
+        <v>241</v>
+      </c>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="5"/>
+      <c r="K92" t="s">
+        <v>17</v>
+      </c>
+      <c r="L92" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="93" spans="2:12">
+      <c r="B93" s="14"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="5"/>
+    </row>
+    <row r="94" spans="2:12">
+      <c r="B94" s="14" t="s">
+        <v>242</v>
+      </c>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="5"/>
+    </row>
+    <row r="95" spans="2:12">
+      <c r="B95" s="14"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="5"/>
+    </row>
+    <row r="96" spans="2:12">
+      <c r="B96" s="14" t="s">
+        <v>243</v>
+      </c>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="5"/>
+    </row>
+    <row r="97" spans="2:10">
+      <c r="B97" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="13"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="5"/>
+    </row>
+    <row r="98" spans="2:10">
+      <c r="B98" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="5"/>
+    </row>
+    <row r="99" spans="2:10">
+      <c r="B99" s="4"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="5"/>
+    </row>
+    <row r="100" spans="2:10">
+      <c r="B100" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="5"/>
+    </row>
+    <row r="101" spans="2:10">
+      <c r="B101" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="5"/>
+    </row>
+    <row r="102" spans="2:10">
+      <c r="B102" s="4"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="5"/>
+    </row>
+    <row r="103" spans="2:10">
+      <c r="B103" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="13"/>
+      <c r="G103" s="13"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="5"/>
+    </row>
+    <row r="104" spans="2:10">
+      <c r="B104" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C104" s="13"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="13"/>
+      <c r="G104" s="13"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="5"/>
+    </row>
+    <row r="105" spans="2:10">
+      <c r="B105" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C105" s="13"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="13"/>
+      <c r="I105" s="13"/>
+      <c r="J105" s="5"/>
+    </row>
+    <row r="106" spans="2:10">
+      <c r="B106" s="4"/>
+      <c r="C106" s="13"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
+      <c r="F106" s="13"/>
+      <c r="G106" s="13"/>
+      <c r="H106" s="13"/>
+      <c r="I106" s="13"/>
+      <c r="J106" s="5"/>
+    </row>
+    <row r="107" spans="2:10">
+      <c r="B107" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="5"/>
+    </row>
+    <row r="108" spans="2:10">
+      <c r="B108" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="5"/>
+    </row>
+    <row r="109" spans="2:10">
+      <c r="B109" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C109" s="13"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="13"/>
+      <c r="G109" s="13"/>
+      <c r="H109" s="13"/>
+      <c r="I109" s="13"/>
+      <c r="J109" s="5"/>
+    </row>
+    <row r="110" spans="2:10">
+      <c r="B110" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="13"/>
+      <c r="H110" s="13"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="5"/>
+    </row>
+    <row r="111" spans="2:10">
+      <c r="B111" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="5"/>
+    </row>
+    <row r="112" spans="2:10">
+      <c r="B112" s="4"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="13"/>
+      <c r="J112" s="5"/>
+    </row>
+    <row r="113" spans="2:10">
+      <c r="B113" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C113" s="13"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
+      <c r="G113" s="13"/>
+      <c r="H113" s="13"/>
+      <c r="I113" s="13"/>
+      <c r="J113" s="5"/>
+    </row>
+    <row r="114" spans="2:10">
+      <c r="B114" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" s="13"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="13"/>
+      <c r="G114" s="13"/>
+      <c r="H114" s="13"/>
+      <c r="I114" s="13"/>
+      <c r="J114" s="5"/>
+    </row>
+    <row r="115" spans="2:10">
+      <c r="B115" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C115" s="13"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13"/>
+      <c r="G115" s="13"/>
+      <c r="H115" s="13"/>
+      <c r="I115" s="13"/>
+      <c r="J115" s="5"/>
+    </row>
+    <row r="116" spans="2:10">
+      <c r="B116" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C116" s="13"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
+      <c r="F116" s="13"/>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="13"/>
+      <c r="J116" s="5"/>
+    </row>
+    <row r="117" spans="2:10">
+      <c r="B117" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C117" s="13"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="13"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="5"/>
+    </row>
+    <row r="118" spans="2:10">
+      <c r="B118" s="4"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="13"/>
+      <c r="G118" s="13"/>
+      <c r="H118" s="13"/>
+      <c r="I118" s="13"/>
+      <c r="J118" s="5"/>
+    </row>
+    <row r="119" spans="2:10">
+      <c r="B119" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13"/>
+      <c r="G119" s="13"/>
+      <c r="H119" s="13"/>
+      <c r="I119" s="13"/>
+      <c r="J119" s="5"/>
+    </row>
+    <row r="120" spans="2:10">
+      <c r="B120" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="13"/>
+      <c r="J120" s="5"/>
+    </row>
+    <row r="121" spans="2:10">
+      <c r="B121" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
+      <c r="F121" s="13"/>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="13"/>
+      <c r="J121" s="5"/>
+    </row>
+    <row r="122" spans="2:10">
+      <c r="B122" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
+      <c r="G122" s="13"/>
+      <c r="H122" s="13"/>
+      <c r="I122" s="13"/>
+      <c r="J122" s="5"/>
+    </row>
+    <row r="123" spans="2:10">
+      <c r="B123" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C123" s="13"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="13"/>
+      <c r="G123" s="13"/>
+      <c r="H123" s="13"/>
+      <c r="I123" s="13"/>
+      <c r="J123" s="5"/>
+    </row>
+    <row r="124" spans="2:10">
+      <c r="B124" s="4"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
+      <c r="F124" s="13"/>
+      <c r="G124" s="13"/>
+      <c r="H124" s="13"/>
+      <c r="I124" s="13"/>
+      <c r="J124" s="5"/>
+    </row>
+    <row r="125" spans="2:10">
+      <c r="B125" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
+      <c r="F125" s="13"/>
+      <c r="G125" s="13"/>
+      <c r="H125" s="13"/>
+      <c r="I125" s="13"/>
+      <c r="J125" s="5"/>
+    </row>
+    <row r="126" spans="2:10">
+      <c r="B126" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="13"/>
+      <c r="G126" s="13"/>
+      <c r="H126" s="13"/>
+      <c r="I126" s="13"/>
+      <c r="J126" s="5"/>
+    </row>
+    <row r="127" spans="2:10">
+      <c r="B127" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="13"/>
+      <c r="F127" s="13"/>
+      <c r="G127" s="13"/>
+      <c r="H127" s="13"/>
+      <c r="I127" s="13"/>
+      <c r="J127" s="5"/>
+    </row>
+    <row r="128" spans="2:10">
+      <c r="B128" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="13"/>
+      <c r="F128" s="13"/>
+      <c r="G128" s="13"/>
+      <c r="H128" s="13"/>
+      <c r="I128" s="13"/>
+      <c r="J128" s="5"/>
+    </row>
+    <row r="129" spans="2:12">
+      <c r="B129" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C129" s="13"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="13"/>
+      <c r="G129" s="13"/>
+      <c r="H129" s="13"/>
+      <c r="I129" s="13"/>
+      <c r="J129" s="5"/>
+    </row>
+    <row r="130" spans="2:12">
+      <c r="B130" s="4"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="13"/>
+      <c r="F130" s="13"/>
+      <c r="G130" s="13"/>
+      <c r="H130" s="13"/>
+      <c r="I130" s="13"/>
+      <c r="J130" s="5"/>
+    </row>
+    <row r="131" spans="2:12">
+      <c r="B131" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="13"/>
+      <c r="G131" s="13"/>
+      <c r="H131" s="13"/>
+      <c r="I131" s="13"/>
+      <c r="J131" s="5"/>
+    </row>
+    <row r="132" spans="2:12">
+      <c r="B132" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="13"/>
+      <c r="F132" s="13"/>
+      <c r="G132" s="13"/>
+      <c r="H132" s="13"/>
+      <c r="I132" s="13"/>
+      <c r="J132" s="5"/>
+    </row>
+    <row r="133" spans="2:12">
+      <c r="B133" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="13"/>
+      <c r="G133" s="13"/>
+      <c r="H133" s="13"/>
+      <c r="I133" s="13"/>
+      <c r="J133" s="5"/>
+    </row>
+    <row r="134" spans="2:12">
+      <c r="B134" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13"/>
+      <c r="F134" s="13"/>
+      <c r="G134" s="13"/>
+      <c r="H134" s="13"/>
+      <c r="I134" s="13"/>
+      <c r="J134" s="5"/>
+    </row>
+    <row r="135" spans="2:12">
+      <c r="B135" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C135" s="13"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="13"/>
+      <c r="F135" s="13"/>
+      <c r="G135" s="13"/>
+      <c r="H135" s="13"/>
+      <c r="I135" s="13"/>
+      <c r="J135" s="5"/>
+    </row>
+    <row r="136" spans="2:12">
+      <c r="B136" s="4"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="13"/>
+      <c r="G136" s="13"/>
+      <c r="H136" s="13"/>
+      <c r="I136" s="13"/>
+      <c r="J136" s="5"/>
+    </row>
+    <row r="137" spans="2:12">
+      <c r="B137" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="C137" s="13"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
+      <c r="H137" s="13"/>
+      <c r="I137" s="13"/>
+      <c r="J137" s="5"/>
+    </row>
+    <row r="138" spans="2:12">
+      <c r="B138" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C138" s="13"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="13"/>
+      <c r="G138" s="13"/>
+      <c r="H138" s="13"/>
+      <c r="I138" s="13"/>
+      <c r="J138" s="5"/>
+    </row>
+    <row r="139" spans="2:12">
+      <c r="B139" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C139" s="13"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="13"/>
+      <c r="F139" s="13"/>
+      <c r="G139" s="13"/>
+      <c r="H139" s="13"/>
+      <c r="I139" s="13"/>
+      <c r="J139" s="5"/>
+    </row>
+    <row r="140" spans="2:12">
+      <c r="B140" s="4"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
+      <c r="H140" s="13"/>
+      <c r="I140" s="13"/>
+      <c r="J140" s="5"/>
+    </row>
+    <row r="141" spans="2:12">
+      <c r="B141" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C141" s="13"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="13"/>
+      <c r="F141" s="13"/>
+      <c r="G141" s="13"/>
+      <c r="H141" s="13"/>
+      <c r="I141" s="13"/>
+      <c r="J141" s="5"/>
+      <c r="K141" t="s">
+        <v>17</v>
+      </c>
+      <c r="L141" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="142" spans="2:12">
+      <c r="B142" s="4"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
+      <c r="F142" s="13"/>
+      <c r="G142" s="13"/>
+      <c r="H142" s="13"/>
+      <c r="I142" s="13"/>
+      <c r="J142" s="5"/>
+      <c r="L142" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="143" spans="2:12">
+      <c r="B143" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
+      <c r="F143" s="13"/>
+      <c r="G143" s="13"/>
+      <c r="H143" s="13"/>
+      <c r="I143" s="13"/>
+      <c r="J143" s="5"/>
+    </row>
+    <row r="144" spans="2:12">
+      <c r="B144" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C144" s="13"/>
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
+      <c r="F144" s="13"/>
+      <c r="G144" s="13"/>
+      <c r="H144" s="13"/>
+      <c r="I144" s="13"/>
+      <c r="J144" s="5"/>
+    </row>
+    <row r="145" spans="1:18">
+      <c r="B145" s="4"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
+      <c r="F145" s="13"/>
+      <c r="G145" s="13"/>
+      <c r="H145" s="13"/>
+      <c r="I145" s="13"/>
+      <c r="J145" s="5"/>
+    </row>
+    <row r="146" spans="1:18">
+      <c r="B146" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C146" s="13"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
+      <c r="F146" s="13"/>
+      <c r="G146" s="13"/>
+      <c r="H146" s="13"/>
+      <c r="I146" s="13"/>
+      <c r="J146" s="5"/>
+    </row>
+    <row r="147" spans="1:18">
+      <c r="B147" s="4"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="13"/>
+      <c r="G147" s="13"/>
+      <c r="H147" s="13"/>
+      <c r="I147" s="13"/>
+      <c r="J147" s="5"/>
+    </row>
+    <row r="148" spans="1:18">
+      <c r="B148" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C148" s="13"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
+      <c r="F148" s="13"/>
+      <c r="G148" s="13"/>
+      <c r="H148" s="13"/>
+      <c r="I148" s="13"/>
+      <c r="J148" s="5"/>
+    </row>
+    <row r="149" spans="1:18">
+      <c r="B149" s="4"/>
+      <c r="C149" s="13"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
+      <c r="F149" s="13"/>
+      <c r="G149" s="13"/>
+      <c r="H149" s="13"/>
+      <c r="I149" s="13"/>
+      <c r="J149" s="5"/>
+    </row>
+    <row r="150" spans="1:18">
+      <c r="B150" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C150" s="13"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
+      <c r="F150" s="13"/>
+      <c r="G150" s="13"/>
+      <c r="H150" s="13"/>
+      <c r="I150" s="13"/>
+      <c r="J150" s="5"/>
+    </row>
+    <row r="151" spans="1:18">
+      <c r="B151" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C151" s="13"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="13"/>
+      <c r="F151" s="13"/>
+      <c r="G151" s="13"/>
+      <c r="H151" s="13"/>
+      <c r="I151" s="13"/>
+      <c r="J151" s="5"/>
+    </row>
+    <row r="152" spans="1:18">
+      <c r="B152" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C152" s="13"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="13"/>
+      <c r="F152" s="13"/>
+      <c r="G152" s="13"/>
+      <c r="H152" s="13"/>
+      <c r="I152" s="13"/>
+      <c r="J152" s="5"/>
+    </row>
+    <row r="153" spans="1:18">
+      <c r="B153" s="4"/>
+      <c r="C153" s="13"/>
+      <c r="D153" s="13"/>
+      <c r="E153" s="13"/>
+      <c r="F153" s="13"/>
+      <c r="G153" s="13"/>
+      <c r="H153" s="13"/>
+      <c r="I153" s="13"/>
+      <c r="J153" s="5"/>
+    </row>
+    <row r="154" spans="1:18">
+      <c r="B154" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C154" s="13"/>
+      <c r="D154" s="13"/>
+      <c r="E154" s="13"/>
+      <c r="F154" s="13"/>
+      <c r="G154" s="13"/>
+      <c r="H154" s="13"/>
+      <c r="I154" s="13"/>
+      <c r="J154" s="5"/>
+    </row>
+    <row r="155" spans="1:18">
+      <c r="B155" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C155" s="13"/>
+      <c r="D155" s="13"/>
+      <c r="E155" s="13"/>
+      <c r="F155" s="13"/>
+      <c r="G155" s="13"/>
+      <c r="H155" s="13"/>
+      <c r="I155" s="13"/>
+      <c r="J155" s="5"/>
+    </row>
+    <row r="156" spans="1:18">
+      <c r="B156" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C156" s="8"/>
+      <c r="D156" s="8"/>
+      <c r="E156" s="8"/>
+      <c r="F156" s="8"/>
+      <c r="G156" s="8"/>
+      <c r="H156" s="8"/>
+      <c r="I156" s="8"/>
+      <c r="J156" s="9"/>
+    </row>
+    <row r="159" spans="1:18">
+      <c r="A159" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="160" spans="1:18">
+      <c r="B160" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C160" s="2"/>
+      <c r="D160" s="2"/>
+      <c r="E160" s="2"/>
+      <c r="F160" s="2"/>
+      <c r="G160" s="2"/>
+      <c r="H160" s="2"/>
+      <c r="I160" s="2"/>
+      <c r="J160" s="2"/>
+      <c r="K160" s="2"/>
+      <c r="L160" s="2"/>
+      <c r="M160" s="2"/>
+      <c r="N160" s="2"/>
+      <c r="O160" s="2"/>
+      <c r="P160" s="2"/>
+      <c r="Q160" s="2"/>
+      <c r="R160" s="3"/>
+    </row>
+    <row r="161" spans="2:18">
+      <c r="B161" s="4"/>
+      <c r="C161" s="13"/>
+      <c r="D161" s="13"/>
+      <c r="E161" s="13"/>
+      <c r="F161" s="13"/>
+      <c r="G161" s="13"/>
+      <c r="H161" s="13"/>
+      <c r="I161" s="13"/>
+      <c r="J161" s="13"/>
+      <c r="K161" s="13"/>
+      <c r="L161" s="13"/>
+      <c r="M161" s="13"/>
+      <c r="N161" s="13"/>
+      <c r="O161" s="13"/>
+      <c r="P161" s="13"/>
+      <c r="Q161" s="13"/>
+      <c r="R161" s="5"/>
+    </row>
+    <row r="162" spans="2:18">
+      <c r="B162" s="4"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="13"/>
+      <c r="F162" s="13"/>
+      <c r="G162" s="13"/>
+      <c r="H162" s="13"/>
+      <c r="I162" s="13"/>
+      <c r="J162" s="13"/>
+      <c r="K162" s="13"/>
+      <c r="L162" s="13"/>
+      <c r="M162" s="13"/>
+      <c r="N162" s="13"/>
+      <c r="O162" s="13"/>
+      <c r="P162" s="13"/>
+      <c r="Q162" s="13"/>
+      <c r="R162" s="5"/>
+    </row>
+    <row r="163" spans="2:18">
+      <c r="B163" s="4"/>
+      <c r="C163" s="13"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="13"/>
+      <c r="F163" s="13"/>
+      <c r="G163" s="13"/>
+      <c r="H163" s="13"/>
+      <c r="I163" s="13"/>
+      <c r="J163" s="13"/>
+      <c r="K163" s="13"/>
+      <c r="L163" s="13"/>
+      <c r="M163" s="13"/>
+      <c r="N163" s="13"/>
+      <c r="O163" s="13"/>
+      <c r="P163" s="13"/>
+      <c r="Q163" s="13"/>
+      <c r="R163" s="5"/>
+    </row>
+    <row r="164" spans="2:18">
+      <c r="B164" s="4"/>
+      <c r="C164" s="13"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="13"/>
+      <c r="F164" s="13"/>
+      <c r="G164" s="13"/>
+      <c r="H164" s="13"/>
+      <c r="I164" s="13"/>
+      <c r="J164" s="13"/>
+      <c r="K164" s="13"/>
+      <c r="L164" s="13"/>
+      <c r="M164" s="13"/>
+      <c r="N164" s="13"/>
+      <c r="O164" s="13"/>
+      <c r="P164" s="13"/>
+      <c r="Q164" s="13"/>
+      <c r="R164" s="5"/>
+    </row>
+    <row r="165" spans="2:18">
+      <c r="B165" s="4"/>
+      <c r="C165" s="13"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="13"/>
+      <c r="F165" s="13"/>
+      <c r="G165" s="13"/>
+      <c r="H165" s="13"/>
+      <c r="I165" s="13"/>
+      <c r="J165" s="13"/>
+      <c r="K165" s="13"/>
+      <c r="L165" s="13"/>
+      <c r="M165" s="13"/>
+      <c r="N165" s="13"/>
+      <c r="O165" s="13"/>
+      <c r="P165" s="13"/>
+      <c r="Q165" s="13"/>
+      <c r="R165" s="5"/>
+    </row>
+    <row r="166" spans="2:18">
+      <c r="B166" s="4"/>
+      <c r="C166" s="13"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="13"/>
+      <c r="F166" s="13"/>
+      <c r="G166" s="13"/>
+      <c r="H166" s="13"/>
+      <c r="I166" s="13"/>
+      <c r="J166" s="13"/>
+      <c r="K166" s="13"/>
+      <c r="L166" s="13"/>
+      <c r="M166" s="13"/>
+      <c r="N166" s="13"/>
+      <c r="O166" s="13"/>
+      <c r="P166" s="13"/>
+      <c r="Q166" s="13"/>
+      <c r="R166" s="5"/>
+    </row>
+    <row r="167" spans="2:18">
+      <c r="B167" s="4"/>
+      <c r="C167" s="13"/>
+      <c r="D167" s="13"/>
+      <c r="E167" s="13"/>
+      <c r="F167" s="13"/>
+      <c r="G167" s="13"/>
+      <c r="H167" s="13"/>
+      <c r="I167" s="13"/>
+      <c r="J167" s="13"/>
+      <c r="K167" s="13"/>
+      <c r="L167" s="13"/>
+      <c r="M167" s="13"/>
+      <c r="N167" s="13"/>
+      <c r="O167" s="13"/>
+      <c r="P167" s="13"/>
+      <c r="Q167" s="13"/>
+      <c r="R167" s="5"/>
+    </row>
+    <row r="168" spans="2:18">
+      <c r="B168" s="4"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="13"/>
+      <c r="F168" s="13"/>
+      <c r="G168" s="13"/>
+      <c r="H168" s="13"/>
+      <c r="I168" s="13"/>
+      <c r="J168" s="13"/>
+      <c r="K168" s="13"/>
+      <c r="L168" s="13"/>
+      <c r="M168" s="13"/>
+      <c r="N168" s="13"/>
+      <c r="O168" s="13"/>
+      <c r="P168" s="13"/>
+      <c r="Q168" s="13"/>
+      <c r="R168" s="5"/>
+    </row>
+    <row r="169" spans="2:18">
+      <c r="B169" s="4"/>
+      <c r="C169" s="13"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="13"/>
+      <c r="F169" s="13"/>
+      <c r="G169" s="13"/>
+      <c r="H169" s="13"/>
+      <c r="I169" s="13"/>
+      <c r="J169" s="13"/>
+      <c r="K169" s="13"/>
+      <c r="L169" s="13"/>
+      <c r="M169" s="13"/>
+      <c r="N169" s="13"/>
+      <c r="O169" s="13"/>
+      <c r="P169" s="13"/>
+      <c r="Q169" s="13"/>
+      <c r="R169" s="5"/>
+    </row>
+    <row r="170" spans="2:18">
+      <c r="B170" s="4"/>
+      <c r="C170" s="13"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="13"/>
+      <c r="F170" s="13"/>
+      <c r="G170" s="13"/>
+      <c r="H170" s="13"/>
+      <c r="I170" s="13"/>
+      <c r="J170" s="13"/>
+      <c r="K170" s="13"/>
+      <c r="L170" s="13"/>
+      <c r="M170" s="13"/>
+      <c r="N170" s="13"/>
+      <c r="O170" s="13"/>
+      <c r="P170" s="13"/>
+      <c r="Q170" s="13"/>
+      <c r="R170" s="5"/>
+    </row>
+    <row r="171" spans="2:18">
+      <c r="B171" s="4"/>
+      <c r="C171" s="13"/>
+      <c r="D171" s="13"/>
+      <c r="E171" s="13"/>
+      <c r="F171" s="13"/>
+      <c r="G171" s="13"/>
+      <c r="H171" s="13"/>
+      <c r="I171" s="13"/>
+      <c r="J171" s="13"/>
+      <c r="K171" s="13"/>
+      <c r="L171" s="13"/>
+      <c r="M171" s="13"/>
+      <c r="N171" s="13"/>
+      <c r="O171" s="13"/>
+      <c r="P171" s="13"/>
+      <c r="Q171" s="13"/>
+      <c r="R171" s="5"/>
+    </row>
+    <row r="172" spans="2:18">
+      <c r="B172" s="4"/>
+      <c r="C172" s="13"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="13"/>
+      <c r="F172" s="13"/>
+      <c r="G172" s="13"/>
+      <c r="H172" s="13"/>
+      <c r="I172" s="13"/>
+      <c r="J172" s="13"/>
+      <c r="K172" s="13"/>
+      <c r="L172" s="13"/>
+      <c r="M172" s="13"/>
+      <c r="N172" s="13"/>
+      <c r="O172" s="13"/>
+      <c r="P172" s="13"/>
+      <c r="Q172" s="13"/>
+      <c r="R172" s="5"/>
+    </row>
+    <row r="173" spans="2:18">
+      <c r="B173" s="4"/>
+      <c r="C173" s="13"/>
+      <c r="D173" s="13"/>
+      <c r="E173" s="13"/>
+      <c r="F173" s="13"/>
+      <c r="G173" s="13"/>
+      <c r="H173" s="13"/>
+      <c r="I173" s="13"/>
+      <c r="J173" s="13"/>
+      <c r="K173" s="13"/>
+      <c r="L173" s="13"/>
+      <c r="M173" s="13"/>
+      <c r="N173" s="13"/>
+      <c r="O173" s="13"/>
+      <c r="P173" s="13"/>
+      <c r="Q173" s="13"/>
+      <c r="R173" s="5"/>
+    </row>
+    <row r="174" spans="2:18">
+      <c r="B174" s="4"/>
+      <c r="C174" s="13"/>
+      <c r="D174" s="13"/>
+      <c r="E174" s="13"/>
+      <c r="F174" s="13"/>
+      <c r="G174" s="13"/>
+      <c r="H174" s="13"/>
+      <c r="I174" s="13"/>
+      <c r="J174" s="13"/>
+      <c r="K174" s="13"/>
+      <c r="L174" s="13"/>
+      <c r="M174" s="13"/>
+      <c r="N174" s="13"/>
+      <c r="O174" s="13"/>
+      <c r="P174" s="13"/>
+      <c r="Q174" s="13"/>
+      <c r="R174" s="5"/>
+    </row>
+    <row r="175" spans="2:18">
+      <c r="B175" s="4"/>
+      <c r="C175" s="13"/>
+      <c r="D175" s="13"/>
+      <c r="E175" s="13"/>
+      <c r="F175" s="13"/>
+      <c r="G175" s="13"/>
+      <c r="H175" s="13"/>
+      <c r="I175" s="13"/>
+      <c r="J175" s="13"/>
+      <c r="K175" s="13"/>
+      <c r="L175" s="13"/>
+      <c r="M175" s="13"/>
+      <c r="N175" s="13"/>
+      <c r="O175" s="13"/>
+      <c r="P175" s="13"/>
+      <c r="Q175" s="13"/>
+      <c r="R175" s="5"/>
+    </row>
+    <row r="176" spans="2:18">
+      <c r="B176" s="4"/>
+      <c r="C176" s="13"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="13"/>
+      <c r="F176" s="13"/>
+      <c r="G176" s="13"/>
+      <c r="H176" s="13"/>
+      <c r="I176" s="13"/>
+      <c r="J176" s="13"/>
+      <c r="K176" s="13"/>
+      <c r="L176" s="13"/>
+      <c r="M176" s="13"/>
+      <c r="N176" s="13"/>
+      <c r="O176" s="13"/>
+      <c r="P176" s="13"/>
+      <c r="Q176" s="13"/>
+      <c r="R176" s="5"/>
+    </row>
+    <row r="177" spans="2:18">
+      <c r="B177" s="4"/>
+      <c r="C177" s="13"/>
+      <c r="D177" s="13"/>
+      <c r="E177" s="13"/>
+      <c r="F177" s="13"/>
+      <c r="G177" s="13"/>
+      <c r="H177" s="13"/>
+      <c r="I177" s="13"/>
+      <c r="J177" s="13"/>
+      <c r="K177" s="13"/>
+      <c r="L177" s="13"/>
+      <c r="M177" s="13"/>
+      <c r="N177" s="13"/>
+      <c r="O177" s="13"/>
+      <c r="P177" s="13"/>
+      <c r="Q177" s="13"/>
+      <c r="R177" s="5"/>
+    </row>
+    <row r="178" spans="2:18">
+      <c r="B178" s="4"/>
+      <c r="C178" s="13"/>
+      <c r="D178" s="13"/>
+      <c r="E178" s="13"/>
+      <c r="F178" s="13"/>
+      <c r="G178" s="13"/>
+      <c r="H178" s="13"/>
+      <c r="I178" s="13"/>
+      <c r="J178" s="13"/>
+      <c r="K178" s="13"/>
+      <c r="L178" s="13"/>
+      <c r="M178" s="13"/>
+      <c r="N178" s="13"/>
+      <c r="O178" s="13"/>
+      <c r="P178" s="13"/>
+      <c r="Q178" s="13"/>
+      <c r="R178" s="5"/>
+    </row>
+    <row r="179" spans="2:18">
+      <c r="B179" s="4"/>
+      <c r="C179" s="13"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13"/>
+      <c r="F179" s="13"/>
+      <c r="G179" s="13"/>
+      <c r="H179" s="13"/>
+      <c r="I179" s="13"/>
+      <c r="J179" s="13"/>
+      <c r="K179" s="13"/>
+      <c r="L179" s="13"/>
+      <c r="M179" s="13"/>
+      <c r="N179" s="13"/>
+      <c r="O179" s="13"/>
+      <c r="P179" s="13"/>
+      <c r="Q179" s="13"/>
+      <c r="R179" s="5"/>
+    </row>
+    <row r="180" spans="2:18">
+      <c r="B180" s="4"/>
+      <c r="C180" s="13"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13"/>
+      <c r="F180" s="13"/>
+      <c r="G180" s="13"/>
+      <c r="H180" s="13"/>
+      <c r="I180" s="13"/>
+      <c r="J180" s="13"/>
+      <c r="K180" s="13"/>
+      <c r="L180" s="13"/>
+      <c r="M180" s="13"/>
+      <c r="N180" s="13"/>
+      <c r="O180" s="13"/>
+      <c r="P180" s="13"/>
+      <c r="Q180" s="13"/>
+      <c r="R180" s="5"/>
+    </row>
+    <row r="181" spans="2:18">
+      <c r="B181" s="4"/>
+      <c r="C181" s="13"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="13"/>
+      <c r="F181" s="13"/>
+      <c r="G181" s="13"/>
+      <c r="H181" s="13"/>
+      <c r="I181" s="13"/>
+      <c r="J181" s="13"/>
+      <c r="K181" s="13"/>
+      <c r="L181" s="13"/>
+      <c r="M181" s="13"/>
+      <c r="N181" s="13"/>
+      <c r="O181" s="13"/>
+      <c r="P181" s="13"/>
+      <c r="Q181" s="13"/>
+      <c r="R181" s="5"/>
+    </row>
+    <row r="182" spans="2:18">
+      <c r="B182" s="4"/>
+      <c r="C182" s="13"/>
+      <c r="D182" s="13"/>
+      <c r="E182" s="13"/>
+      <c r="F182" s="13"/>
+      <c r="G182" s="13"/>
+      <c r="H182" s="13"/>
+      <c r="I182" s="13"/>
+      <c r="J182" s="13"/>
+      <c r="K182" s="13"/>
+      <c r="L182" s="13"/>
+      <c r="M182" s="13"/>
+      <c r="N182" s="13"/>
+      <c r="O182" s="13"/>
+      <c r="P182" s="13"/>
+      <c r="Q182" s="13"/>
+      <c r="R182" s="5"/>
+    </row>
+    <row r="183" spans="2:18">
+      <c r="B183" s="4"/>
+      <c r="C183" s="13"/>
+      <c r="D183" s="13"/>
+      <c r="E183" s="13"/>
+      <c r="F183" s="13"/>
+      <c r="G183" s="13"/>
+      <c r="H183" s="13"/>
+      <c r="I183" s="13"/>
+      <c r="J183" s="13"/>
+      <c r="K183" s="13"/>
+      <c r="L183" s="13"/>
+      <c r="M183" s="13"/>
+      <c r="N183" s="13"/>
+      <c r="O183" s="13"/>
+      <c r="P183" s="13"/>
+      <c r="Q183" s="13"/>
+      <c r="R183" s="5"/>
+    </row>
+    <row r="184" spans="2:18">
+      <c r="B184" s="4"/>
+      <c r="C184" s="13"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="13"/>
+      <c r="F184" s="13"/>
+      <c r="G184" s="13"/>
+      <c r="H184" s="13"/>
+      <c r="I184" s="13"/>
+      <c r="J184" s="13"/>
+      <c r="K184" s="13"/>
+      <c r="L184" s="13"/>
+      <c r="M184" s="13"/>
+      <c r="N184" s="13"/>
+      <c r="O184" s="13"/>
+      <c r="P184" s="13"/>
+      <c r="Q184" s="13"/>
+      <c r="R184" s="5"/>
+    </row>
+    <row r="185" spans="2:18">
+      <c r="B185" s="7"/>
+      <c r="C185" s="8"/>
+      <c r="D185" s="8"/>
+      <c r="E185" s="8"/>
+      <c r="F185" s="8"/>
+      <c r="G185" s="8"/>
+      <c r="H185" s="8"/>
+      <c r="I185" s="8"/>
+      <c r="J185" s="8"/>
+      <c r="K185" s="8"/>
+      <c r="L185" s="8"/>
+      <c r="M185" s="8"/>
+      <c r="N185" s="8"/>
+      <c r="O185" s="8"/>
+      <c r="P185" s="8"/>
+      <c r="Q185" s="8"/>
+      <c r="R185" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Get the data from the request for updating an existing record
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/3.create-update-and-delete-individual-resources.xlsx
+++ b/me/4.create-a-restful-api/3.create-update-and-delete-individual-resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD907677-2315-4268-AC68-993F3A3685B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2957A2E6-9E1B-4940-9992-EA9A57D5390F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="get request JSON data" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="add generic error handler" sheetId="3" r:id="rId3"/>
     <sheet name="Validate data respond 422status" sheetId="4" r:id="rId4"/>
     <sheet name="validate update existing record" sheetId="5" r:id="rId5"/>
+    <sheet name="get data from request update" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="283">
   <si>
     <t>構成</t>
   </si>
@@ -961,6 +962,99 @@
   </si>
   <si>
     <t>call api để update data, data truyền lên ko cần chứa trường name, response trả về là OK(200)</t>
+  </si>
+  <si>
+    <t>Get the data from the request for updating an existing record</t>
+  </si>
+  <si>
+    <t>                    $this-&gt;gateway-&gt;update($id, $data);</t>
+  </si>
+  <si>
+    <t>    private function getValidationErrors(array $data, bool $is_new = true): array</t>
+  </si>
+  <si>
+    <t>        if ($is_new &amp;&amp; empty($data["name"])) {</t>
+  </si>
+  <si>
+    <t>    public function update(string $id, array $data)</t>
+  </si>
+  <si>
+    <t>        $fields = [];</t>
+  </si>
+  <si>
+    <t>        if (!empty($data["name"])) {</t>
+  </si>
+  <si>
+    <t>            $fields["name"] = [</t>
+  </si>
+  <si>
+    <t>                $data["name"],</t>
+  </si>
+  <si>
+    <t>                PDO::PARAM_STR</t>
+  </si>
+  <si>
+    <t>            ];</t>
+  </si>
+  <si>
+    <t>        if (array_key_exists("priority", $data)) {</t>
+  </si>
+  <si>
+    <t>            $fields["priority"] = [</t>
+  </si>
+  <si>
+    <t>                $data["priority"],</t>
+  </si>
+  <si>
+    <t>                $data["priority"] === null ? PDO::PARAM_NULL : PDO::PARAM_INT</t>
+  </si>
+  <si>
+    <t>        if (array_key_exists("is_completed", $data)) {</t>
+  </si>
+  <si>
+    <t>            $fields["is_completed"] = [</t>
+  </si>
+  <si>
+    <t>                $data["is_completed"],</t>
+  </si>
+  <si>
+    <t>                PDO::PARAM_BOOL</t>
+  </si>
+  <si>
+    <t>        echo json_encode($fields);</t>
+  </si>
+  <si>
+    <t>        exit;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Không giống như insert, đối với update thì mình chỉ cần dựa vào data request xác định những trường nào </t>
+  </si>
+  <si>
+    <t>cần update dựa để tạo câu sql update dựa trên các trường đó</t>
+  </si>
+  <si>
+    <t>Mình sẽ dùng phương thức bindValue() bind các giá trị được request đến để placeholder câu SQL do đó</t>
+  </si>
+  <si>
+    <t>ở đây mình sẽ đưa thêm PDO data type</t>
+  </si>
+  <si>
+    <t>Trong trường hợp giá trị is_completed được truyền đến được set giá trị là false thì nếu dùng empty() như đối</t>
+  </si>
+  <si>
+    <t>với name thì !empty($data["is_completed"]) nhận giá trị false nên giá trị is_completed truyền đến</t>
+  </si>
+  <si>
+    <t>sẽ ko được set vào $fields. Do đó thay cho việc dùng empty() thì mình phải dùng array_key_exists() để check</t>
+  </si>
+  <si>
+    <t>Tương tự đối với priority cũng vậy, đối với priority thì nó có thể được truyền đến giá trị null và empty(null) có</t>
+  </si>
+  <si>
+    <t>Giá trị của priority thì có thể là null hoặc int</t>
+  </si>
+  <si>
+    <t>giá trị true nên priority cũng phải dùng array_key_exists() để check</t>
   </si>
 </sst>
 </file>
@@ -5015,6 +5109,585 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>239</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EBB320C-6D28-CDC9-2133-88333C072912}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1752600" y="18449925"/>
+          <a:ext cx="647700" cy="27146250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{838AD943-2737-B293-47D9-8915B0401515}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1600200" y="45853350"/>
+          <a:ext cx="4495800" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>247</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C03A600-43E8-FDA3-510A-1A40EDFC636C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2019300" y="46958250"/>
+          <a:ext cx="8096250" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>243</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FABD41C1-4F32-A4D3-1F3B-E624831EF7EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1476375" y="46453425"/>
+          <a:ext cx="10086975" cy="2962275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Straight Arrow Connector 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F56A2BE-182E-D76A-8E34-CDF88F5BDBCE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2000250" y="49520475"/>
+          <a:ext cx="8677275" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>251</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81FA1141-306B-B5C8-8BF8-9BBA720A3044}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2076450" y="47986950"/>
+          <a:ext cx="5114925" cy="1981200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>274</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>332124</xdr:colOff>
+      <xdr:row>302</xdr:row>
+      <xdr:rowOff>123151</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{160855DE-4CCA-1D6A-C29D-30B6E4673453}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="52263675"/>
+          <a:ext cx="10009524" cy="5390476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Arrow Connector 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7B002ED-CF29-7154-7EE4-467C25C9C07D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2790825" y="49501425"/>
+          <a:ext cx="7829550" cy="4238625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>282</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>299</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Straight Arrow Connector 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{725EA8C8-5E46-0655-E3DB-9F8411F93A9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1971675" y="53844825"/>
+          <a:ext cx="581025" cy="3286125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>262</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>281</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Straight Arrow Connector 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D6AACA4-0158-5393-41A9-C5D9DCE6251E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2466975" y="50091975"/>
+          <a:ext cx="8867775" cy="3505200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>281</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>297</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Arrow Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63AF65A4-39A0-1B29-1B8F-56777971F8AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1838325" y="53692425"/>
+          <a:ext cx="438150" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -26220,8 +26893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D565EF0-601C-40DC-B5D3-AD4BBA1DD3AA}">
   <dimension ref="A2:R185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28461,4 +29134,3665 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805CB3D0-F6EF-4C81-9127-64B24E106742}">
+  <dimension ref="A2:R304"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="C310" sqref="C310"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="B2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="4"/>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" s="4"/>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="4"/>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="B17" s="4"/>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="B18" s="4"/>
+      <c r="F18" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="B19" s="4"/>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="B20" s="4"/>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="B21" s="4"/>
+      <c r="F21" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="B22" s="4"/>
+      <c r="F22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="B23" s="4"/>
+      <c r="F23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="B24" s="4"/>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="B25" s="4"/>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="B26" s="4"/>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="B27" s="4"/>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="B28" s="4"/>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
+      <c r="B33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="2:10">
+      <c r="B34" s="4"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="2:10">
+      <c r="B35" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="2:10">
+      <c r="B36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="2:10">
+      <c r="B37" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="2:10">
+      <c r="B38" s="4"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="2:10">
+      <c r="B39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="2:10">
+      <c r="B40" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="2:10">
+      <c r="B41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="2:10">
+      <c r="B42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="2:10">
+      <c r="B43" s="4"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="2:10">
+      <c r="B44" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="2:10">
+      <c r="B45" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="2:10">
+      <c r="B46" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="2:10">
+      <c r="B47" s="4"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="2:10">
+      <c r="B48" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="2:10">
+      <c r="B49" s="4"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="2:10">
+      <c r="B50" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="2:10">
+      <c r="B51" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="2:10">
+      <c r="B52" s="4"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="2:10">
+      <c r="B53" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="2:10">
+      <c r="B54" s="4"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="2:10">
+      <c r="B55" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="2:10">
+      <c r="B56" s="4"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="2:10">
+      <c r="B57" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="2:10">
+      <c r="B58" s="4"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="2:10">
+      <c r="B59" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="2:10">
+      <c r="B60" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="2:10">
+      <c r="B61" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="2:10">
+      <c r="B62" s="4"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="2:10">
+      <c r="B63" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="2:10">
+      <c r="B64" s="4"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="2:10">
+      <c r="B65" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="2:10">
+      <c r="B66" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="2:10">
+      <c r="B67" s="4"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="2:10">
+      <c r="B68" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="2:10">
+      <c r="B69" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="2:10">
+      <c r="B70" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="2:10">
+      <c r="B71" s="4"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="2:10">
+      <c r="B72" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="2:10">
+      <c r="B73" s="4"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" spans="2:10">
+      <c r="B74" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="2:10">
+      <c r="B75" s="4"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" spans="2:10">
+      <c r="B76" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="5"/>
+    </row>
+    <row r="77" spans="2:10">
+      <c r="B77" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="5"/>
+    </row>
+    <row r="78" spans="2:10">
+      <c r="B78" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="5"/>
+    </row>
+    <row r="79" spans="2:10">
+      <c r="B79" s="4"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" spans="2:10">
+      <c r="B80" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="5"/>
+    </row>
+    <row r="81" spans="2:10">
+      <c r="B81" s="4"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="5"/>
+    </row>
+    <row r="82" spans="2:10">
+      <c r="B82" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="5"/>
+    </row>
+    <row r="83" spans="2:10">
+      <c r="B83" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="5"/>
+    </row>
+    <row r="84" spans="2:10">
+      <c r="B84" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="5"/>
+    </row>
+    <row r="85" spans="2:10">
+      <c r="B85" s="4"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="5"/>
+    </row>
+    <row r="86" spans="2:10">
+      <c r="B86" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="5"/>
+    </row>
+    <row r="87" spans="2:10">
+      <c r="B87" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="5"/>
+    </row>
+    <row r="88" spans="2:10">
+      <c r="B88" s="4"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="5"/>
+    </row>
+    <row r="89" spans="2:10">
+      <c r="B89" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="5"/>
+    </row>
+    <row r="90" spans="2:10">
+      <c r="B90" s="4"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="5"/>
+    </row>
+    <row r="91" spans="2:10">
+      <c r="B91" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="13"/>
+      <c r="J91" s="5"/>
+    </row>
+    <row r="92" spans="2:10">
+      <c r="B92" s="4"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="13"/>
+      <c r="J92" s="5"/>
+    </row>
+    <row r="93" spans="2:10">
+      <c r="B93" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="13"/>
+      <c r="J93" s="5"/>
+    </row>
+    <row r="94" spans="2:10">
+      <c r="B94" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
+      <c r="J94" s="5"/>
+    </row>
+    <row r="95" spans="2:10">
+      <c r="B95" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="13"/>
+      <c r="J95" s="5"/>
+    </row>
+    <row r="96" spans="2:10">
+      <c r="B96" s="4"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
+      <c r="J96" s="5"/>
+    </row>
+    <row r="97" spans="2:10">
+      <c r="B97" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="13"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="13"/>
+      <c r="J97" s="5"/>
+    </row>
+    <row r="98" spans="2:10">
+      <c r="B98" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="13"/>
+      <c r="J98" s="5"/>
+    </row>
+    <row r="99" spans="2:10">
+      <c r="B99" s="4"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="13"/>
+      <c r="J99" s="5"/>
+    </row>
+    <row r="100" spans="2:10">
+      <c r="B100" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="13"/>
+      <c r="J100" s="5"/>
+    </row>
+    <row r="101" spans="2:10">
+      <c r="B101" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="13"/>
+      <c r="J101" s="5"/>
+    </row>
+    <row r="102" spans="2:10">
+      <c r="B102" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="13"/>
+      <c r="J102" s="5"/>
+    </row>
+    <row r="103" spans="2:10">
+      <c r="B103" s="4"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="13"/>
+      <c r="G103" s="13"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="13"/>
+      <c r="J103" s="5"/>
+    </row>
+    <row r="104" spans="2:10">
+      <c r="B104" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C104" s="13"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="13"/>
+      <c r="G104" s="13"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="13"/>
+      <c r="J104" s="5"/>
+    </row>
+    <row r="105" spans="2:10">
+      <c r="B105" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C105" s="13"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="13"/>
+      <c r="I105" s="13"/>
+      <c r="J105" s="5"/>
+    </row>
+    <row r="106" spans="2:10">
+      <c r="B106" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C106" s="13"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
+      <c r="F106" s="13"/>
+      <c r="G106" s="13"/>
+      <c r="H106" s="13"/>
+      <c r="I106" s="13"/>
+      <c r="J106" s="5"/>
+    </row>
+    <row r="107" spans="2:10">
+      <c r="B107" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="13"/>
+      <c r="J107" s="5"/>
+    </row>
+    <row r="108" spans="2:10">
+      <c r="B108" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="13"/>
+      <c r="J108" s="5"/>
+    </row>
+    <row r="109" spans="2:10">
+      <c r="B109" s="4"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="13"/>
+      <c r="G109" s="13"/>
+      <c r="H109" s="13"/>
+      <c r="I109" s="13"/>
+      <c r="J109" s="5"/>
+    </row>
+    <row r="110" spans="2:10">
+      <c r="B110" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="13"/>
+      <c r="H110" s="13"/>
+      <c r="I110" s="13"/>
+      <c r="J110" s="5"/>
+    </row>
+    <row r="111" spans="2:10">
+      <c r="B111" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="13"/>
+      <c r="J111" s="5"/>
+    </row>
+    <row r="112" spans="2:10">
+      <c r="B112" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="13"/>
+      <c r="J112" s="5"/>
+    </row>
+    <row r="113" spans="2:10">
+      <c r="B113" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C113" s="13"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
+      <c r="G113" s="13"/>
+      <c r="H113" s="13"/>
+      <c r="I113" s="13"/>
+      <c r="J113" s="5"/>
+    </row>
+    <row r="114" spans="2:10">
+      <c r="B114" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C114" s="13"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="13"/>
+      <c r="G114" s="13"/>
+      <c r="H114" s="13"/>
+      <c r="I114" s="13"/>
+      <c r="J114" s="5"/>
+    </row>
+    <row r="115" spans="2:10">
+      <c r="B115" s="4"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13"/>
+      <c r="G115" s="13"/>
+      <c r="H115" s="13"/>
+      <c r="I115" s="13"/>
+      <c r="J115" s="5"/>
+    </row>
+    <row r="116" spans="2:10">
+      <c r="B116" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C116" s="13"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
+      <c r="F116" s="13"/>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="13"/>
+      <c r="J116" s="5"/>
+    </row>
+    <row r="117" spans="2:10">
+      <c r="B117" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C117" s="13"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="13"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="13"/>
+      <c r="J117" s="5"/>
+    </row>
+    <row r="118" spans="2:10">
+      <c r="B118" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C118" s="13"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="13"/>
+      <c r="G118" s="13"/>
+      <c r="H118" s="13"/>
+      <c r="I118" s="13"/>
+      <c r="J118" s="5"/>
+    </row>
+    <row r="119" spans="2:10">
+      <c r="B119" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13"/>
+      <c r="G119" s="13"/>
+      <c r="H119" s="13"/>
+      <c r="I119" s="13"/>
+      <c r="J119" s="5"/>
+    </row>
+    <row r="120" spans="2:10">
+      <c r="B120" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="13"/>
+      <c r="J120" s="5"/>
+    </row>
+    <row r="121" spans="2:10">
+      <c r="B121" s="4"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
+      <c r="F121" s="13"/>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="13"/>
+      <c r="J121" s="5"/>
+    </row>
+    <row r="122" spans="2:10">
+      <c r="B122" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
+      <c r="G122" s="13"/>
+      <c r="H122" s="13"/>
+      <c r="I122" s="13"/>
+      <c r="J122" s="5"/>
+    </row>
+    <row r="123" spans="2:10">
+      <c r="B123" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C123" s="13"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="13"/>
+      <c r="G123" s="13"/>
+      <c r="H123" s="13"/>
+      <c r="I123" s="13"/>
+      <c r="J123" s="5"/>
+    </row>
+    <row r="124" spans="2:10">
+      <c r="B124" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C124" s="13"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
+      <c r="F124" s="13"/>
+      <c r="G124" s="13"/>
+      <c r="H124" s="13"/>
+      <c r="I124" s="13"/>
+      <c r="J124" s="5"/>
+    </row>
+    <row r="125" spans="2:10">
+      <c r="B125" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
+      <c r="F125" s="13"/>
+      <c r="G125" s="13"/>
+      <c r="H125" s="13"/>
+      <c r="I125" s="13"/>
+      <c r="J125" s="5"/>
+    </row>
+    <row r="126" spans="2:10">
+      <c r="B126" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="13"/>
+      <c r="G126" s="13"/>
+      <c r="H126" s="13"/>
+      <c r="I126" s="13"/>
+      <c r="J126" s="5"/>
+    </row>
+    <row r="127" spans="2:10">
+      <c r="B127" s="4"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="13"/>
+      <c r="F127" s="13"/>
+      <c r="G127" s="13"/>
+      <c r="H127" s="13"/>
+      <c r="I127" s="13"/>
+      <c r="J127" s="5"/>
+    </row>
+    <row r="128" spans="2:10">
+      <c r="B128" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="13"/>
+      <c r="F128" s="13"/>
+      <c r="G128" s="13"/>
+      <c r="H128" s="13"/>
+      <c r="I128" s="13"/>
+      <c r="J128" s="5"/>
+    </row>
+    <row r="129" spans="2:10">
+      <c r="B129" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C129" s="13"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="13"/>
+      <c r="G129" s="13"/>
+      <c r="H129" s="13"/>
+      <c r="I129" s="13"/>
+      <c r="J129" s="5"/>
+    </row>
+    <row r="130" spans="2:10">
+      <c r="B130" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="13"/>
+      <c r="F130" s="13"/>
+      <c r="G130" s="13"/>
+      <c r="H130" s="13"/>
+      <c r="I130" s="13"/>
+      <c r="J130" s="5"/>
+    </row>
+    <row r="131" spans="2:10">
+      <c r="B131" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="13"/>
+      <c r="G131" s="13"/>
+      <c r="H131" s="13"/>
+      <c r="I131" s="13"/>
+      <c r="J131" s="5"/>
+    </row>
+    <row r="132" spans="2:10">
+      <c r="B132" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="13"/>
+      <c r="F132" s="13"/>
+      <c r="G132" s="13"/>
+      <c r="H132" s="13"/>
+      <c r="I132" s="13"/>
+      <c r="J132" s="5"/>
+    </row>
+    <row r="133" spans="2:10">
+      <c r="B133" s="4"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="13"/>
+      <c r="G133" s="13"/>
+      <c r="H133" s="13"/>
+      <c r="I133" s="13"/>
+      <c r="J133" s="5"/>
+    </row>
+    <row r="134" spans="2:10">
+      <c r="B134" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13"/>
+      <c r="F134" s="13"/>
+      <c r="G134" s="13"/>
+      <c r="H134" s="13"/>
+      <c r="I134" s="13"/>
+      <c r="J134" s="5"/>
+    </row>
+    <row r="135" spans="2:10">
+      <c r="B135" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C135" s="13"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="13"/>
+      <c r="F135" s="13"/>
+      <c r="G135" s="13"/>
+      <c r="H135" s="13"/>
+      <c r="I135" s="13"/>
+      <c r="J135" s="5"/>
+    </row>
+    <row r="136" spans="2:10">
+      <c r="B136" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C136" s="13"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="13"/>
+      <c r="G136" s="13"/>
+      <c r="H136" s="13"/>
+      <c r="I136" s="13"/>
+      <c r="J136" s="5"/>
+    </row>
+    <row r="137" spans="2:10">
+      <c r="B137" s="4"/>
+      <c r="C137" s="13"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
+      <c r="H137" s="13"/>
+      <c r="I137" s="13"/>
+      <c r="J137" s="5"/>
+    </row>
+    <row r="138" spans="2:10">
+      <c r="B138" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C138" s="13"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="13"/>
+      <c r="G138" s="13"/>
+      <c r="H138" s="13"/>
+      <c r="I138" s="13"/>
+      <c r="J138" s="5"/>
+    </row>
+    <row r="139" spans="2:10">
+      <c r="B139" s="4"/>
+      <c r="C139" s="13"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="13"/>
+      <c r="F139" s="13"/>
+      <c r="G139" s="13"/>
+      <c r="H139" s="13"/>
+      <c r="I139" s="13"/>
+      <c r="J139" s="5"/>
+    </row>
+    <row r="140" spans="2:10">
+      <c r="B140" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C140" s="13"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
+      <c r="H140" s="13"/>
+      <c r="I140" s="13"/>
+      <c r="J140" s="5"/>
+    </row>
+    <row r="141" spans="2:10">
+      <c r="B141" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C141" s="13"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="13"/>
+      <c r="F141" s="13"/>
+      <c r="G141" s="13"/>
+      <c r="H141" s="13"/>
+      <c r="I141" s="13"/>
+      <c r="J141" s="5"/>
+    </row>
+    <row r="142" spans="2:10">
+      <c r="B142" s="4"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
+      <c r="F142" s="13"/>
+      <c r="G142" s="13"/>
+      <c r="H142" s="13"/>
+      <c r="I142" s="13"/>
+      <c r="J142" s="5"/>
+    </row>
+    <row r="143" spans="2:10">
+      <c r="B143" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
+      <c r="F143" s="13"/>
+      <c r="G143" s="13"/>
+      <c r="H143" s="13"/>
+      <c r="I143" s="13"/>
+      <c r="J143" s="5"/>
+    </row>
+    <row r="144" spans="2:10">
+      <c r="B144" s="4"/>
+      <c r="C144" s="13"/>
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
+      <c r="F144" s="13"/>
+      <c r="G144" s="13"/>
+      <c r="H144" s="13"/>
+      <c r="I144" s="13"/>
+      <c r="J144" s="5"/>
+    </row>
+    <row r="145" spans="1:10">
+      <c r="B145" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C145" s="13"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
+      <c r="F145" s="13"/>
+      <c r="G145" s="13"/>
+      <c r="H145" s="13"/>
+      <c r="I145" s="13"/>
+      <c r="J145" s="5"/>
+    </row>
+    <row r="146" spans="1:10">
+      <c r="B146" s="4"/>
+      <c r="C146" s="13"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
+      <c r="F146" s="13"/>
+      <c r="G146" s="13"/>
+      <c r="H146" s="13"/>
+      <c r="I146" s="13"/>
+      <c r="J146" s="5"/>
+    </row>
+    <row r="147" spans="1:10">
+      <c r="B147" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C147" s="13"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="13"/>
+      <c r="G147" s="13"/>
+      <c r="H147" s="13"/>
+      <c r="I147" s="13"/>
+      <c r="J147" s="5"/>
+    </row>
+    <row r="148" spans="1:10">
+      <c r="B148" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C148" s="13"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
+      <c r="F148" s="13"/>
+      <c r="G148" s="13"/>
+      <c r="H148" s="13"/>
+      <c r="I148" s="13"/>
+      <c r="J148" s="5"/>
+    </row>
+    <row r="149" spans="1:10">
+      <c r="B149" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C149" s="13"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
+      <c r="F149" s="13"/>
+      <c r="G149" s="13"/>
+      <c r="H149" s="13"/>
+      <c r="I149" s="13"/>
+      <c r="J149" s="5"/>
+    </row>
+    <row r="150" spans="1:10">
+      <c r="B150" s="4"/>
+      <c r="C150" s="13"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
+      <c r="F150" s="13"/>
+      <c r="G150" s="13"/>
+      <c r="H150" s="13"/>
+      <c r="I150" s="13"/>
+      <c r="J150" s="5"/>
+    </row>
+    <row r="151" spans="1:10">
+      <c r="B151" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C151" s="13"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="13"/>
+      <c r="F151" s="13"/>
+      <c r="G151" s="13"/>
+      <c r="H151" s="13"/>
+      <c r="I151" s="13"/>
+      <c r="J151" s="5"/>
+    </row>
+    <row r="152" spans="1:10">
+      <c r="B152" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C152" s="13"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="13"/>
+      <c r="F152" s="13"/>
+      <c r="G152" s="13"/>
+      <c r="H152" s="13"/>
+      <c r="I152" s="13"/>
+      <c r="J152" s="5"/>
+    </row>
+    <row r="153" spans="1:10">
+      <c r="B153" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C153" s="8"/>
+      <c r="D153" s="8"/>
+      <c r="E153" s="8"/>
+      <c r="F153" s="8"/>
+      <c r="G153" s="8"/>
+      <c r="H153" s="8"/>
+      <c r="I153" s="8"/>
+      <c r="J153" s="9"/>
+    </row>
+    <row r="156" spans="1:10">
+      <c r="A156" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10">
+      <c r="B157" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C157" s="2"/>
+      <c r="D157" s="2"/>
+      <c r="E157" s="2"/>
+      <c r="F157" s="2"/>
+      <c r="G157" s="2"/>
+      <c r="H157" s="2"/>
+      <c r="I157" s="3"/>
+    </row>
+    <row r="158" spans="1:10">
+      <c r="B158" s="4"/>
+      <c r="C158" s="13"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="13"/>
+      <c r="F158" s="13"/>
+      <c r="G158" s="13"/>
+      <c r="H158" s="13"/>
+      <c r="I158" s="5"/>
+    </row>
+    <row r="159" spans="1:10">
+      <c r="B159" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C159" s="13"/>
+      <c r="D159" s="13"/>
+      <c r="E159" s="13"/>
+      <c r="F159" s="13"/>
+      <c r="G159" s="13"/>
+      <c r="H159" s="13"/>
+      <c r="I159" s="5"/>
+    </row>
+    <row r="160" spans="1:10">
+      <c r="B160" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C160" s="13"/>
+      <c r="D160" s="13"/>
+      <c r="E160" s="13"/>
+      <c r="F160" s="13"/>
+      <c r="G160" s="13"/>
+      <c r="H160" s="13"/>
+      <c r="I160" s="5"/>
+    </row>
+    <row r="161" spans="2:9">
+      <c r="B161" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C161" s="13"/>
+      <c r="D161" s="13"/>
+      <c r="E161" s="13"/>
+      <c r="F161" s="13"/>
+      <c r="G161" s="13"/>
+      <c r="H161" s="13"/>
+      <c r="I161" s="5"/>
+    </row>
+    <row r="162" spans="2:9">
+      <c r="B162" s="4"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="13"/>
+      <c r="F162" s="13"/>
+      <c r="G162" s="13"/>
+      <c r="H162" s="13"/>
+      <c r="I162" s="5"/>
+    </row>
+    <row r="163" spans="2:9">
+      <c r="B163" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C163" s="13"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="13"/>
+      <c r="F163" s="13"/>
+      <c r="G163" s="13"/>
+      <c r="H163" s="13"/>
+      <c r="I163" s="5"/>
+    </row>
+    <row r="164" spans="2:9">
+      <c r="B164" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C164" s="13"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="13"/>
+      <c r="F164" s="13"/>
+      <c r="G164" s="13"/>
+      <c r="H164" s="13"/>
+      <c r="I164" s="5"/>
+    </row>
+    <row r="165" spans="2:9">
+      <c r="B165" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C165" s="13"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="13"/>
+      <c r="F165" s="13"/>
+      <c r="G165" s="13"/>
+      <c r="H165" s="13"/>
+      <c r="I165" s="5"/>
+    </row>
+    <row r="166" spans="2:9">
+      <c r="B166" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C166" s="13"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="13"/>
+      <c r="F166" s="13"/>
+      <c r="G166" s="13"/>
+      <c r="H166" s="13"/>
+      <c r="I166" s="5"/>
+    </row>
+    <row r="167" spans="2:9">
+      <c r="B167" s="4"/>
+      <c r="C167" s="13"/>
+      <c r="D167" s="13"/>
+      <c r="E167" s="13"/>
+      <c r="F167" s="13"/>
+      <c r="G167" s="13"/>
+      <c r="H167" s="13"/>
+      <c r="I167" s="5"/>
+    </row>
+    <row r="168" spans="2:9">
+      <c r="B168" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C168" s="13"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="13"/>
+      <c r="F168" s="13"/>
+      <c r="G168" s="13"/>
+      <c r="H168" s="13"/>
+      <c r="I168" s="5"/>
+    </row>
+    <row r="169" spans="2:9">
+      <c r="B169" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C169" s="13"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="13"/>
+      <c r="F169" s="13"/>
+      <c r="G169" s="13"/>
+      <c r="H169" s="13"/>
+      <c r="I169" s="5"/>
+    </row>
+    <row r="170" spans="2:9">
+      <c r="B170" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C170" s="13"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="13"/>
+      <c r="F170" s="13"/>
+      <c r="G170" s="13"/>
+      <c r="H170" s="13"/>
+      <c r="I170" s="5"/>
+    </row>
+    <row r="171" spans="2:9">
+      <c r="B171" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C171" s="13"/>
+      <c r="D171" s="13"/>
+      <c r="E171" s="13"/>
+      <c r="F171" s="13"/>
+      <c r="G171" s="13"/>
+      <c r="H171" s="13"/>
+      <c r="I171" s="5"/>
+    </row>
+    <row r="172" spans="2:9">
+      <c r="B172" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C172" s="13"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="13"/>
+      <c r="F172" s="13"/>
+      <c r="G172" s="13"/>
+      <c r="H172" s="13"/>
+      <c r="I172" s="5"/>
+    </row>
+    <row r="173" spans="2:9">
+      <c r="B173" s="4"/>
+      <c r="C173" s="13"/>
+      <c r="D173" s="13"/>
+      <c r="E173" s="13"/>
+      <c r="F173" s="13"/>
+      <c r="G173" s="13"/>
+      <c r="H173" s="13"/>
+      <c r="I173" s="5"/>
+    </row>
+    <row r="174" spans="2:9">
+      <c r="B174" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C174" s="13"/>
+      <c r="D174" s="13"/>
+      <c r="E174" s="13"/>
+      <c r="F174" s="13"/>
+      <c r="G174" s="13"/>
+      <c r="H174" s="13"/>
+      <c r="I174" s="5"/>
+    </row>
+    <row r="175" spans="2:9">
+      <c r="B175" s="4"/>
+      <c r="C175" s="13"/>
+      <c r="D175" s="13"/>
+      <c r="E175" s="13"/>
+      <c r="F175" s="13"/>
+      <c r="G175" s="13"/>
+      <c r="H175" s="13"/>
+      <c r="I175" s="5"/>
+    </row>
+    <row r="176" spans="2:9">
+      <c r="B176" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C176" s="13"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="13"/>
+      <c r="F176" s="13"/>
+      <c r="G176" s="13"/>
+      <c r="H176" s="13"/>
+      <c r="I176" s="5"/>
+    </row>
+    <row r="177" spans="2:9">
+      <c r="B177" s="4"/>
+      <c r="C177" s="13"/>
+      <c r="D177" s="13"/>
+      <c r="E177" s="13"/>
+      <c r="F177" s="13"/>
+      <c r="G177" s="13"/>
+      <c r="H177" s="13"/>
+      <c r="I177" s="5"/>
+    </row>
+    <row r="178" spans="2:9">
+      <c r="B178" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C178" s="13"/>
+      <c r="D178" s="13"/>
+      <c r="E178" s="13"/>
+      <c r="F178" s="13"/>
+      <c r="G178" s="13"/>
+      <c r="H178" s="13"/>
+      <c r="I178" s="5"/>
+    </row>
+    <row r="179" spans="2:9">
+      <c r="B179" s="4"/>
+      <c r="C179" s="13"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13"/>
+      <c r="F179" s="13"/>
+      <c r="G179" s="13"/>
+      <c r="H179" s="13"/>
+      <c r="I179" s="5"/>
+    </row>
+    <row r="180" spans="2:9">
+      <c r="B180" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C180" s="13"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13"/>
+      <c r="F180" s="13"/>
+      <c r="G180" s="13"/>
+      <c r="H180" s="13"/>
+      <c r="I180" s="5"/>
+    </row>
+    <row r="181" spans="2:9">
+      <c r="B181" s="4"/>
+      <c r="C181" s="13"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="13"/>
+      <c r="F181" s="13"/>
+      <c r="G181" s="13"/>
+      <c r="H181" s="13"/>
+      <c r="I181" s="5"/>
+    </row>
+    <row r="182" spans="2:9">
+      <c r="B182" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C182" s="13"/>
+      <c r="D182" s="13"/>
+      <c r="E182" s="13"/>
+      <c r="F182" s="13"/>
+      <c r="G182" s="13"/>
+      <c r="H182" s="13"/>
+      <c r="I182" s="5"/>
+    </row>
+    <row r="183" spans="2:9">
+      <c r="B183" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C183" s="13"/>
+      <c r="D183" s="13"/>
+      <c r="E183" s="13"/>
+      <c r="F183" s="13"/>
+      <c r="G183" s="13"/>
+      <c r="H183" s="13"/>
+      <c r="I183" s="5"/>
+    </row>
+    <row r="184" spans="2:9">
+      <c r="B184" s="4"/>
+      <c r="C184" s="13"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="13"/>
+      <c r="F184" s="13"/>
+      <c r="G184" s="13"/>
+      <c r="H184" s="13"/>
+      <c r="I184" s="5"/>
+    </row>
+    <row r="185" spans="2:9">
+      <c r="B185" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C185" s="13"/>
+      <c r="D185" s="13"/>
+      <c r="E185" s="13"/>
+      <c r="F185" s="13"/>
+      <c r="G185" s="13"/>
+      <c r="H185" s="13"/>
+      <c r="I185" s="5"/>
+    </row>
+    <row r="186" spans="2:9">
+      <c r="B186" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C186" s="13"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="13"/>
+      <c r="F186" s="13"/>
+      <c r="G186" s="13"/>
+      <c r="H186" s="13"/>
+      <c r="I186" s="5"/>
+    </row>
+    <row r="187" spans="2:9">
+      <c r="B187" s="4"/>
+      <c r="C187" s="13"/>
+      <c r="D187" s="13"/>
+      <c r="E187" s="13"/>
+      <c r="F187" s="13"/>
+      <c r="G187" s="13"/>
+      <c r="H187" s="13"/>
+      <c r="I187" s="5"/>
+    </row>
+    <row r="188" spans="2:9">
+      <c r="B188" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C188" s="13"/>
+      <c r="D188" s="13"/>
+      <c r="E188" s="13"/>
+      <c r="F188" s="13"/>
+      <c r="G188" s="13"/>
+      <c r="H188" s="13"/>
+      <c r="I188" s="5"/>
+    </row>
+    <row r="189" spans="2:9">
+      <c r="B189" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C189" s="13"/>
+      <c r="D189" s="13"/>
+      <c r="E189" s="13"/>
+      <c r="F189" s="13"/>
+      <c r="G189" s="13"/>
+      <c r="H189" s="13"/>
+      <c r="I189" s="5"/>
+    </row>
+    <row r="190" spans="2:9">
+      <c r="B190" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C190" s="13"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="13"/>
+      <c r="F190" s="13"/>
+      <c r="G190" s="13"/>
+      <c r="H190" s="13"/>
+      <c r="I190" s="5"/>
+    </row>
+    <row r="191" spans="2:9">
+      <c r="B191" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C191" s="13"/>
+      <c r="D191" s="13"/>
+      <c r="E191" s="13"/>
+      <c r="F191" s="13"/>
+      <c r="G191" s="13"/>
+      <c r="H191" s="13"/>
+      <c r="I191" s="5"/>
+    </row>
+    <row r="192" spans="2:9">
+      <c r="B192" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C192" s="13"/>
+      <c r="D192" s="13"/>
+      <c r="E192" s="13"/>
+      <c r="F192" s="13"/>
+      <c r="G192" s="13"/>
+      <c r="H192" s="13"/>
+      <c r="I192" s="5"/>
+    </row>
+    <row r="193" spans="2:9">
+      <c r="B193" s="4"/>
+      <c r="C193" s="13"/>
+      <c r="D193" s="13"/>
+      <c r="E193" s="13"/>
+      <c r="F193" s="13"/>
+      <c r="G193" s="13"/>
+      <c r="H193" s="13"/>
+      <c r="I193" s="5"/>
+    </row>
+    <row r="194" spans="2:9">
+      <c r="B194" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C194" s="13"/>
+      <c r="D194" s="13"/>
+      <c r="E194" s="13"/>
+      <c r="F194" s="13"/>
+      <c r="G194" s="13"/>
+      <c r="H194" s="13"/>
+      <c r="I194" s="5"/>
+    </row>
+    <row r="195" spans="2:9">
+      <c r="B195" s="4"/>
+      <c r="C195" s="13"/>
+      <c r="D195" s="13"/>
+      <c r="E195" s="13"/>
+      <c r="F195" s="13"/>
+      <c r="G195" s="13"/>
+      <c r="H195" s="13"/>
+      <c r="I195" s="5"/>
+    </row>
+    <row r="196" spans="2:9">
+      <c r="B196" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C196" s="13"/>
+      <c r="D196" s="13"/>
+      <c r="E196" s="13"/>
+      <c r="F196" s="13"/>
+      <c r="G196" s="13"/>
+      <c r="H196" s="13"/>
+      <c r="I196" s="5"/>
+    </row>
+    <row r="197" spans="2:9">
+      <c r="B197" s="4"/>
+      <c r="C197" s="13"/>
+      <c r="D197" s="13"/>
+      <c r="E197" s="13"/>
+      <c r="F197" s="13"/>
+      <c r="G197" s="13"/>
+      <c r="H197" s="13"/>
+      <c r="I197" s="5"/>
+    </row>
+    <row r="198" spans="2:9">
+      <c r="B198" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C198" s="13"/>
+      <c r="D198" s="13"/>
+      <c r="E198" s="13"/>
+      <c r="F198" s="13"/>
+      <c r="G198" s="13"/>
+      <c r="H198" s="13"/>
+      <c r="I198" s="5"/>
+    </row>
+    <row r="199" spans="2:9">
+      <c r="B199" s="4"/>
+      <c r="C199" s="13"/>
+      <c r="D199" s="13"/>
+      <c r="E199" s="13"/>
+      <c r="F199" s="13"/>
+      <c r="G199" s="13"/>
+      <c r="H199" s="13"/>
+      <c r="I199" s="5"/>
+    </row>
+    <row r="200" spans="2:9">
+      <c r="B200" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C200" s="13"/>
+      <c r="D200" s="13"/>
+      <c r="E200" s="13"/>
+      <c r="F200" s="13"/>
+      <c r="G200" s="13"/>
+      <c r="H200" s="13"/>
+      <c r="I200" s="5"/>
+    </row>
+    <row r="201" spans="2:9">
+      <c r="B201" s="4"/>
+      <c r="C201" s="13"/>
+      <c r="D201" s="13"/>
+      <c r="E201" s="13"/>
+      <c r="F201" s="13"/>
+      <c r="G201" s="13"/>
+      <c r="H201" s="13"/>
+      <c r="I201" s="5"/>
+    </row>
+    <row r="202" spans="2:9">
+      <c r="B202" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C202" s="13"/>
+      <c r="D202" s="13"/>
+      <c r="E202" s="13"/>
+      <c r="F202" s="13"/>
+      <c r="G202" s="13"/>
+      <c r="H202" s="13"/>
+      <c r="I202" s="5"/>
+    </row>
+    <row r="203" spans="2:9">
+      <c r="B203" s="4"/>
+      <c r="C203" s="13"/>
+      <c r="D203" s="13"/>
+      <c r="E203" s="13"/>
+      <c r="F203" s="13"/>
+      <c r="G203" s="13"/>
+      <c r="H203" s="13"/>
+      <c r="I203" s="5"/>
+    </row>
+    <row r="204" spans="2:9">
+      <c r="B204" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C204" s="13"/>
+      <c r="D204" s="13"/>
+      <c r="E204" s="13"/>
+      <c r="F204" s="13"/>
+      <c r="G204" s="13"/>
+      <c r="H204" s="13"/>
+      <c r="I204" s="5"/>
+    </row>
+    <row r="205" spans="2:9">
+      <c r="B205" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C205" s="13"/>
+      <c r="D205" s="13"/>
+      <c r="E205" s="13"/>
+      <c r="F205" s="13"/>
+      <c r="G205" s="13"/>
+      <c r="H205" s="13"/>
+      <c r="I205" s="5"/>
+    </row>
+    <row r="206" spans="2:9">
+      <c r="B206" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C206" s="13"/>
+      <c r="D206" s="13"/>
+      <c r="E206" s="13"/>
+      <c r="F206" s="13"/>
+      <c r="G206" s="13"/>
+      <c r="H206" s="13"/>
+      <c r="I206" s="5"/>
+    </row>
+    <row r="207" spans="2:9">
+      <c r="B207" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C207" s="13"/>
+      <c r="D207" s="13"/>
+      <c r="E207" s="13"/>
+      <c r="F207" s="13"/>
+      <c r="G207" s="13"/>
+      <c r="H207" s="13"/>
+      <c r="I207" s="5"/>
+    </row>
+    <row r="208" spans="2:9">
+      <c r="B208" s="4"/>
+      <c r="C208" s="13"/>
+      <c r="D208" s="13"/>
+      <c r="E208" s="13"/>
+      <c r="F208" s="13"/>
+      <c r="G208" s="13"/>
+      <c r="H208" s="13"/>
+      <c r="I208" s="5"/>
+    </row>
+    <row r="209" spans="2:9">
+      <c r="B209" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C209" s="13"/>
+      <c r="D209" s="13"/>
+      <c r="E209" s="13"/>
+      <c r="F209" s="13"/>
+      <c r="G209" s="13"/>
+      <c r="H209" s="13"/>
+      <c r="I209" s="5"/>
+    </row>
+    <row r="210" spans="2:9">
+      <c r="B210" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C210" s="13"/>
+      <c r="D210" s="13"/>
+      <c r="E210" s="13"/>
+      <c r="F210" s="13"/>
+      <c r="G210" s="13"/>
+      <c r="H210" s="13"/>
+      <c r="I210" s="5"/>
+    </row>
+    <row r="211" spans="2:9">
+      <c r="B211" s="4"/>
+      <c r="C211" s="13"/>
+      <c r="D211" s="13"/>
+      <c r="E211" s="13"/>
+      <c r="F211" s="13"/>
+      <c r="G211" s="13"/>
+      <c r="H211" s="13"/>
+      <c r="I211" s="5"/>
+    </row>
+    <row r="212" spans="2:9">
+      <c r="B212" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C212" s="13"/>
+      <c r="D212" s="13"/>
+      <c r="E212" s="13"/>
+      <c r="F212" s="13"/>
+      <c r="G212" s="13"/>
+      <c r="H212" s="13"/>
+      <c r="I212" s="5"/>
+    </row>
+    <row r="213" spans="2:9">
+      <c r="B213" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C213" s="13"/>
+      <c r="D213" s="13"/>
+      <c r="E213" s="13"/>
+      <c r="F213" s="13"/>
+      <c r="G213" s="13"/>
+      <c r="H213" s="13"/>
+      <c r="I213" s="5"/>
+    </row>
+    <row r="214" spans="2:9">
+      <c r="B214" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C214" s="13"/>
+      <c r="D214" s="13"/>
+      <c r="E214" s="13"/>
+      <c r="F214" s="13"/>
+      <c r="G214" s="13"/>
+      <c r="H214" s="13"/>
+      <c r="I214" s="5"/>
+    </row>
+    <row r="215" spans="2:9">
+      <c r="B215" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C215" s="13"/>
+      <c r="D215" s="13"/>
+      <c r="E215" s="13"/>
+      <c r="F215" s="13"/>
+      <c r="G215" s="13"/>
+      <c r="H215" s="13"/>
+      <c r="I215" s="5"/>
+    </row>
+    <row r="216" spans="2:9">
+      <c r="B216" s="4"/>
+      <c r="C216" s="13"/>
+      <c r="D216" s="13"/>
+      <c r="E216" s="13"/>
+      <c r="F216" s="13"/>
+      <c r="G216" s="13"/>
+      <c r="H216" s="13"/>
+      <c r="I216" s="5"/>
+    </row>
+    <row r="217" spans="2:9">
+      <c r="B217" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C217" s="13"/>
+      <c r="D217" s="13"/>
+      <c r="E217" s="13"/>
+      <c r="F217" s="13"/>
+      <c r="G217" s="13"/>
+      <c r="H217" s="13"/>
+      <c r="I217" s="5"/>
+    </row>
+    <row r="218" spans="2:9">
+      <c r="B218" s="4"/>
+      <c r="C218" s="13"/>
+      <c r="D218" s="13"/>
+      <c r="E218" s="13"/>
+      <c r="F218" s="13"/>
+      <c r="G218" s="13"/>
+      <c r="H218" s="13"/>
+      <c r="I218" s="5"/>
+    </row>
+    <row r="219" spans="2:9">
+      <c r="B219" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C219" s="13"/>
+      <c r="D219" s="13"/>
+      <c r="E219" s="13"/>
+      <c r="F219" s="13"/>
+      <c r="G219" s="13"/>
+      <c r="H219" s="13"/>
+      <c r="I219" s="5"/>
+    </row>
+    <row r="220" spans="2:9">
+      <c r="B220" s="4"/>
+      <c r="C220" s="13"/>
+      <c r="D220" s="13"/>
+      <c r="E220" s="13"/>
+      <c r="F220" s="13"/>
+      <c r="G220" s="13"/>
+      <c r="H220" s="13"/>
+      <c r="I220" s="5"/>
+    </row>
+    <row r="221" spans="2:9">
+      <c r="B221" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C221" s="13"/>
+      <c r="D221" s="13"/>
+      <c r="E221" s="13"/>
+      <c r="F221" s="13"/>
+      <c r="G221" s="13"/>
+      <c r="H221" s="13"/>
+      <c r="I221" s="5"/>
+    </row>
+    <row r="222" spans="2:9">
+      <c r="B222" s="4"/>
+      <c r="C222" s="13"/>
+      <c r="D222" s="13"/>
+      <c r="E222" s="13"/>
+      <c r="F222" s="13"/>
+      <c r="G222" s="13"/>
+      <c r="H222" s="13"/>
+      <c r="I222" s="5"/>
+    </row>
+    <row r="223" spans="2:9">
+      <c r="B223" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C223" s="13"/>
+      <c r="D223" s="13"/>
+      <c r="E223" s="13"/>
+      <c r="F223" s="13"/>
+      <c r="G223" s="13"/>
+      <c r="H223" s="13"/>
+      <c r="I223" s="5"/>
+    </row>
+    <row r="224" spans="2:9">
+      <c r="B224" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C224" s="13"/>
+      <c r="D224" s="13"/>
+      <c r="E224" s="13"/>
+      <c r="F224" s="13"/>
+      <c r="G224" s="13"/>
+      <c r="H224" s="13"/>
+      <c r="I224" s="5"/>
+    </row>
+    <row r="225" spans="2:11">
+      <c r="B225" s="4"/>
+      <c r="C225" s="13"/>
+      <c r="D225" s="13"/>
+      <c r="E225" s="13"/>
+      <c r="F225" s="13"/>
+      <c r="G225" s="13"/>
+      <c r="H225" s="13"/>
+      <c r="I225" s="5"/>
+    </row>
+    <row r="226" spans="2:11">
+      <c r="B226" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C226" s="13"/>
+      <c r="D226" s="13"/>
+      <c r="E226" s="13"/>
+      <c r="F226" s="13"/>
+      <c r="G226" s="13"/>
+      <c r="H226" s="13"/>
+      <c r="I226" s="5"/>
+    </row>
+    <row r="227" spans="2:11">
+      <c r="B227" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C227" s="13"/>
+      <c r="D227" s="13"/>
+      <c r="E227" s="13"/>
+      <c r="F227" s="13"/>
+      <c r="G227" s="13"/>
+      <c r="H227" s="13"/>
+      <c r="I227" s="5"/>
+    </row>
+    <row r="228" spans="2:11">
+      <c r="B228" s="4"/>
+      <c r="C228" s="13"/>
+      <c r="D228" s="13"/>
+      <c r="E228" s="13"/>
+      <c r="F228" s="13"/>
+      <c r="G228" s="13"/>
+      <c r="H228" s="13"/>
+      <c r="I228" s="5"/>
+    </row>
+    <row r="229" spans="2:11">
+      <c r="B229" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C229" s="13"/>
+      <c r="D229" s="13"/>
+      <c r="E229" s="13"/>
+      <c r="F229" s="13"/>
+      <c r="G229" s="13"/>
+      <c r="H229" s="13"/>
+      <c r="I229" s="5"/>
+    </row>
+    <row r="230" spans="2:11">
+      <c r="B230" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C230" s="13"/>
+      <c r="D230" s="13"/>
+      <c r="E230" s="13"/>
+      <c r="F230" s="13"/>
+      <c r="G230" s="13"/>
+      <c r="H230" s="13"/>
+      <c r="I230" s="5"/>
+    </row>
+    <row r="231" spans="2:11">
+      <c r="B231" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C231" s="13"/>
+      <c r="D231" s="13"/>
+      <c r="E231" s="13"/>
+      <c r="F231" s="13"/>
+      <c r="G231" s="13"/>
+      <c r="H231" s="13"/>
+      <c r="I231" s="5"/>
+    </row>
+    <row r="232" spans="2:11">
+      <c r="B232" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C232" s="13"/>
+      <c r="D232" s="13"/>
+      <c r="E232" s="13"/>
+      <c r="F232" s="13"/>
+      <c r="G232" s="13"/>
+      <c r="H232" s="13"/>
+      <c r="I232" s="5"/>
+    </row>
+    <row r="233" spans="2:11">
+      <c r="B233" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C233" s="13"/>
+      <c r="D233" s="13"/>
+      <c r="E233" s="13"/>
+      <c r="F233" s="13"/>
+      <c r="G233" s="13"/>
+      <c r="H233" s="13"/>
+      <c r="I233" s="5"/>
+    </row>
+    <row r="234" spans="2:11">
+      <c r="B234" s="4"/>
+      <c r="C234" s="13"/>
+      <c r="D234" s="13"/>
+      <c r="E234" s="13"/>
+      <c r="F234" s="13"/>
+      <c r="G234" s="13"/>
+      <c r="H234" s="13"/>
+      <c r="I234" s="5"/>
+    </row>
+    <row r="235" spans="2:11">
+      <c r="B235" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C235" s="13"/>
+      <c r="D235" s="13"/>
+      <c r="E235" s="13"/>
+      <c r="F235" s="13"/>
+      <c r="G235" s="13"/>
+      <c r="H235" s="13"/>
+      <c r="I235" s="5"/>
+    </row>
+    <row r="236" spans="2:11">
+      <c r="B236" s="4"/>
+      <c r="C236" s="13"/>
+      <c r="D236" s="13"/>
+      <c r="E236" s="13"/>
+      <c r="F236" s="13"/>
+      <c r="G236" s="13"/>
+      <c r="H236" s="13"/>
+      <c r="I236" s="5"/>
+    </row>
+    <row r="237" spans="2:11">
+      <c r="B237" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C237" s="13"/>
+      <c r="D237" s="13"/>
+      <c r="E237" s="13"/>
+      <c r="F237" s="13"/>
+      <c r="G237" s="13"/>
+      <c r="H237" s="13"/>
+      <c r="I237" s="5"/>
+    </row>
+    <row r="238" spans="2:11">
+      <c r="B238" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C238" s="13"/>
+      <c r="D238" s="13"/>
+      <c r="E238" s="13"/>
+      <c r="F238" s="13"/>
+      <c r="G238" s="13"/>
+      <c r="H238" s="13"/>
+      <c r="I238" s="5"/>
+    </row>
+    <row r="239" spans="2:11">
+      <c r="B239" s="4"/>
+      <c r="C239" s="13"/>
+      <c r="D239" s="13"/>
+      <c r="E239" s="13"/>
+      <c r="F239" s="13"/>
+      <c r="G239" s="13"/>
+      <c r="H239" s="13"/>
+      <c r="I239" s="5"/>
+    </row>
+    <row r="240" spans="2:11">
+      <c r="B240" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C240" s="13"/>
+      <c r="D240" s="13"/>
+      <c r="E240" s="13"/>
+      <c r="F240" s="13"/>
+      <c r="G240" s="13"/>
+      <c r="H240" s="13"/>
+      <c r="I240" s="5"/>
+      <c r="J240" t="s">
+        <v>17</v>
+      </c>
+      <c r="K240" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="241" spans="2:11">
+      <c r="B241" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C241" s="13"/>
+      <c r="D241" s="13"/>
+      <c r="E241" s="13"/>
+      <c r="F241" s="13"/>
+      <c r="G241" s="13"/>
+      <c r="H241" s="13"/>
+      <c r="I241" s="5"/>
+      <c r="K241" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="242" spans="2:11">
+      <c r="B242" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C242" s="13"/>
+      <c r="D242" s="13"/>
+      <c r="E242" s="13"/>
+      <c r="F242" s="13"/>
+      <c r="G242" s="13"/>
+      <c r="H242" s="13"/>
+      <c r="I242" s="5"/>
+    </row>
+    <row r="243" spans="2:11">
+      <c r="B243" s="14"/>
+      <c r="C243" s="13"/>
+      <c r="D243" s="13"/>
+      <c r="E243" s="13"/>
+      <c r="F243" s="13"/>
+      <c r="G243" s="13"/>
+      <c r="H243" s="13"/>
+      <c r="I243" s="5"/>
+    </row>
+    <row r="244" spans="2:11">
+      <c r="B244" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C244" s="13"/>
+      <c r="D244" s="13"/>
+      <c r="E244" s="13"/>
+      <c r="F244" s="13"/>
+      <c r="G244" s="13"/>
+      <c r="H244" s="13"/>
+      <c r="I244" s="5"/>
+    </row>
+    <row r="245" spans="2:11">
+      <c r="B245" s="14"/>
+      <c r="C245" s="13"/>
+      <c r="D245" s="13"/>
+      <c r="E245" s="13"/>
+      <c r="F245" s="13"/>
+      <c r="G245" s="13"/>
+      <c r="H245" s="13"/>
+      <c r="I245" s="5"/>
+    </row>
+    <row r="246" spans="2:11">
+      <c r="B246" s="14" t="s">
+        <v>259</v>
+      </c>
+      <c r="C246" s="13"/>
+      <c r="D246" s="13"/>
+      <c r="E246" s="13"/>
+      <c r="F246" s="13"/>
+      <c r="G246" s="13"/>
+      <c r="H246" s="13"/>
+      <c r="I246" s="5"/>
+    </row>
+    <row r="247" spans="2:11">
+      <c r="B247" s="14" t="s">
+        <v>260</v>
+      </c>
+      <c r="C247" s="13"/>
+      <c r="D247" s="13"/>
+      <c r="E247" s="13"/>
+      <c r="F247" s="13"/>
+      <c r="G247" s="13"/>
+      <c r="H247" s="13"/>
+      <c r="I247" s="5"/>
+    </row>
+    <row r="248" spans="2:11">
+      <c r="B248" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="C248" s="13"/>
+      <c r="D248" s="13"/>
+      <c r="E248" s="13"/>
+      <c r="F248" s="13"/>
+      <c r="G248" s="13"/>
+      <c r="H248" s="13"/>
+      <c r="I248" s="5"/>
+      <c r="J248" t="s">
+        <v>17</v>
+      </c>
+      <c r="K248" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="249" spans="2:11">
+      <c r="B249" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C249" s="13"/>
+      <c r="D249" s="13"/>
+      <c r="E249" s="13"/>
+      <c r="F249" s="13"/>
+      <c r="G249" s="13"/>
+      <c r="H249" s="13"/>
+      <c r="I249" s="5"/>
+      <c r="K249" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="250" spans="2:11">
+      <c r="B250" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C250" s="13"/>
+      <c r="D250" s="13"/>
+      <c r="E250" s="13"/>
+      <c r="F250" s="13"/>
+      <c r="G250" s="13"/>
+      <c r="H250" s="13"/>
+      <c r="I250" s="5"/>
+    </row>
+    <row r="251" spans="2:11">
+      <c r="B251" s="14"/>
+      <c r="C251" s="13"/>
+      <c r="D251" s="13"/>
+      <c r="E251" s="13"/>
+      <c r="F251" s="13"/>
+      <c r="G251" s="13"/>
+      <c r="H251" s="13"/>
+      <c r="I251" s="5"/>
+    </row>
+    <row r="252" spans="2:11">
+      <c r="B252" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C252" s="13"/>
+      <c r="D252" s="13"/>
+      <c r="E252" s="13"/>
+      <c r="F252" s="13"/>
+      <c r="G252" s="13"/>
+      <c r="H252" s="13"/>
+      <c r="I252" s="5"/>
+    </row>
+    <row r="253" spans="2:11">
+      <c r="B253" s="14"/>
+      <c r="C253" s="13"/>
+      <c r="D253" s="13"/>
+      <c r="E253" s="13"/>
+      <c r="F253" s="13"/>
+      <c r="G253" s="13"/>
+      <c r="H253" s="13"/>
+      <c r="I253" s="5"/>
+    </row>
+    <row r="254" spans="2:11">
+      <c r="B254" s="14" t="s">
+        <v>264</v>
+      </c>
+      <c r="C254" s="13"/>
+      <c r="D254" s="13"/>
+      <c r="E254" s="13"/>
+      <c r="F254" s="13"/>
+      <c r="G254" s="13"/>
+      <c r="H254" s="13"/>
+      <c r="I254" s="5"/>
+    </row>
+    <row r="255" spans="2:11">
+      <c r="B255" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C255" s="13"/>
+      <c r="D255" s="13"/>
+      <c r="E255" s="13"/>
+      <c r="F255" s="13"/>
+      <c r="G255" s="13"/>
+      <c r="H255" s="13"/>
+      <c r="I255" s="5"/>
+    </row>
+    <row r="256" spans="2:11">
+      <c r="B256" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="C256" s="13"/>
+      <c r="D256" s="13"/>
+      <c r="E256" s="13"/>
+      <c r="F256" s="13"/>
+      <c r="G256" s="13"/>
+      <c r="H256" s="13"/>
+      <c r="I256" s="5"/>
+      <c r="J256" t="s">
+        <v>17</v>
+      </c>
+      <c r="K256" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="257" spans="2:11">
+      <c r="B257" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C257" s="13"/>
+      <c r="D257" s="13"/>
+      <c r="E257" s="13"/>
+      <c r="F257" s="13"/>
+      <c r="G257" s="13"/>
+      <c r="H257" s="13"/>
+      <c r="I257" s="5"/>
+    </row>
+    <row r="258" spans="2:11">
+      <c r="B258" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C258" s="13"/>
+      <c r="D258" s="13"/>
+      <c r="E258" s="13"/>
+      <c r="F258" s="13"/>
+      <c r="G258" s="13"/>
+      <c r="H258" s="13"/>
+      <c r="I258" s="5"/>
+    </row>
+    <row r="259" spans="2:11">
+      <c r="B259" s="14"/>
+      <c r="C259" s="13"/>
+      <c r="D259" s="13"/>
+      <c r="E259" s="13"/>
+      <c r="F259" s="13"/>
+      <c r="G259" s="13"/>
+      <c r="H259" s="13"/>
+      <c r="I259" s="5"/>
+    </row>
+    <row r="260" spans="2:11">
+      <c r="B260" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="C260" s="13"/>
+      <c r="D260" s="13"/>
+      <c r="E260" s="13"/>
+      <c r="F260" s="13"/>
+      <c r="G260" s="13"/>
+      <c r="H260" s="13"/>
+      <c r="I260" s="5"/>
+      <c r="J260" t="s">
+        <v>17</v>
+      </c>
+      <c r="K260" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="261" spans="2:11">
+      <c r="B261" s="14"/>
+      <c r="C261" s="13"/>
+      <c r="D261" s="13"/>
+      <c r="E261" s="13"/>
+      <c r="F261" s="13"/>
+      <c r="G261" s="13"/>
+      <c r="H261" s="13"/>
+      <c r="I261" s="5"/>
+      <c r="K261" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="262" spans="2:11">
+      <c r="B262" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="C262" s="13"/>
+      <c r="D262" s="13"/>
+      <c r="E262" s="13"/>
+      <c r="F262" s="13"/>
+      <c r="G262" s="13"/>
+      <c r="H262" s="13"/>
+      <c r="I262" s="5"/>
+      <c r="K262" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="263" spans="2:11">
+      <c r="B263" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C263" s="13"/>
+      <c r="D263" s="13"/>
+      <c r="E263" s="13"/>
+      <c r="F263" s="13"/>
+      <c r="G263" s="13"/>
+      <c r="H263" s="13"/>
+      <c r="I263" s="5"/>
+      <c r="K263" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="264" spans="2:11">
+      <c r="B264" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="C264" s="13"/>
+      <c r="D264" s="13"/>
+      <c r="E264" s="13"/>
+      <c r="F264" s="13"/>
+      <c r="G264" s="13"/>
+      <c r="H264" s="13"/>
+      <c r="I264" s="5"/>
+      <c r="K264" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="265" spans="2:11">
+      <c r="B265" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C265" s="13"/>
+      <c r="D265" s="13"/>
+      <c r="E265" s="13"/>
+      <c r="F265" s="13"/>
+      <c r="G265" s="13"/>
+      <c r="H265" s="13"/>
+      <c r="I265" s="5"/>
+    </row>
+    <row r="266" spans="2:11">
+      <c r="B266" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C266" s="13"/>
+      <c r="D266" s="13"/>
+      <c r="E266" s="13"/>
+      <c r="F266" s="13"/>
+      <c r="G266" s="13"/>
+      <c r="H266" s="13"/>
+      <c r="I266" s="5"/>
+    </row>
+    <row r="267" spans="2:11">
+      <c r="B267" s="14"/>
+      <c r="C267" s="13"/>
+      <c r="D267" s="13"/>
+      <c r="E267" s="13"/>
+      <c r="F267" s="13"/>
+      <c r="G267" s="13"/>
+      <c r="H267" s="13"/>
+      <c r="I267" s="5"/>
+    </row>
+    <row r="268" spans="2:11">
+      <c r="B268" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="C268" s="13"/>
+      <c r="D268" s="13"/>
+      <c r="E268" s="13"/>
+      <c r="F268" s="13"/>
+      <c r="G268" s="13"/>
+      <c r="H268" s="13"/>
+      <c r="I268" s="5"/>
+    </row>
+    <row r="269" spans="2:11">
+      <c r="B269" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="C269" s="13"/>
+      <c r="D269" s="13"/>
+      <c r="E269" s="13"/>
+      <c r="F269" s="13"/>
+      <c r="G269" s="13"/>
+      <c r="H269" s="13"/>
+      <c r="I269" s="5"/>
+    </row>
+    <row r="270" spans="2:11">
+      <c r="B270" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C270" s="13"/>
+      <c r="D270" s="13"/>
+      <c r="E270" s="13"/>
+      <c r="F270" s="13"/>
+      <c r="G270" s="13"/>
+      <c r="H270" s="13"/>
+      <c r="I270" s="5"/>
+    </row>
+    <row r="271" spans="2:11">
+      <c r="B271" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C271" s="8"/>
+      <c r="D271" s="8"/>
+      <c r="E271" s="8"/>
+      <c r="F271" s="8"/>
+      <c r="G271" s="8"/>
+      <c r="H271" s="8"/>
+      <c r="I271" s="9"/>
+    </row>
+    <row r="274" spans="1:18">
+      <c r="A274" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="275" spans="1:18">
+      <c r="B275" s="1"/>
+      <c r="C275" s="2"/>
+      <c r="D275" s="2"/>
+      <c r="E275" s="2"/>
+      <c r="F275" s="2"/>
+      <c r="G275" s="2"/>
+      <c r="H275" s="2"/>
+      <c r="I275" s="2"/>
+      <c r="J275" s="2"/>
+      <c r="K275" s="2"/>
+      <c r="L275" s="2"/>
+      <c r="M275" s="2"/>
+      <c r="N275" s="2"/>
+      <c r="O275" s="2"/>
+      <c r="P275" s="2"/>
+      <c r="Q275" s="2"/>
+      <c r="R275" s="3"/>
+    </row>
+    <row r="276" spans="1:18">
+      <c r="B276" s="4"/>
+      <c r="C276" s="13"/>
+      <c r="D276" s="13"/>
+      <c r="E276" s="13"/>
+      <c r="F276" s="13"/>
+      <c r="G276" s="13"/>
+      <c r="H276" s="13"/>
+      <c r="I276" s="13"/>
+      <c r="J276" s="13"/>
+      <c r="K276" s="13"/>
+      <c r="L276" s="13"/>
+      <c r="M276" s="13"/>
+      <c r="N276" s="13"/>
+      <c r="O276" s="13"/>
+      <c r="P276" s="13"/>
+      <c r="Q276" s="13"/>
+      <c r="R276" s="5"/>
+    </row>
+    <row r="277" spans="1:18">
+      <c r="B277" s="4"/>
+      <c r="C277" s="13"/>
+      <c r="D277" s="13"/>
+      <c r="E277" s="13"/>
+      <c r="F277" s="13"/>
+      <c r="G277" s="13"/>
+      <c r="H277" s="13"/>
+      <c r="I277" s="13"/>
+      <c r="J277" s="13"/>
+      <c r="K277" s="13"/>
+      <c r="L277" s="13"/>
+      <c r="M277" s="13"/>
+      <c r="N277" s="13"/>
+      <c r="O277" s="13"/>
+      <c r="P277" s="13"/>
+      <c r="Q277" s="13"/>
+      <c r="R277" s="5"/>
+    </row>
+    <row r="278" spans="1:18">
+      <c r="B278" s="4"/>
+      <c r="C278" s="13"/>
+      <c r="D278" s="13"/>
+      <c r="E278" s="13"/>
+      <c r="F278" s="13"/>
+      <c r="G278" s="13"/>
+      <c r="H278" s="13"/>
+      <c r="I278" s="13"/>
+      <c r="J278" s="13"/>
+      <c r="K278" s="13"/>
+      <c r="L278" s="13"/>
+      <c r="M278" s="13"/>
+      <c r="N278" s="13"/>
+      <c r="O278" s="13"/>
+      <c r="P278" s="13"/>
+      <c r="Q278" s="13"/>
+      <c r="R278" s="5"/>
+    </row>
+    <row r="279" spans="1:18">
+      <c r="B279" s="4"/>
+      <c r="C279" s="13"/>
+      <c r="D279" s="13"/>
+      <c r="E279" s="13"/>
+      <c r="F279" s="13"/>
+      <c r="G279" s="13"/>
+      <c r="H279" s="13"/>
+      <c r="I279" s="13"/>
+      <c r="J279" s="13"/>
+      <c r="K279" s="13"/>
+      <c r="L279" s="13"/>
+      <c r="M279" s="13"/>
+      <c r="N279" s="13"/>
+      <c r="O279" s="13"/>
+      <c r="P279" s="13"/>
+      <c r="Q279" s="13"/>
+      <c r="R279" s="5"/>
+    </row>
+    <row r="280" spans="1:18">
+      <c r="B280" s="4"/>
+      <c r="C280" s="13"/>
+      <c r="D280" s="13"/>
+      <c r="E280" s="13"/>
+      <c r="F280" s="13"/>
+      <c r="G280" s="13"/>
+      <c r="H280" s="13"/>
+      <c r="I280" s="13"/>
+      <c r="J280" s="13"/>
+      <c r="K280" s="13"/>
+      <c r="L280" s="13"/>
+      <c r="M280" s="13"/>
+      <c r="N280" s="13"/>
+      <c r="O280" s="13"/>
+      <c r="P280" s="13"/>
+      <c r="Q280" s="13"/>
+      <c r="R280" s="5"/>
+    </row>
+    <row r="281" spans="1:18">
+      <c r="B281" s="4"/>
+      <c r="C281" s="13"/>
+      <c r="D281" s="13"/>
+      <c r="E281" s="13"/>
+      <c r="F281" s="13"/>
+      <c r="G281" s="13"/>
+      <c r="H281" s="13"/>
+      <c r="I281" s="13"/>
+      <c r="J281" s="13"/>
+      <c r="K281" s="13"/>
+      <c r="L281" s="13"/>
+      <c r="M281" s="13"/>
+      <c r="N281" s="13"/>
+      <c r="O281" s="13"/>
+      <c r="P281" s="13"/>
+      <c r="Q281" s="13"/>
+      <c r="R281" s="5"/>
+    </row>
+    <row r="282" spans="1:18">
+      <c r="B282" s="4"/>
+      <c r="C282" s="13"/>
+      <c r="D282" s="13"/>
+      <c r="E282" s="13"/>
+      <c r="F282" s="13"/>
+      <c r="G282" s="13"/>
+      <c r="H282" s="13"/>
+      <c r="I282" s="13"/>
+      <c r="J282" s="13"/>
+      <c r="K282" s="13"/>
+      <c r="L282" s="13"/>
+      <c r="M282" s="13"/>
+      <c r="N282" s="13"/>
+      <c r="O282" s="13"/>
+      <c r="P282" s="13"/>
+      <c r="Q282" s="13"/>
+      <c r="R282" s="5"/>
+    </row>
+    <row r="283" spans="1:18">
+      <c r="B283" s="4"/>
+      <c r="C283" s="13"/>
+      <c r="D283" s="13"/>
+      <c r="E283" s="13"/>
+      <c r="F283" s="13"/>
+      <c r="G283" s="13"/>
+      <c r="H283" s="13"/>
+      <c r="I283" s="13"/>
+      <c r="J283" s="13"/>
+      <c r="K283" s="13"/>
+      <c r="L283" s="13"/>
+      <c r="M283" s="13"/>
+      <c r="N283" s="13"/>
+      <c r="O283" s="13"/>
+      <c r="P283" s="13"/>
+      <c r="Q283" s="13"/>
+      <c r="R283" s="5"/>
+    </row>
+    <row r="284" spans="1:18">
+      <c r="B284" s="4"/>
+      <c r="C284" s="13"/>
+      <c r="D284" s="13"/>
+      <c r="E284" s="13"/>
+      <c r="F284" s="13"/>
+      <c r="G284" s="13"/>
+      <c r="H284" s="13"/>
+      <c r="I284" s="13"/>
+      <c r="J284" s="13"/>
+      <c r="K284" s="13"/>
+      <c r="L284" s="13"/>
+      <c r="M284" s="13"/>
+      <c r="N284" s="13"/>
+      <c r="O284" s="13"/>
+      <c r="P284" s="13"/>
+      <c r="Q284" s="13"/>
+      <c r="R284" s="5"/>
+    </row>
+    <row r="285" spans="1:18">
+      <c r="B285" s="4"/>
+      <c r="C285" s="13"/>
+      <c r="D285" s="13"/>
+      <c r="E285" s="13"/>
+      <c r="F285" s="13"/>
+      <c r="G285" s="13"/>
+      <c r="H285" s="13"/>
+      <c r="I285" s="13"/>
+      <c r="J285" s="13"/>
+      <c r="K285" s="13"/>
+      <c r="L285" s="13"/>
+      <c r="M285" s="13"/>
+      <c r="N285" s="13"/>
+      <c r="O285" s="13"/>
+      <c r="P285" s="13"/>
+      <c r="Q285" s="13"/>
+      <c r="R285" s="5"/>
+    </row>
+    <row r="286" spans="1:18">
+      <c r="B286" s="4"/>
+      <c r="C286" s="13"/>
+      <c r="D286" s="13"/>
+      <c r="E286" s="13"/>
+      <c r="F286" s="13"/>
+      <c r="G286" s="13"/>
+      <c r="H286" s="13"/>
+      <c r="I286" s="13"/>
+      <c r="J286" s="13"/>
+      <c r="K286" s="13"/>
+      <c r="L286" s="13"/>
+      <c r="M286" s="13"/>
+      <c r="N286" s="13"/>
+      <c r="O286" s="13"/>
+      <c r="P286" s="13"/>
+      <c r="Q286" s="13"/>
+      <c r="R286" s="5"/>
+    </row>
+    <row r="287" spans="1:18">
+      <c r="B287" s="4"/>
+      <c r="C287" s="13"/>
+      <c r="D287" s="13"/>
+      <c r="E287" s="13"/>
+      <c r="F287" s="13"/>
+      <c r="G287" s="13"/>
+      <c r="H287" s="13"/>
+      <c r="I287" s="13"/>
+      <c r="J287" s="13"/>
+      <c r="K287" s="13"/>
+      <c r="L287" s="13"/>
+      <c r="M287" s="13"/>
+      <c r="N287" s="13"/>
+      <c r="O287" s="13"/>
+      <c r="P287" s="13"/>
+      <c r="Q287" s="13"/>
+      <c r="R287" s="5"/>
+    </row>
+    <row r="288" spans="1:18">
+      <c r="B288" s="4"/>
+      <c r="C288" s="13"/>
+      <c r="D288" s="13"/>
+      <c r="E288" s="13"/>
+      <c r="F288" s="13"/>
+      <c r="G288" s="13"/>
+      <c r="H288" s="13"/>
+      <c r="I288" s="13"/>
+      <c r="J288" s="13"/>
+      <c r="K288" s="13"/>
+      <c r="L288" s="13"/>
+      <c r="M288" s="13"/>
+      <c r="N288" s="13"/>
+      <c r="O288" s="13"/>
+      <c r="P288" s="13"/>
+      <c r="Q288" s="13"/>
+      <c r="R288" s="5"/>
+    </row>
+    <row r="289" spans="2:18">
+      <c r="B289" s="4"/>
+      <c r="C289" s="13"/>
+      <c r="D289" s="13"/>
+      <c r="E289" s="13"/>
+      <c r="F289" s="13"/>
+      <c r="G289" s="13"/>
+      <c r="H289" s="13"/>
+      <c r="I289" s="13"/>
+      <c r="J289" s="13"/>
+      <c r="K289" s="13"/>
+      <c r="L289" s="13"/>
+      <c r="M289" s="13"/>
+      <c r="N289" s="13"/>
+      <c r="O289" s="13"/>
+      <c r="P289" s="13"/>
+      <c r="Q289" s="13"/>
+      <c r="R289" s="5"/>
+    </row>
+    <row r="290" spans="2:18">
+      <c r="B290" s="4"/>
+      <c r="C290" s="13"/>
+      <c r="D290" s="13"/>
+      <c r="E290" s="13"/>
+      <c r="F290" s="13"/>
+      <c r="G290" s="13"/>
+      <c r="H290" s="13"/>
+      <c r="I290" s="13"/>
+      <c r="J290" s="13"/>
+      <c r="K290" s="13"/>
+      <c r="L290" s="13"/>
+      <c r="M290" s="13"/>
+      <c r="N290" s="13"/>
+      <c r="O290" s="13"/>
+      <c r="P290" s="13"/>
+      <c r="Q290" s="13"/>
+      <c r="R290" s="5"/>
+    </row>
+    <row r="291" spans="2:18">
+      <c r="B291" s="4"/>
+      <c r="C291" s="13"/>
+      <c r="D291" s="13"/>
+      <c r="E291" s="13"/>
+      <c r="F291" s="13"/>
+      <c r="G291" s="13"/>
+      <c r="H291" s="13"/>
+      <c r="I291" s="13"/>
+      <c r="J291" s="13"/>
+      <c r="K291" s="13"/>
+      <c r="L291" s="13"/>
+      <c r="M291" s="13"/>
+      <c r="N291" s="13"/>
+      <c r="O291" s="13"/>
+      <c r="P291" s="13"/>
+      <c r="Q291" s="13"/>
+      <c r="R291" s="5"/>
+    </row>
+    <row r="292" spans="2:18">
+      <c r="B292" s="4"/>
+      <c r="C292" s="13"/>
+      <c r="D292" s="13"/>
+      <c r="E292" s="13"/>
+      <c r="F292" s="13"/>
+      <c r="G292" s="13"/>
+      <c r="H292" s="13"/>
+      <c r="I292" s="13"/>
+      <c r="J292" s="13"/>
+      <c r="K292" s="13"/>
+      <c r="L292" s="13"/>
+      <c r="M292" s="13"/>
+      <c r="N292" s="13"/>
+      <c r="O292" s="13"/>
+      <c r="P292" s="13"/>
+      <c r="Q292" s="13"/>
+      <c r="R292" s="5"/>
+    </row>
+    <row r="293" spans="2:18">
+      <c r="B293" s="4"/>
+      <c r="C293" s="13"/>
+      <c r="D293" s="13"/>
+      <c r="E293" s="13"/>
+      <c r="F293" s="13"/>
+      <c r="G293" s="13"/>
+      <c r="H293" s="13"/>
+      <c r="I293" s="13"/>
+      <c r="J293" s="13"/>
+      <c r="K293" s="13"/>
+      <c r="L293" s="13"/>
+      <c r="M293" s="13"/>
+      <c r="N293" s="13"/>
+      <c r="O293" s="13"/>
+      <c r="P293" s="13"/>
+      <c r="Q293" s="13"/>
+      <c r="R293" s="5"/>
+    </row>
+    <row r="294" spans="2:18">
+      <c r="B294" s="4"/>
+      <c r="C294" s="13"/>
+      <c r="D294" s="13"/>
+      <c r="E294" s="13"/>
+      <c r="F294" s="13"/>
+      <c r="G294" s="13"/>
+      <c r="H294" s="13"/>
+      <c r="I294" s="13"/>
+      <c r="J294" s="13"/>
+      <c r="K294" s="13"/>
+      <c r="L294" s="13"/>
+      <c r="M294" s="13"/>
+      <c r="N294" s="13"/>
+      <c r="O294" s="13"/>
+      <c r="P294" s="13"/>
+      <c r="Q294" s="13"/>
+      <c r="R294" s="5"/>
+    </row>
+    <row r="295" spans="2:18">
+      <c r="B295" s="4"/>
+      <c r="C295" s="13"/>
+      <c r="D295" s="13"/>
+      <c r="E295" s="13"/>
+      <c r="F295" s="13"/>
+      <c r="G295" s="13"/>
+      <c r="H295" s="13"/>
+      <c r="I295" s="13"/>
+      <c r="J295" s="13"/>
+      <c r="K295" s="13"/>
+      <c r="L295" s="13"/>
+      <c r="M295" s="13"/>
+      <c r="N295" s="13"/>
+      <c r="O295" s="13"/>
+      <c r="P295" s="13"/>
+      <c r="Q295" s="13"/>
+      <c r="R295" s="5"/>
+    </row>
+    <row r="296" spans="2:18">
+      <c r="B296" s="4"/>
+      <c r="C296" s="13"/>
+      <c r="D296" s="13"/>
+      <c r="E296" s="13"/>
+      <c r="F296" s="13"/>
+      <c r="G296" s="13"/>
+      <c r="H296" s="13"/>
+      <c r="I296" s="13"/>
+      <c r="J296" s="13"/>
+      <c r="K296" s="13"/>
+      <c r="L296" s="13"/>
+      <c r="M296" s="13"/>
+      <c r="N296" s="13"/>
+      <c r="O296" s="13"/>
+      <c r="P296" s="13"/>
+      <c r="Q296" s="13"/>
+      <c r="R296" s="5"/>
+    </row>
+    <row r="297" spans="2:18">
+      <c r="B297" s="4"/>
+      <c r="C297" s="13"/>
+      <c r="D297" s="13"/>
+      <c r="E297" s="13"/>
+      <c r="F297" s="13"/>
+      <c r="G297" s="13"/>
+      <c r="H297" s="13"/>
+      <c r="I297" s="13"/>
+      <c r="J297" s="13"/>
+      <c r="K297" s="13"/>
+      <c r="L297" s="13"/>
+      <c r="M297" s="13"/>
+      <c r="N297" s="13"/>
+      <c r="O297" s="13"/>
+      <c r="P297" s="13"/>
+      <c r="Q297" s="13"/>
+      <c r="R297" s="5"/>
+    </row>
+    <row r="298" spans="2:18">
+      <c r="B298" s="4"/>
+      <c r="C298" s="13"/>
+      <c r="D298" s="13"/>
+      <c r="E298" s="13"/>
+      <c r="F298" s="13"/>
+      <c r="G298" s="13"/>
+      <c r="H298" s="13"/>
+      <c r="I298" s="13"/>
+      <c r="J298" s="13"/>
+      <c r="K298" s="13"/>
+      <c r="L298" s="13"/>
+      <c r="M298" s="13"/>
+      <c r="N298" s="13"/>
+      <c r="O298" s="13"/>
+      <c r="P298" s="13"/>
+      <c r="Q298" s="13"/>
+      <c r="R298" s="5"/>
+    </row>
+    <row r="299" spans="2:18">
+      <c r="B299" s="4"/>
+      <c r="C299" s="13"/>
+      <c r="D299" s="13"/>
+      <c r="E299" s="13"/>
+      <c r="F299" s="13"/>
+      <c r="G299" s="13"/>
+      <c r="H299" s="13"/>
+      <c r="I299" s="13"/>
+      <c r="J299" s="13"/>
+      <c r="K299" s="13"/>
+      <c r="L299" s="13"/>
+      <c r="M299" s="13"/>
+      <c r="N299" s="13"/>
+      <c r="O299" s="13"/>
+      <c r="P299" s="13"/>
+      <c r="Q299" s="13"/>
+      <c r="R299" s="5"/>
+    </row>
+    <row r="300" spans="2:18">
+      <c r="B300" s="4"/>
+      <c r="C300" s="13"/>
+      <c r="D300" s="13"/>
+      <c r="E300" s="13"/>
+      <c r="F300" s="13"/>
+      <c r="G300" s="13"/>
+      <c r="H300" s="13"/>
+      <c r="I300" s="13"/>
+      <c r="J300" s="13"/>
+      <c r="K300" s="13"/>
+      <c r="L300" s="13"/>
+      <c r="M300" s="13"/>
+      <c r="N300" s="13"/>
+      <c r="O300" s="13"/>
+      <c r="P300" s="13"/>
+      <c r="Q300" s="13"/>
+      <c r="R300" s="5"/>
+    </row>
+    <row r="301" spans="2:18">
+      <c r="B301" s="4"/>
+      <c r="C301" s="13"/>
+      <c r="D301" s="13"/>
+      <c r="E301" s="13"/>
+      <c r="F301" s="13"/>
+      <c r="G301" s="13"/>
+      <c r="H301" s="13"/>
+      <c r="I301" s="13"/>
+      <c r="J301" s="13"/>
+      <c r="K301" s="13"/>
+      <c r="L301" s="13"/>
+      <c r="M301" s="13"/>
+      <c r="N301" s="13"/>
+      <c r="O301" s="13"/>
+      <c r="P301" s="13"/>
+      <c r="Q301" s="13"/>
+      <c r="R301" s="5"/>
+    </row>
+    <row r="302" spans="2:18">
+      <c r="B302" s="4"/>
+      <c r="C302" s="13"/>
+      <c r="D302" s="13"/>
+      <c r="E302" s="13"/>
+      <c r="F302" s="13"/>
+      <c r="G302" s="13"/>
+      <c r="H302" s="13"/>
+      <c r="I302" s="13"/>
+      <c r="J302" s="13"/>
+      <c r="K302" s="13"/>
+      <c r="L302" s="13"/>
+      <c r="M302" s="13"/>
+      <c r="N302" s="13"/>
+      <c r="O302" s="13"/>
+      <c r="P302" s="13"/>
+      <c r="Q302" s="13"/>
+      <c r="R302" s="5"/>
+    </row>
+    <row r="303" spans="2:18">
+      <c r="B303" s="4"/>
+      <c r="C303" s="13"/>
+      <c r="D303" s="13"/>
+      <c r="E303" s="13"/>
+      <c r="F303" s="13"/>
+      <c r="G303" s="13"/>
+      <c r="H303" s="13"/>
+      <c r="I303" s="13"/>
+      <c r="J303" s="13"/>
+      <c r="K303" s="13"/>
+      <c r="L303" s="13"/>
+      <c r="M303" s="13"/>
+      <c r="N303" s="13"/>
+      <c r="O303" s="13"/>
+      <c r="P303" s="13"/>
+      <c r="Q303" s="13"/>
+      <c r="R303" s="5"/>
+    </row>
+    <row r="304" spans="2:18">
+      <c r="B304" s="7"/>
+      <c r="C304" s="8"/>
+      <c r="D304" s="8"/>
+      <c r="E304" s="8"/>
+      <c r="F304" s="8"/>
+      <c r="G304" s="8"/>
+      <c r="H304" s="8"/>
+      <c r="I304" s="8"/>
+      <c r="J304" s="8"/>
+      <c r="K304" s="8"/>
+      <c r="L304" s="8"/>
+      <c r="M304" s="8"/>
+      <c r="N304" s="8"/>
+      <c r="O304" s="8"/>
+      <c r="P304" s="8"/>
+      <c r="Q304" s="8"/>
+      <c r="R304" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the record in the database and return a 200 status code
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/3.create-update-and-delete-individual-resources.xlsx
+++ b/me/4.create-a-restful-api/3.create-update-and-delete-individual-resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2957A2E6-9E1B-4940-9992-EA9A57D5390F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A890080A-47C5-4473-A306-36B47A56E0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="get request JSON data" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Validate data respond 422status" sheetId="4" r:id="rId4"/>
     <sheet name="validate update existing record" sheetId="5" r:id="rId5"/>
     <sheet name="get data from request update" sheetId="6" r:id="rId6"/>
+    <sheet name="Update record status 200" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="341">
   <si>
     <t>構成</t>
   </si>
@@ -1055,6 +1056,192 @@
   </si>
   <si>
     <t>giá trị true nên priority cũng phải dùng array_key_exists() để check</t>
+  </si>
+  <si>
+    <t>Update the record in the database and return a 200 status code</t>
+  </si>
+  <si>
+    <t>$sets=</t>
+  </si>
+  <si>
+    <t>implode(", ", $sets) = "name = :name, priority = :priority, is_completed = :is_completed"</t>
+  </si>
+  <si>
+    <t>$sql="UPDATE task SET name = :name, priority = :priority, is_completed = :is_completed WHERE id = :id"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        $fields = [];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if ( ! empty($data["name"])) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">            $fields["name"] = [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                $data["name"],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                PDO::PARAM_STR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            ];</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (array_key_exists("priority", $data)) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            $fields["priority"] = [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                $data["priority"],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                $data["priority"] === null ? PDO::PARAM_NULL : PDO::PARAM_INT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        } </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (array_key_exists("is_completed", $data)) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            $fields["is_completed"] = [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                $data["is_completed"],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                PDO::PARAM_BOOL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        }         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        if (empty($fields)) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            return 0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        } else {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            $sets = array_map(function($value) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                return "$value = :$value";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            }, array_keys($fields));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            $sql = "UPDATE task"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 . " SET " . implode(", ", $sets)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 . " WHERE id = :id";</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            $stmt = $this-&gt;conn-&gt;prepare($sql);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            $stmt-&gt;bindValue(":id", $id, PDO::PARAM_INT);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            foreach ($fields as $name =&gt; $values) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                $stmt-&gt;bindValue(":$name", $values[0], $values[1]);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            $stmt-&gt;execute();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            return $stmt-&gt;rowCount();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    public function update(string $id, array $data)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: int</t>
+    </r>
+  </si>
+  <si>
+    <t>                    $rows = $this-&gt;gateway-&gt;update($id, $data);</t>
+  </si>
+  <si>
+    <t>                    echo json_encode(["message" =&gt; "Task updated", "rows" =&gt; $rows]);</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [0] =&gt; name = :name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [1] =&gt; priority = :priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [2] =&gt; is_completed = :is_completed</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Trường hợp ko có data update được request lên thì return luôn, ko có row nào trong DB được update</t>
+  </si>
+  <si>
+    <t>code khác</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mặc định thì update trả về status code 200 nên ko cần dùng http_response_code() để thay đổi giá trị status </t>
+  </si>
+  <si>
+    <t>Trả về số row trong DB được update, sau khi update rồi mà tiếp tục gửi request 1 lần nữa với cùng 1 data thì</t>
+  </si>
+  <si>
+    <t>cũng sẽ trả về 0</t>
+  </si>
+  <si>
+    <t>Gửi request update data có id là 1</t>
+  </si>
+  <si>
+    <t>Check data được update</t>
   </si>
 </sst>
 </file>
@@ -5688,6 +5875,369 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1999958-AC9A-5158-3A8B-72BD42D538DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1724025" y="18449925"/>
+          <a:ext cx="1009650" cy="27336750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>103835</xdr:colOff>
+      <xdr:row>303</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285438</xdr:colOff>
+      <xdr:row>326</xdr:row>
+      <xdr:rowOff>56602</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D83B31-2270-DAB5-4747-C8281A121680}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="713435" y="57588150"/>
+          <a:ext cx="9935203" cy="4380952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>323</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE301C85-BC7F-2C38-26C2-D757D75B829F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2771775" y="18630900"/>
+          <a:ext cx="600075" cy="42872025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>296</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>324</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Straight Arrow Connector 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23891CAC-B460-33BC-9209-B8CA5AEC9850}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1905000" y="56568975"/>
+          <a:ext cx="66675" cy="5000625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>318</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Arrow Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81CE9CCA-EEE4-B782-C6B5-313EB94CD034}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8458200" y="18659475"/>
+          <a:ext cx="952500" cy="41871900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>327</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>103946</xdr:colOff>
+      <xdr:row>350</xdr:row>
+      <xdr:rowOff>189944</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94E39199-C5C3-51F4-9BD1-C66D48468D69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="790575" y="62226825"/>
+          <a:ext cx="6628571" cy="4447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>313</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>343</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Straight Arrow Connector 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{537A11E4-A6A7-5AF8-EE60-84F592EBA700}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="59702700"/>
+          <a:ext cx="628650" cy="5762625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -29140,8 +29690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805CB3D0-F6EF-4C81-9127-64B24E106742}">
   <dimension ref="A2:R304"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C310" sqref="C310"/>
+    <sheetView topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32795,4 +33345,4382 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B9898AF-4849-4985-8931-E787DD3D8789}">
+  <dimension ref="A2:R352"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A289" workbookViewId="0">
+      <selection activeCell="N345" sqref="N345"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" s="4"/>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" s="4"/>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" s="4"/>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" s="4"/>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="B16" s="4"/>
+      <c r="E16" t="s">
+        <v>11</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="B17" s="4"/>
+      <c r="F17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="B18" s="4"/>
+      <c r="F18" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="B19" s="4"/>
+      <c r="E19" t="s">
+        <v>13</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="B20" s="4"/>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="B21" s="4"/>
+      <c r="F21" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="B22" s="4"/>
+      <c r="F22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="5"/>
+      <c r="K22" t="s">
+        <v>17</v>
+      </c>
+      <c r="L22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="B23" s="4"/>
+      <c r="F23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="5"/>
+      <c r="K23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="B24" s="4"/>
+      <c r="E24" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="B25" s="4"/>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="B26" s="4"/>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="B27" s="4"/>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="B28" s="4"/>
+      <c r="E28" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="B29" s="7"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="9"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" s="4"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="2:9">
+      <c r="B37" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="2:9">
+      <c r="B38" s="4"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43" s="4"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="2:9">
+      <c r="B45" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="2:9">
+      <c r="B46" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="2:9">
+      <c r="B47" s="4"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="2:9">
+      <c r="B48" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="2:9">
+      <c r="B49" s="4"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:9">
+      <c r="B50" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:9">
+      <c r="B51" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="2:9">
+      <c r="B52" s="4"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="2:9">
+      <c r="B53" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="2:9">
+      <c r="B54" s="4"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="2:9">
+      <c r="B55" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="2:9">
+      <c r="B56" s="4"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="2:9">
+      <c r="B57" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="2:9">
+      <c r="B58" s="4"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="2:9">
+      <c r="B59" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="2:9">
+      <c r="B60" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="2:9">
+      <c r="B61" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="2:9">
+      <c r="B62" s="4"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="2:9">
+      <c r="B63" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="2:9">
+      <c r="B64" s="4"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="2:9">
+      <c r="B65" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9">
+      <c r="B66" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:9">
+      <c r="B67" s="4"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:9">
+      <c r="B68" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:9">
+      <c r="B69" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:9">
+      <c r="B70" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9">
+      <c r="B71" s="4"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:9">
+      <c r="B72" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:9">
+      <c r="B73" s="4"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="2:9">
+      <c r="B74" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:9">
+      <c r="B75" s="4"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9">
+      <c r="B76" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="2:9">
+      <c r="B77" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:9">
+      <c r="B78" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="2:9">
+      <c r="B79" s="4"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:9">
+      <c r="B80" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9">
+      <c r="B81" s="4"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9">
+      <c r="B82" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9">
+      <c r="B83" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:9">
+      <c r="B84" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9">
+      <c r="B85" s="4"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9">
+      <c r="B86" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9">
+      <c r="B87" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9">
+      <c r="B88" s="4"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9">
+      <c r="B89" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9">
+      <c r="B90" s="4"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13"/>
+      <c r="H90" s="13"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9">
+      <c r="B91" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="13"/>
+      <c r="G91" s="13"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9">
+      <c r="B92" s="4"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="13"/>
+      <c r="G92" s="13"/>
+      <c r="H92" s="13"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9">
+      <c r="B93" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="13"/>
+      <c r="G93" s="13"/>
+      <c r="H93" s="13"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9">
+      <c r="B94" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="13"/>
+      <c r="G94" s="13"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9">
+      <c r="B95" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="13"/>
+      <c r="H95" s="13"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:9">
+      <c r="B96" s="4"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="13"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:11">
+      <c r="B97" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="13"/>
+      <c r="G97" s="13"/>
+      <c r="H97" s="13"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="2:11">
+      <c r="B98" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="13"/>
+      <c r="G98" s="13"/>
+      <c r="H98" s="13"/>
+      <c r="I98" s="5"/>
+      <c r="J98" t="s">
+        <v>17</v>
+      </c>
+      <c r="K98" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="99" spans="2:11">
+      <c r="B99" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="13"/>
+      <c r="G99" s="13"/>
+      <c r="H99" s="13"/>
+      <c r="I99" s="5"/>
+      <c r="K99" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="100" spans="2:11">
+      <c r="B100" s="4"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="13"/>
+      <c r="G100" s="13"/>
+      <c r="H100" s="13"/>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="2:11">
+      <c r="B101" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="13"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="2:11">
+      <c r="B102" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="13"/>
+      <c r="G102" s="13"/>
+      <c r="H102" s="13"/>
+      <c r="I102" s="5"/>
+    </row>
+    <row r="103" spans="2:11">
+      <c r="B103" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="13"/>
+      <c r="G103" s="13"/>
+      <c r="H103" s="13"/>
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="2:11">
+      <c r="B104" s="4"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="13"/>
+      <c r="G104" s="13"/>
+      <c r="H104" s="13"/>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="2:11">
+      <c r="B105" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C105" s="13"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="13"/>
+      <c r="G105" s="13"/>
+      <c r="H105" s="13"/>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:11">
+      <c r="B106" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C106" s="13"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
+      <c r="F106" s="13"/>
+      <c r="G106" s="13"/>
+      <c r="H106" s="13"/>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="2:11">
+      <c r="B107" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="13"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
+      <c r="I107" s="5"/>
+    </row>
+    <row r="108" spans="2:11">
+      <c r="B108" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="13"/>
+      <c r="G108" s="13"/>
+      <c r="H108" s="13"/>
+      <c r="I108" s="5"/>
+    </row>
+    <row r="109" spans="2:11">
+      <c r="B109" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C109" s="13"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="13"/>
+      <c r="G109" s="13"/>
+      <c r="H109" s="13"/>
+      <c r="I109" s="5"/>
+    </row>
+    <row r="110" spans="2:11">
+      <c r="B110" s="4"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="13"/>
+      <c r="G110" s="13"/>
+      <c r="H110" s="13"/>
+      <c r="I110" s="5"/>
+    </row>
+    <row r="111" spans="2:11">
+      <c r="B111" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="13"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="5"/>
+    </row>
+    <row r="112" spans="2:11">
+      <c r="B112" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="13"/>
+      <c r="G112" s="13"/>
+      <c r="H112" s="13"/>
+      <c r="I112" s="5"/>
+    </row>
+    <row r="113" spans="2:9">
+      <c r="B113" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C113" s="13"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="13"/>
+      <c r="G113" s="13"/>
+      <c r="H113" s="13"/>
+      <c r="I113" s="5"/>
+    </row>
+    <row r="114" spans="2:9">
+      <c r="B114" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C114" s="13"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="13"/>
+      <c r="G114" s="13"/>
+      <c r="H114" s="13"/>
+      <c r="I114" s="5"/>
+    </row>
+    <row r="115" spans="2:9">
+      <c r="B115" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C115" s="13"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="13"/>
+      <c r="G115" s="13"/>
+      <c r="H115" s="13"/>
+      <c r="I115" s="5"/>
+    </row>
+    <row r="116" spans="2:9">
+      <c r="B116" s="4"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
+      <c r="F116" s="13"/>
+      <c r="G116" s="13"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="5"/>
+    </row>
+    <row r="117" spans="2:9">
+      <c r="B117" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C117" s="13"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="13"/>
+      <c r="G117" s="13"/>
+      <c r="H117" s="13"/>
+      <c r="I117" s="5"/>
+    </row>
+    <row r="118" spans="2:9">
+      <c r="B118" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C118" s="13"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="13"/>
+      <c r="G118" s="13"/>
+      <c r="H118" s="13"/>
+      <c r="I118" s="5"/>
+    </row>
+    <row r="119" spans="2:9">
+      <c r="B119" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="13"/>
+      <c r="G119" s="13"/>
+      <c r="H119" s="13"/>
+      <c r="I119" s="5"/>
+    </row>
+    <row r="120" spans="2:9">
+      <c r="B120" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="13"/>
+      <c r="G120" s="13"/>
+      <c r="H120" s="13"/>
+      <c r="I120" s="5"/>
+    </row>
+    <row r="121" spans="2:9">
+      <c r="B121" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
+      <c r="F121" s="13"/>
+      <c r="G121" s="13"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="5"/>
+    </row>
+    <row r="122" spans="2:9">
+      <c r="B122" s="4"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="13"/>
+      <c r="G122" s="13"/>
+      <c r="H122" s="13"/>
+      <c r="I122" s="5"/>
+    </row>
+    <row r="123" spans="2:9">
+      <c r="B123" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C123" s="13"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="13"/>
+      <c r="G123" s="13"/>
+      <c r="H123" s="13"/>
+      <c r="I123" s="5"/>
+    </row>
+    <row r="124" spans="2:9">
+      <c r="B124" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C124" s="13"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
+      <c r="F124" s="13"/>
+      <c r="G124" s="13"/>
+      <c r="H124" s="13"/>
+      <c r="I124" s="5"/>
+    </row>
+    <row r="125" spans="2:9">
+      <c r="B125" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
+      <c r="F125" s="13"/>
+      <c r="G125" s="13"/>
+      <c r="H125" s="13"/>
+      <c r="I125" s="5"/>
+    </row>
+    <row r="126" spans="2:9">
+      <c r="B126" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="13"/>
+      <c r="G126" s="13"/>
+      <c r="H126" s="13"/>
+      <c r="I126" s="5"/>
+    </row>
+    <row r="127" spans="2:9">
+      <c r="B127" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="13"/>
+      <c r="F127" s="13"/>
+      <c r="G127" s="13"/>
+      <c r="H127" s="13"/>
+      <c r="I127" s="5"/>
+    </row>
+    <row r="128" spans="2:9">
+      <c r="B128" s="4"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="13"/>
+      <c r="F128" s="13"/>
+      <c r="G128" s="13"/>
+      <c r="H128" s="13"/>
+      <c r="I128" s="5"/>
+    </row>
+    <row r="129" spans="2:9">
+      <c r="B129" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C129" s="13"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="13"/>
+      <c r="G129" s="13"/>
+      <c r="H129" s="13"/>
+      <c r="I129" s="5"/>
+    </row>
+    <row r="130" spans="2:9">
+      <c r="B130" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="13"/>
+      <c r="F130" s="13"/>
+      <c r="G130" s="13"/>
+      <c r="H130" s="13"/>
+      <c r="I130" s="5"/>
+    </row>
+    <row r="131" spans="2:9">
+      <c r="B131" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="13"/>
+      <c r="G131" s="13"/>
+      <c r="H131" s="13"/>
+      <c r="I131" s="5"/>
+    </row>
+    <row r="132" spans="2:9">
+      <c r="B132" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="13"/>
+      <c r="F132" s="13"/>
+      <c r="G132" s="13"/>
+      <c r="H132" s="13"/>
+      <c r="I132" s="5"/>
+    </row>
+    <row r="133" spans="2:9">
+      <c r="B133" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="13"/>
+      <c r="G133" s="13"/>
+      <c r="H133" s="13"/>
+      <c r="I133" s="5"/>
+    </row>
+    <row r="134" spans="2:9">
+      <c r="B134" s="4"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13"/>
+      <c r="F134" s="13"/>
+      <c r="G134" s="13"/>
+      <c r="H134" s="13"/>
+      <c r="I134" s="5"/>
+    </row>
+    <row r="135" spans="2:9">
+      <c r="B135" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C135" s="13"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="13"/>
+      <c r="F135" s="13"/>
+      <c r="G135" s="13"/>
+      <c r="H135" s="13"/>
+      <c r="I135" s="5"/>
+    </row>
+    <row r="136" spans="2:9">
+      <c r="B136" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C136" s="13"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="13"/>
+      <c r="G136" s="13"/>
+      <c r="H136" s="13"/>
+      <c r="I136" s="5"/>
+    </row>
+    <row r="137" spans="2:9">
+      <c r="B137" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C137" s="13"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
+      <c r="F137" s="13"/>
+      <c r="G137" s="13"/>
+      <c r="H137" s="13"/>
+      <c r="I137" s="5"/>
+    </row>
+    <row r="138" spans="2:9">
+      <c r="B138" s="4"/>
+      <c r="C138" s="13"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="13"/>
+      <c r="G138" s="13"/>
+      <c r="H138" s="13"/>
+      <c r="I138" s="5"/>
+    </row>
+    <row r="139" spans="2:9">
+      <c r="B139" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C139" s="13"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="13"/>
+      <c r="F139" s="13"/>
+      <c r="G139" s="13"/>
+      <c r="H139" s="13"/>
+      <c r="I139" s="5"/>
+    </row>
+    <row r="140" spans="2:9">
+      <c r="B140" s="4"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
+      <c r="F140" s="13"/>
+      <c r="G140" s="13"/>
+      <c r="H140" s="13"/>
+      <c r="I140" s="5"/>
+    </row>
+    <row r="141" spans="2:9">
+      <c r="B141" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C141" s="13"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="13"/>
+      <c r="F141" s="13"/>
+      <c r="G141" s="13"/>
+      <c r="H141" s="13"/>
+      <c r="I141" s="5"/>
+    </row>
+    <row r="142" spans="2:9">
+      <c r="B142" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C142" s="13"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
+      <c r="F142" s="13"/>
+      <c r="G142" s="13"/>
+      <c r="H142" s="13"/>
+      <c r="I142" s="5"/>
+    </row>
+    <row r="143" spans="2:9">
+      <c r="B143" s="4"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
+      <c r="F143" s="13"/>
+      <c r="G143" s="13"/>
+      <c r="H143" s="13"/>
+      <c r="I143" s="5"/>
+    </row>
+    <row r="144" spans="2:9">
+      <c r="B144" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C144" s="13"/>
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
+      <c r="F144" s="13"/>
+      <c r="G144" s="13"/>
+      <c r="H144" s="13"/>
+      <c r="I144" s="5"/>
+    </row>
+    <row r="145" spans="1:9">
+      <c r="B145" s="4"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
+      <c r="F145" s="13"/>
+      <c r="G145" s="13"/>
+      <c r="H145" s="13"/>
+      <c r="I145" s="5"/>
+    </row>
+    <row r="146" spans="1:9">
+      <c r="B146" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C146" s="13"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
+      <c r="F146" s="13"/>
+      <c r="G146" s="13"/>
+      <c r="H146" s="13"/>
+      <c r="I146" s="5"/>
+    </row>
+    <row r="147" spans="1:9">
+      <c r="B147" s="4"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="13"/>
+      <c r="G147" s="13"/>
+      <c r="H147" s="13"/>
+      <c r="I147" s="5"/>
+    </row>
+    <row r="148" spans="1:9">
+      <c r="B148" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C148" s="13"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
+      <c r="F148" s="13"/>
+      <c r="G148" s="13"/>
+      <c r="H148" s="13"/>
+      <c r="I148" s="5"/>
+    </row>
+    <row r="149" spans="1:9">
+      <c r="B149" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C149" s="13"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
+      <c r="F149" s="13"/>
+      <c r="G149" s="13"/>
+      <c r="H149" s="13"/>
+      <c r="I149" s="5"/>
+    </row>
+    <row r="150" spans="1:9">
+      <c r="B150" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C150" s="13"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
+      <c r="F150" s="13"/>
+      <c r="G150" s="13"/>
+      <c r="H150" s="13"/>
+      <c r="I150" s="5"/>
+    </row>
+    <row r="151" spans="1:9">
+      <c r="B151" s="4"/>
+      <c r="C151" s="13"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="13"/>
+      <c r="F151" s="13"/>
+      <c r="G151" s="13"/>
+      <c r="H151" s="13"/>
+      <c r="I151" s="5"/>
+    </row>
+    <row r="152" spans="1:9">
+      <c r="B152" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C152" s="13"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="13"/>
+      <c r="F152" s="13"/>
+      <c r="G152" s="13"/>
+      <c r="H152" s="13"/>
+      <c r="I152" s="5"/>
+    </row>
+    <row r="153" spans="1:9">
+      <c r="B153" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C153" s="13"/>
+      <c r="D153" s="13"/>
+      <c r="E153" s="13"/>
+      <c r="F153" s="13"/>
+      <c r="G153" s="13"/>
+      <c r="H153" s="13"/>
+      <c r="I153" s="5"/>
+    </row>
+    <row r="154" spans="1:9">
+      <c r="B154" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C154" s="8"/>
+      <c r="D154" s="8"/>
+      <c r="E154" s="8"/>
+      <c r="F154" s="8"/>
+      <c r="G154" s="8"/>
+      <c r="H154" s="8"/>
+      <c r="I154" s="9"/>
+    </row>
+    <row r="157" spans="1:9">
+      <c r="A157" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9">
+      <c r="B158" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+      <c r="E158" s="2"/>
+      <c r="F158" s="2"/>
+      <c r="G158" s="2"/>
+      <c r="H158" s="2"/>
+      <c r="I158" s="3"/>
+    </row>
+    <row r="159" spans="1:9">
+      <c r="B159" s="4"/>
+      <c r="C159" s="13"/>
+      <c r="D159" s="13"/>
+      <c r="E159" s="13"/>
+      <c r="F159" s="13"/>
+      <c r="G159" s="13"/>
+      <c r="H159" s="13"/>
+      <c r="I159" s="5"/>
+    </row>
+    <row r="160" spans="1:9">
+      <c r="B160" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C160" s="13"/>
+      <c r="D160" s="13"/>
+      <c r="E160" s="13"/>
+      <c r="F160" s="13"/>
+      <c r="G160" s="13"/>
+      <c r="H160" s="13"/>
+      <c r="I160" s="5"/>
+    </row>
+    <row r="161" spans="2:9">
+      <c r="B161" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C161" s="13"/>
+      <c r="D161" s="13"/>
+      <c r="E161" s="13"/>
+      <c r="F161" s="13"/>
+      <c r="G161" s="13"/>
+      <c r="H161" s="13"/>
+      <c r="I161" s="5"/>
+    </row>
+    <row r="162" spans="2:9">
+      <c r="B162" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C162" s="13"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="13"/>
+      <c r="F162" s="13"/>
+      <c r="G162" s="13"/>
+      <c r="H162" s="13"/>
+      <c r="I162" s="5"/>
+    </row>
+    <row r="163" spans="2:9">
+      <c r="B163" s="4"/>
+      <c r="C163" s="13"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="13"/>
+      <c r="F163" s="13"/>
+      <c r="G163" s="13"/>
+      <c r="H163" s="13"/>
+      <c r="I163" s="5"/>
+    </row>
+    <row r="164" spans="2:9">
+      <c r="B164" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C164" s="13"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="13"/>
+      <c r="F164" s="13"/>
+      <c r="G164" s="13"/>
+      <c r="H164" s="13"/>
+      <c r="I164" s="5"/>
+    </row>
+    <row r="165" spans="2:9">
+      <c r="B165" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C165" s="13"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="13"/>
+      <c r="F165" s="13"/>
+      <c r="G165" s="13"/>
+      <c r="H165" s="13"/>
+      <c r="I165" s="5"/>
+    </row>
+    <row r="166" spans="2:9">
+      <c r="B166" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C166" s="13"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="13"/>
+      <c r="F166" s="13"/>
+      <c r="G166" s="13"/>
+      <c r="H166" s="13"/>
+      <c r="I166" s="5"/>
+    </row>
+    <row r="167" spans="2:9">
+      <c r="B167" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C167" s="13"/>
+      <c r="D167" s="13"/>
+      <c r="E167" s="13"/>
+      <c r="F167" s="13"/>
+      <c r="G167" s="13"/>
+      <c r="H167" s="13"/>
+      <c r="I167" s="5"/>
+    </row>
+    <row r="168" spans="2:9">
+      <c r="B168" s="4"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="13"/>
+      <c r="F168" s="13"/>
+      <c r="G168" s="13"/>
+      <c r="H168" s="13"/>
+      <c r="I168" s="5"/>
+    </row>
+    <row r="169" spans="2:9">
+      <c r="B169" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C169" s="13"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="13"/>
+      <c r="F169" s="13"/>
+      <c r="G169" s="13"/>
+      <c r="H169" s="13"/>
+      <c r="I169" s="5"/>
+    </row>
+    <row r="170" spans="2:9">
+      <c r="B170" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C170" s="13"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="13"/>
+      <c r="F170" s="13"/>
+      <c r="G170" s="13"/>
+      <c r="H170" s="13"/>
+      <c r="I170" s="5"/>
+    </row>
+    <row r="171" spans="2:9">
+      <c r="B171" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C171" s="13"/>
+      <c r="D171" s="13"/>
+      <c r="E171" s="13"/>
+      <c r="F171" s="13"/>
+      <c r="G171" s="13"/>
+      <c r="H171" s="13"/>
+      <c r="I171" s="5"/>
+    </row>
+    <row r="172" spans="2:9">
+      <c r="B172" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C172" s="13"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="13"/>
+      <c r="F172" s="13"/>
+      <c r="G172" s="13"/>
+      <c r="H172" s="13"/>
+      <c r="I172" s="5"/>
+    </row>
+    <row r="173" spans="2:9">
+      <c r="B173" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C173" s="13"/>
+      <c r="D173" s="13"/>
+      <c r="E173" s="13"/>
+      <c r="F173" s="13"/>
+      <c r="G173" s="13"/>
+      <c r="H173" s="13"/>
+      <c r="I173" s="5"/>
+    </row>
+    <row r="174" spans="2:9">
+      <c r="B174" s="4"/>
+      <c r="C174" s="13"/>
+      <c r="D174" s="13"/>
+      <c r="E174" s="13"/>
+      <c r="F174" s="13"/>
+      <c r="G174" s="13"/>
+      <c r="H174" s="13"/>
+      <c r="I174" s="5"/>
+    </row>
+    <row r="175" spans="2:9">
+      <c r="B175" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C175" s="13"/>
+      <c r="D175" s="13"/>
+      <c r="E175" s="13"/>
+      <c r="F175" s="13"/>
+      <c r="G175" s="13"/>
+      <c r="H175" s="13"/>
+      <c r="I175" s="5"/>
+    </row>
+    <row r="176" spans="2:9">
+      <c r="B176" s="4"/>
+      <c r="C176" s="13"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="13"/>
+      <c r="F176" s="13"/>
+      <c r="G176" s="13"/>
+      <c r="H176" s="13"/>
+      <c r="I176" s="5"/>
+    </row>
+    <row r="177" spans="2:9">
+      <c r="B177" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C177" s="13"/>
+      <c r="D177" s="13"/>
+      <c r="E177" s="13"/>
+      <c r="F177" s="13"/>
+      <c r="G177" s="13"/>
+      <c r="H177" s="13"/>
+      <c r="I177" s="5"/>
+    </row>
+    <row r="178" spans="2:9">
+      <c r="B178" s="4"/>
+      <c r="C178" s="13"/>
+      <c r="D178" s="13"/>
+      <c r="E178" s="13"/>
+      <c r="F178" s="13"/>
+      <c r="G178" s="13"/>
+      <c r="H178" s="13"/>
+      <c r="I178" s="5"/>
+    </row>
+    <row r="179" spans="2:9">
+      <c r="B179" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C179" s="13"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13"/>
+      <c r="F179" s="13"/>
+      <c r="G179" s="13"/>
+      <c r="H179" s="13"/>
+      <c r="I179" s="5"/>
+    </row>
+    <row r="180" spans="2:9">
+      <c r="B180" s="4"/>
+      <c r="C180" s="13"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13"/>
+      <c r="F180" s="13"/>
+      <c r="G180" s="13"/>
+      <c r="H180" s="13"/>
+      <c r="I180" s="5"/>
+    </row>
+    <row r="181" spans="2:9">
+      <c r="B181" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C181" s="13"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="13"/>
+      <c r="F181" s="13"/>
+      <c r="G181" s="13"/>
+      <c r="H181" s="13"/>
+      <c r="I181" s="5"/>
+    </row>
+    <row r="182" spans="2:9">
+      <c r="B182" s="4"/>
+      <c r="C182" s="13"/>
+      <c r="D182" s="13"/>
+      <c r="E182" s="13"/>
+      <c r="F182" s="13"/>
+      <c r="G182" s="13"/>
+      <c r="H182" s="13"/>
+      <c r="I182" s="5"/>
+    </row>
+    <row r="183" spans="2:9">
+      <c r="B183" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C183" s="13"/>
+      <c r="D183" s="13"/>
+      <c r="E183" s="13"/>
+      <c r="F183" s="13"/>
+      <c r="G183" s="13"/>
+      <c r="H183" s="13"/>
+      <c r="I183" s="5"/>
+    </row>
+    <row r="184" spans="2:9">
+      <c r="B184" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C184" s="13"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="13"/>
+      <c r="F184" s="13"/>
+      <c r="G184" s="13"/>
+      <c r="H184" s="13"/>
+      <c r="I184" s="5"/>
+    </row>
+    <row r="185" spans="2:9">
+      <c r="B185" s="4"/>
+      <c r="C185" s="13"/>
+      <c r="D185" s="13"/>
+      <c r="E185" s="13"/>
+      <c r="F185" s="13"/>
+      <c r="G185" s="13"/>
+      <c r="H185" s="13"/>
+      <c r="I185" s="5"/>
+    </row>
+    <row r="186" spans="2:9">
+      <c r="B186" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C186" s="13"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="13"/>
+      <c r="F186" s="13"/>
+      <c r="G186" s="13"/>
+      <c r="H186" s="13"/>
+      <c r="I186" s="5"/>
+    </row>
+    <row r="187" spans="2:9">
+      <c r="B187" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C187" s="13"/>
+      <c r="D187" s="13"/>
+      <c r="E187" s="13"/>
+      <c r="F187" s="13"/>
+      <c r="G187" s="13"/>
+      <c r="H187" s="13"/>
+      <c r="I187" s="5"/>
+    </row>
+    <row r="188" spans="2:9">
+      <c r="B188" s="4"/>
+      <c r="C188" s="13"/>
+      <c r="D188" s="13"/>
+      <c r="E188" s="13"/>
+      <c r="F188" s="13"/>
+      <c r="G188" s="13"/>
+      <c r="H188" s="13"/>
+      <c r="I188" s="5"/>
+    </row>
+    <row r="189" spans="2:9">
+      <c r="B189" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C189" s="13"/>
+      <c r="D189" s="13"/>
+      <c r="E189" s="13"/>
+      <c r="F189" s="13"/>
+      <c r="G189" s="13"/>
+      <c r="H189" s="13"/>
+      <c r="I189" s="5"/>
+    </row>
+    <row r="190" spans="2:9">
+      <c r="B190" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C190" s="13"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="13"/>
+      <c r="F190" s="13"/>
+      <c r="G190" s="13"/>
+      <c r="H190" s="13"/>
+      <c r="I190" s="5"/>
+    </row>
+    <row r="191" spans="2:9">
+      <c r="B191" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C191" s="13"/>
+      <c r="D191" s="13"/>
+      <c r="E191" s="13"/>
+      <c r="F191" s="13"/>
+      <c r="G191" s="13"/>
+      <c r="H191" s="13"/>
+      <c r="I191" s="5"/>
+    </row>
+    <row r="192" spans="2:9">
+      <c r="B192" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C192" s="13"/>
+      <c r="D192" s="13"/>
+      <c r="E192" s="13"/>
+      <c r="F192" s="13"/>
+      <c r="G192" s="13"/>
+      <c r="H192" s="13"/>
+      <c r="I192" s="5"/>
+    </row>
+    <row r="193" spans="2:9">
+      <c r="B193" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C193" s="13"/>
+      <c r="D193" s="13"/>
+      <c r="E193" s="13"/>
+      <c r="F193" s="13"/>
+      <c r="G193" s="13"/>
+      <c r="H193" s="13"/>
+      <c r="I193" s="5"/>
+    </row>
+    <row r="194" spans="2:9">
+      <c r="B194" s="4"/>
+      <c r="C194" s="13"/>
+      <c r="D194" s="13"/>
+      <c r="E194" s="13"/>
+      <c r="F194" s="13"/>
+      <c r="G194" s="13"/>
+      <c r="H194" s="13"/>
+      <c r="I194" s="5"/>
+    </row>
+    <row r="195" spans="2:9">
+      <c r="B195" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C195" s="13"/>
+      <c r="D195" s="13"/>
+      <c r="E195" s="13"/>
+      <c r="F195" s="13"/>
+      <c r="G195" s="13"/>
+      <c r="H195" s="13"/>
+      <c r="I195" s="5"/>
+    </row>
+    <row r="196" spans="2:9">
+      <c r="B196" s="4"/>
+      <c r="C196" s="13"/>
+      <c r="D196" s="13"/>
+      <c r="E196" s="13"/>
+      <c r="F196" s="13"/>
+      <c r="G196" s="13"/>
+      <c r="H196" s="13"/>
+      <c r="I196" s="5"/>
+    </row>
+    <row r="197" spans="2:9">
+      <c r="B197" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C197" s="13"/>
+      <c r="D197" s="13"/>
+      <c r="E197" s="13"/>
+      <c r="F197" s="13"/>
+      <c r="G197" s="13"/>
+      <c r="H197" s="13"/>
+      <c r="I197" s="5"/>
+    </row>
+    <row r="198" spans="2:9">
+      <c r="B198" s="4"/>
+      <c r="C198" s="13"/>
+      <c r="D198" s="13"/>
+      <c r="E198" s="13"/>
+      <c r="F198" s="13"/>
+      <c r="G198" s="13"/>
+      <c r="H198" s="13"/>
+      <c r="I198" s="5"/>
+    </row>
+    <row r="199" spans="2:9">
+      <c r="B199" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C199" s="13"/>
+      <c r="D199" s="13"/>
+      <c r="E199" s="13"/>
+      <c r="F199" s="13"/>
+      <c r="G199" s="13"/>
+      <c r="H199" s="13"/>
+      <c r="I199" s="5"/>
+    </row>
+    <row r="200" spans="2:9">
+      <c r="B200" s="4"/>
+      <c r="C200" s="13"/>
+      <c r="D200" s="13"/>
+      <c r="E200" s="13"/>
+      <c r="F200" s="13"/>
+      <c r="G200" s="13"/>
+      <c r="H200" s="13"/>
+      <c r="I200" s="5"/>
+    </row>
+    <row r="201" spans="2:9">
+      <c r="B201" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C201" s="13"/>
+      <c r="D201" s="13"/>
+      <c r="E201" s="13"/>
+      <c r="F201" s="13"/>
+      <c r="G201" s="13"/>
+      <c r="H201" s="13"/>
+      <c r="I201" s="5"/>
+    </row>
+    <row r="202" spans="2:9">
+      <c r="B202" s="4"/>
+      <c r="C202" s="13"/>
+      <c r="D202" s="13"/>
+      <c r="E202" s="13"/>
+      <c r="F202" s="13"/>
+      <c r="G202" s="13"/>
+      <c r="H202" s="13"/>
+      <c r="I202" s="5"/>
+    </row>
+    <row r="203" spans="2:9">
+      <c r="B203" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C203" s="13"/>
+      <c r="D203" s="13"/>
+      <c r="E203" s="13"/>
+      <c r="F203" s="13"/>
+      <c r="G203" s="13"/>
+      <c r="H203" s="13"/>
+      <c r="I203" s="5"/>
+    </row>
+    <row r="204" spans="2:9">
+      <c r="B204" s="4"/>
+      <c r="C204" s="13"/>
+      <c r="D204" s="13"/>
+      <c r="E204" s="13"/>
+      <c r="F204" s="13"/>
+      <c r="G204" s="13"/>
+      <c r="H204" s="13"/>
+      <c r="I204" s="5"/>
+    </row>
+    <row r="205" spans="2:9">
+      <c r="B205" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C205" s="13"/>
+      <c r="D205" s="13"/>
+      <c r="E205" s="13"/>
+      <c r="F205" s="13"/>
+      <c r="G205" s="13"/>
+      <c r="H205" s="13"/>
+      <c r="I205" s="5"/>
+    </row>
+    <row r="206" spans="2:9">
+      <c r="B206" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C206" s="13"/>
+      <c r="D206" s="13"/>
+      <c r="E206" s="13"/>
+      <c r="F206" s="13"/>
+      <c r="G206" s="13"/>
+      <c r="H206" s="13"/>
+      <c r="I206" s="5"/>
+    </row>
+    <row r="207" spans="2:9">
+      <c r="B207" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C207" s="13"/>
+      <c r="D207" s="13"/>
+      <c r="E207" s="13"/>
+      <c r="F207" s="13"/>
+      <c r="G207" s="13"/>
+      <c r="H207" s="13"/>
+      <c r="I207" s="5"/>
+    </row>
+    <row r="208" spans="2:9">
+      <c r="B208" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C208" s="13"/>
+      <c r="D208" s="13"/>
+      <c r="E208" s="13"/>
+      <c r="F208" s="13"/>
+      <c r="G208" s="13"/>
+      <c r="H208" s="13"/>
+      <c r="I208" s="5"/>
+    </row>
+    <row r="209" spans="2:9">
+      <c r="B209" s="4"/>
+      <c r="C209" s="13"/>
+      <c r="D209" s="13"/>
+      <c r="E209" s="13"/>
+      <c r="F209" s="13"/>
+      <c r="G209" s="13"/>
+      <c r="H209" s="13"/>
+      <c r="I209" s="5"/>
+    </row>
+    <row r="210" spans="2:9">
+      <c r="B210" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C210" s="13"/>
+      <c r="D210" s="13"/>
+      <c r="E210" s="13"/>
+      <c r="F210" s="13"/>
+      <c r="G210" s="13"/>
+      <c r="H210" s="13"/>
+      <c r="I210" s="5"/>
+    </row>
+    <row r="211" spans="2:9">
+      <c r="B211" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C211" s="13"/>
+      <c r="D211" s="13"/>
+      <c r="E211" s="13"/>
+      <c r="F211" s="13"/>
+      <c r="G211" s="13"/>
+      <c r="H211" s="13"/>
+      <c r="I211" s="5"/>
+    </row>
+    <row r="212" spans="2:9">
+      <c r="B212" s="4"/>
+      <c r="C212" s="13"/>
+      <c r="D212" s="13"/>
+      <c r="E212" s="13"/>
+      <c r="F212" s="13"/>
+      <c r="G212" s="13"/>
+      <c r="H212" s="13"/>
+      <c r="I212" s="5"/>
+    </row>
+    <row r="213" spans="2:9">
+      <c r="B213" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C213" s="13"/>
+      <c r="D213" s="13"/>
+      <c r="E213" s="13"/>
+      <c r="F213" s="13"/>
+      <c r="G213" s="13"/>
+      <c r="H213" s="13"/>
+      <c r="I213" s="5"/>
+    </row>
+    <row r="214" spans="2:9">
+      <c r="B214" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C214" s="13"/>
+      <c r="D214" s="13"/>
+      <c r="E214" s="13"/>
+      <c r="F214" s="13"/>
+      <c r="G214" s="13"/>
+      <c r="H214" s="13"/>
+      <c r="I214" s="5"/>
+    </row>
+    <row r="215" spans="2:9">
+      <c r="B215" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C215" s="13"/>
+      <c r="D215" s="13"/>
+      <c r="E215" s="13"/>
+      <c r="F215" s="13"/>
+      <c r="G215" s="13"/>
+      <c r="H215" s="13"/>
+      <c r="I215" s="5"/>
+    </row>
+    <row r="216" spans="2:9">
+      <c r="B216" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C216" s="13"/>
+      <c r="D216" s="13"/>
+      <c r="E216" s="13"/>
+      <c r="F216" s="13"/>
+      <c r="G216" s="13"/>
+      <c r="H216" s="13"/>
+      <c r="I216" s="5"/>
+    </row>
+    <row r="217" spans="2:9">
+      <c r="B217" s="4"/>
+      <c r="C217" s="13"/>
+      <c r="D217" s="13"/>
+      <c r="E217" s="13"/>
+      <c r="F217" s="13"/>
+      <c r="G217" s="13"/>
+      <c r="H217" s="13"/>
+      <c r="I217" s="5"/>
+    </row>
+    <row r="218" spans="2:9">
+      <c r="B218" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C218" s="13"/>
+      <c r="D218" s="13"/>
+      <c r="E218" s="13"/>
+      <c r="F218" s="13"/>
+      <c r="G218" s="13"/>
+      <c r="H218" s="13"/>
+      <c r="I218" s="5"/>
+    </row>
+    <row r="219" spans="2:9">
+      <c r="B219" s="4"/>
+      <c r="C219" s="13"/>
+      <c r="D219" s="13"/>
+      <c r="E219" s="13"/>
+      <c r="F219" s="13"/>
+      <c r="G219" s="13"/>
+      <c r="H219" s="13"/>
+      <c r="I219" s="5"/>
+    </row>
+    <row r="220" spans="2:9">
+      <c r="B220" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C220" s="13"/>
+      <c r="D220" s="13"/>
+      <c r="E220" s="13"/>
+      <c r="F220" s="13"/>
+      <c r="G220" s="13"/>
+      <c r="H220" s="13"/>
+      <c r="I220" s="5"/>
+    </row>
+    <row r="221" spans="2:9">
+      <c r="B221" s="4"/>
+      <c r="C221" s="13"/>
+      <c r="D221" s="13"/>
+      <c r="E221" s="13"/>
+      <c r="F221" s="13"/>
+      <c r="G221" s="13"/>
+      <c r="H221" s="13"/>
+      <c r="I221" s="5"/>
+    </row>
+    <row r="222" spans="2:9">
+      <c r="B222" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C222" s="13"/>
+      <c r="D222" s="13"/>
+      <c r="E222" s="13"/>
+      <c r="F222" s="13"/>
+      <c r="G222" s="13"/>
+      <c r="H222" s="13"/>
+      <c r="I222" s="5"/>
+    </row>
+    <row r="223" spans="2:9">
+      <c r="B223" s="4"/>
+      <c r="C223" s="13"/>
+      <c r="D223" s="13"/>
+      <c r="E223" s="13"/>
+      <c r="F223" s="13"/>
+      <c r="G223" s="13"/>
+      <c r="H223" s="13"/>
+      <c r="I223" s="5"/>
+    </row>
+    <row r="224" spans="2:9">
+      <c r="B224" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C224" s="13"/>
+      <c r="D224" s="13"/>
+      <c r="E224" s="13"/>
+      <c r="F224" s="13"/>
+      <c r="G224" s="13"/>
+      <c r="H224" s="13"/>
+      <c r="I224" s="5"/>
+    </row>
+    <row r="225" spans="2:9">
+      <c r="B225" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C225" s="13"/>
+      <c r="D225" s="13"/>
+      <c r="E225" s="13"/>
+      <c r="F225" s="13"/>
+      <c r="G225" s="13"/>
+      <c r="H225" s="13"/>
+      <c r="I225" s="5"/>
+    </row>
+    <row r="226" spans="2:9">
+      <c r="B226" s="4"/>
+      <c r="C226" s="13"/>
+      <c r="D226" s="13"/>
+      <c r="E226" s="13"/>
+      <c r="F226" s="13"/>
+      <c r="G226" s="13"/>
+      <c r="H226" s="13"/>
+      <c r="I226" s="5"/>
+    </row>
+    <row r="227" spans="2:9">
+      <c r="B227" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C227" s="13"/>
+      <c r="D227" s="13"/>
+      <c r="E227" s="13"/>
+      <c r="F227" s="13"/>
+      <c r="G227" s="13"/>
+      <c r="H227" s="13"/>
+      <c r="I227" s="5"/>
+    </row>
+    <row r="228" spans="2:9">
+      <c r="B228" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C228" s="13"/>
+      <c r="D228" s="13"/>
+      <c r="E228" s="13"/>
+      <c r="F228" s="13"/>
+      <c r="G228" s="13"/>
+      <c r="H228" s="13"/>
+      <c r="I228" s="5"/>
+    </row>
+    <row r="229" spans="2:9">
+      <c r="B229" s="4"/>
+      <c r="C229" s="13"/>
+      <c r="D229" s="13"/>
+      <c r="E229" s="13"/>
+      <c r="F229" s="13"/>
+      <c r="G229" s="13"/>
+      <c r="H229" s="13"/>
+      <c r="I229" s="5"/>
+    </row>
+    <row r="230" spans="2:9">
+      <c r="B230" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C230" s="13"/>
+      <c r="D230" s="13"/>
+      <c r="E230" s="13"/>
+      <c r="F230" s="13"/>
+      <c r="G230" s="13"/>
+      <c r="H230" s="13"/>
+      <c r="I230" s="5"/>
+    </row>
+    <row r="231" spans="2:9">
+      <c r="B231" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C231" s="13"/>
+      <c r="D231" s="13"/>
+      <c r="E231" s="13"/>
+      <c r="F231" s="13"/>
+      <c r="G231" s="13"/>
+      <c r="H231" s="13"/>
+      <c r="I231" s="5"/>
+    </row>
+    <row r="232" spans="2:9">
+      <c r="B232" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C232" s="13"/>
+      <c r="D232" s="13"/>
+      <c r="E232" s="13"/>
+      <c r="F232" s="13"/>
+      <c r="G232" s="13"/>
+      <c r="H232" s="13"/>
+      <c r="I232" s="5"/>
+    </row>
+    <row r="233" spans="2:9">
+      <c r="B233" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C233" s="13"/>
+      <c r="D233" s="13"/>
+      <c r="E233" s="13"/>
+      <c r="F233" s="13"/>
+      <c r="G233" s="13"/>
+      <c r="H233" s="13"/>
+      <c r="I233" s="5"/>
+    </row>
+    <row r="234" spans="2:9">
+      <c r="B234" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C234" s="13"/>
+      <c r="D234" s="13"/>
+      <c r="E234" s="13"/>
+      <c r="F234" s="13"/>
+      <c r="G234" s="13"/>
+      <c r="H234" s="13"/>
+      <c r="I234" s="5"/>
+    </row>
+    <row r="235" spans="2:9">
+      <c r="B235" s="4"/>
+      <c r="C235" s="13"/>
+      <c r="D235" s="13"/>
+      <c r="E235" s="13"/>
+      <c r="F235" s="13"/>
+      <c r="G235" s="13"/>
+      <c r="H235" s="13"/>
+      <c r="I235" s="5"/>
+    </row>
+    <row r="236" spans="2:9">
+      <c r="B236" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C236" s="13"/>
+      <c r="D236" s="13"/>
+      <c r="E236" s="13"/>
+      <c r="F236" s="13"/>
+      <c r="G236" s="13"/>
+      <c r="H236" s="13"/>
+      <c r="I236" s="5"/>
+    </row>
+    <row r="237" spans="2:9">
+      <c r="B237" s="4"/>
+      <c r="C237" s="13"/>
+      <c r="D237" s="13"/>
+      <c r="E237" s="13"/>
+      <c r="F237" s="13"/>
+      <c r="G237" s="13"/>
+      <c r="H237" s="13"/>
+      <c r="I237" s="5"/>
+    </row>
+    <row r="238" spans="2:9">
+      <c r="B238" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C238" s="13"/>
+      <c r="D238" s="13"/>
+      <c r="E238" s="13"/>
+      <c r="F238" s="13"/>
+      <c r="G238" s="13"/>
+      <c r="H238" s="13"/>
+      <c r="I238" s="5"/>
+    </row>
+    <row r="239" spans="2:9">
+      <c r="B239" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C239" s="13"/>
+      <c r="D239" s="13"/>
+      <c r="E239" s="13"/>
+      <c r="F239" s="13"/>
+      <c r="G239" s="13"/>
+      <c r="H239" s="13"/>
+      <c r="I239" s="5"/>
+    </row>
+    <row r="240" spans="2:9">
+      <c r="B240" s="4"/>
+      <c r="C240" s="13"/>
+      <c r="D240" s="13"/>
+      <c r="E240" s="13"/>
+      <c r="F240" s="13"/>
+      <c r="G240" s="13"/>
+      <c r="H240" s="13"/>
+      <c r="I240" s="5"/>
+    </row>
+    <row r="241" spans="2:9">
+      <c r="B241" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C241" s="13"/>
+      <c r="D241" s="13"/>
+      <c r="E241" s="13"/>
+      <c r="F241" s="13"/>
+      <c r="G241" s="13"/>
+      <c r="H241" s="13"/>
+      <c r="I241" s="5"/>
+    </row>
+    <row r="242" spans="2:9">
+      <c r="B242" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C242" s="13"/>
+      <c r="D242" s="13"/>
+      <c r="E242" s="13"/>
+      <c r="F242" s="13"/>
+      <c r="G242" s="13"/>
+      <c r="H242" s="13"/>
+      <c r="I242" s="5"/>
+    </row>
+    <row r="243" spans="2:9">
+      <c r="B243" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C243" s="13"/>
+      <c r="D243" s="13"/>
+      <c r="E243" s="13"/>
+      <c r="F243" s="13"/>
+      <c r="G243" s="13"/>
+      <c r="H243" s="13"/>
+      <c r="I243" s="5"/>
+    </row>
+    <row r="244" spans="2:9">
+      <c r="B244" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C244" s="13"/>
+      <c r="D244" s="13"/>
+      <c r="E244" s="13"/>
+      <c r="F244" s="13"/>
+      <c r="G244" s="13"/>
+      <c r="H244" s="13"/>
+      <c r="I244" s="5"/>
+    </row>
+    <row r="245" spans="2:9">
+      <c r="B245" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C245" s="13"/>
+      <c r="D245" s="13"/>
+      <c r="E245" s="13"/>
+      <c r="F245" s="13"/>
+      <c r="G245" s="13"/>
+      <c r="H245" s="13"/>
+      <c r="I245" s="5"/>
+    </row>
+    <row r="246" spans="2:9">
+      <c r="B246" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C246" s="13"/>
+      <c r="D246" s="13"/>
+      <c r="E246" s="13"/>
+      <c r="F246" s="13"/>
+      <c r="G246" s="13"/>
+      <c r="H246" s="13"/>
+      <c r="I246" s="5"/>
+    </row>
+    <row r="247" spans="2:9">
+      <c r="B247" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C247" s="13"/>
+      <c r="D247" s="13"/>
+      <c r="E247" s="13"/>
+      <c r="F247" s="13"/>
+      <c r="G247" s="13"/>
+      <c r="H247" s="13"/>
+      <c r="I247" s="5"/>
+    </row>
+    <row r="248" spans="2:9">
+      <c r="B248" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C248" s="13"/>
+      <c r="D248" s="13"/>
+      <c r="E248" s="13"/>
+      <c r="F248" s="13"/>
+      <c r="G248" s="13"/>
+      <c r="H248" s="13"/>
+      <c r="I248" s="5"/>
+    </row>
+    <row r="249" spans="2:9">
+      <c r="B249" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C249" s="13"/>
+      <c r="D249" s="13"/>
+      <c r="E249" s="13"/>
+      <c r="F249" s="13"/>
+      <c r="G249" s="13"/>
+      <c r="H249" s="13"/>
+      <c r="I249" s="5"/>
+    </row>
+    <row r="250" spans="2:9">
+      <c r="B250" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C250" s="13"/>
+      <c r="D250" s="13"/>
+      <c r="E250" s="13"/>
+      <c r="F250" s="13"/>
+      <c r="G250" s="13"/>
+      <c r="H250" s="13"/>
+      <c r="I250" s="5"/>
+    </row>
+    <row r="251" spans="2:9">
+      <c r="B251" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C251" s="13"/>
+      <c r="D251" s="13"/>
+      <c r="E251" s="13"/>
+      <c r="F251" s="13"/>
+      <c r="G251" s="13"/>
+      <c r="H251" s="13"/>
+      <c r="I251" s="5"/>
+    </row>
+    <row r="252" spans="2:9">
+      <c r="B252" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C252" s="13"/>
+      <c r="D252" s="13"/>
+      <c r="E252" s="13"/>
+      <c r="F252" s="13"/>
+      <c r="G252" s="13"/>
+      <c r="H252" s="13"/>
+      <c r="I252" s="5"/>
+    </row>
+    <row r="253" spans="2:9">
+      <c r="B253" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C253" s="13"/>
+      <c r="D253" s="13"/>
+      <c r="E253" s="13"/>
+      <c r="F253" s="13"/>
+      <c r="G253" s="13"/>
+      <c r="H253" s="13"/>
+      <c r="I253" s="5"/>
+    </row>
+    <row r="254" spans="2:9">
+      <c r="B254" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C254" s="13"/>
+      <c r="D254" s="13"/>
+      <c r="E254" s="13"/>
+      <c r="F254" s="13"/>
+      <c r="G254" s="13"/>
+      <c r="H254" s="13"/>
+      <c r="I254" s="5"/>
+    </row>
+    <row r="255" spans="2:9">
+      <c r="B255" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C255" s="13"/>
+      <c r="D255" s="13"/>
+      <c r="E255" s="13"/>
+      <c r="F255" s="13"/>
+      <c r="G255" s="13"/>
+      <c r="H255" s="13"/>
+      <c r="I255" s="5"/>
+    </row>
+    <row r="256" spans="2:9">
+      <c r="B256" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C256" s="13"/>
+      <c r="D256" s="13"/>
+      <c r="E256" s="13"/>
+      <c r="F256" s="13"/>
+      <c r="G256" s="13"/>
+      <c r="H256" s="13"/>
+      <c r="I256" s="5"/>
+    </row>
+    <row r="257" spans="2:11">
+      <c r="B257" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C257" s="13"/>
+      <c r="D257" s="13"/>
+      <c r="E257" s="13"/>
+      <c r="F257" s="13"/>
+      <c r="G257" s="13"/>
+      <c r="H257" s="13"/>
+      <c r="I257" s="5"/>
+    </row>
+    <row r="258" spans="2:11">
+      <c r="B258" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C258" s="13"/>
+      <c r="D258" s="13"/>
+      <c r="E258" s="13"/>
+      <c r="F258" s="13"/>
+      <c r="G258" s="13"/>
+      <c r="H258" s="13"/>
+      <c r="I258" s="5"/>
+    </row>
+    <row r="259" spans="2:11">
+      <c r="B259" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C259" s="13"/>
+      <c r="D259" s="13"/>
+      <c r="E259" s="13"/>
+      <c r="F259" s="13"/>
+      <c r="G259" s="13"/>
+      <c r="H259" s="13"/>
+      <c r="I259" s="5"/>
+    </row>
+    <row r="260" spans="2:11">
+      <c r="B260" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C260" s="13"/>
+      <c r="D260" s="13"/>
+      <c r="E260" s="13"/>
+      <c r="F260" s="13"/>
+      <c r="G260" s="13"/>
+      <c r="H260" s="13"/>
+      <c r="I260" s="5"/>
+    </row>
+    <row r="261" spans="2:11">
+      <c r="B261" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="C261" s="13"/>
+      <c r="D261" s="13"/>
+      <c r="E261" s="13"/>
+      <c r="F261" s="13"/>
+      <c r="G261" s="13"/>
+      <c r="H261" s="13"/>
+      <c r="I261" s="5"/>
+    </row>
+    <row r="262" spans="2:11">
+      <c r="B262" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C262" s="13"/>
+      <c r="D262" s="13"/>
+      <c r="E262" s="13"/>
+      <c r="F262" s="13"/>
+      <c r="G262" s="13"/>
+      <c r="H262" s="13"/>
+      <c r="I262" s="5"/>
+    </row>
+    <row r="263" spans="2:11">
+      <c r="B263" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C263" s="13"/>
+      <c r="D263" s="13"/>
+      <c r="E263" s="13"/>
+      <c r="F263" s="13"/>
+      <c r="G263" s="13"/>
+      <c r="H263" s="13"/>
+      <c r="I263" s="5"/>
+    </row>
+    <row r="264" spans="2:11">
+      <c r="B264" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C264" s="13"/>
+      <c r="D264" s="13"/>
+      <c r="E264" s="13"/>
+      <c r="F264" s="13"/>
+      <c r="G264" s="13"/>
+      <c r="H264" s="13"/>
+      <c r="I264" s="5"/>
+    </row>
+    <row r="265" spans="2:11">
+      <c r="B265" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C265" s="13"/>
+      <c r="D265" s="13"/>
+      <c r="E265" s="13"/>
+      <c r="F265" s="13"/>
+      <c r="G265" s="13"/>
+      <c r="H265" s="13"/>
+      <c r="I265" s="5"/>
+    </row>
+    <row r="266" spans="2:11">
+      <c r="B266" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C266" s="13"/>
+      <c r="D266" s="13"/>
+      <c r="E266" s="13"/>
+      <c r="F266" s="13"/>
+      <c r="G266" s="13"/>
+      <c r="H266" s="13"/>
+      <c r="I266" s="5"/>
+    </row>
+    <row r="267" spans="2:11">
+      <c r="B267" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C267" s="13"/>
+      <c r="D267" s="13"/>
+      <c r="E267" s="13"/>
+      <c r="F267" s="13"/>
+      <c r="G267" s="13"/>
+      <c r="H267" s="13"/>
+      <c r="I267" s="5"/>
+    </row>
+    <row r="268" spans="2:11">
+      <c r="B268" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C268" s="13"/>
+      <c r="D268" s="13"/>
+      <c r="E268" s="13"/>
+      <c r="F268" s="13"/>
+      <c r="G268" s="13"/>
+      <c r="H268" s="13"/>
+      <c r="I268" s="5"/>
+    </row>
+    <row r="269" spans="2:11">
+      <c r="B269" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="C269" s="13"/>
+      <c r="D269" s="13"/>
+      <c r="E269" s="13"/>
+      <c r="F269" s="13"/>
+      <c r="G269" s="13"/>
+      <c r="H269" s="13"/>
+      <c r="I269" s="5"/>
+    </row>
+    <row r="270" spans="2:11">
+      <c r="B270" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C270" s="13"/>
+      <c r="D270" s="13"/>
+      <c r="E270" s="13"/>
+      <c r="F270" s="13"/>
+      <c r="G270" s="13"/>
+      <c r="H270" s="13"/>
+      <c r="I270" s="5"/>
+    </row>
+    <row r="271" spans="2:11">
+      <c r="B271" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="C271" s="13"/>
+      <c r="D271" s="13"/>
+      <c r="E271" s="13"/>
+      <c r="F271" s="13"/>
+      <c r="G271" s="13"/>
+      <c r="H271" s="13"/>
+      <c r="I271" s="5"/>
+      <c r="J271" t="s">
+        <v>17</v>
+      </c>
+      <c r="K271" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="272" spans="2:11">
+      <c r="B272" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C272" s="13"/>
+      <c r="D272" s="13"/>
+      <c r="E272" s="13"/>
+      <c r="F272" s="13"/>
+      <c r="G272" s="13"/>
+      <c r="H272" s="13"/>
+      <c r="I272" s="5"/>
+    </row>
+    <row r="273" spans="2:15">
+      <c r="B273" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="C273" s="13"/>
+      <c r="D273" s="13"/>
+      <c r="E273" s="13"/>
+      <c r="F273" s="13"/>
+      <c r="G273" s="13"/>
+      <c r="H273" s="13"/>
+      <c r="I273" s="5"/>
+    </row>
+    <row r="274" spans="2:15">
+      <c r="B274" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="C274" s="13"/>
+      <c r="D274" s="13"/>
+      <c r="E274" s="13"/>
+      <c r="F274" s="13"/>
+      <c r="G274" s="13"/>
+      <c r="H274" s="13"/>
+      <c r="I274" s="5"/>
+    </row>
+    <row r="275" spans="2:15">
+      <c r="B275" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="C275" s="13"/>
+      <c r="D275" s="13"/>
+      <c r="E275" s="13"/>
+      <c r="F275" s="13"/>
+      <c r="G275" s="13"/>
+      <c r="H275" s="13"/>
+      <c r="I275" s="5"/>
+      <c r="J275" t="s">
+        <v>17</v>
+      </c>
+      <c r="K275" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="L275" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="M275" s="2"/>
+      <c r="N275" s="2"/>
+      <c r="O275" s="3"/>
+    </row>
+    <row r="276" spans="2:15">
+      <c r="B276" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C276" s="13"/>
+      <c r="D276" s="13"/>
+      <c r="E276" s="13"/>
+      <c r="F276" s="13"/>
+      <c r="G276" s="13"/>
+      <c r="H276" s="13"/>
+      <c r="I276" s="5"/>
+      <c r="K276" s="4"/>
+      <c r="L276" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="M276" s="13"/>
+      <c r="N276" s="13"/>
+      <c r="O276" s="5"/>
+    </row>
+    <row r="277" spans="2:15">
+      <c r="B277" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C277" s="13"/>
+      <c r="D277" s="13"/>
+      <c r="E277" s="13"/>
+      <c r="F277" s="13"/>
+      <c r="G277" s="13"/>
+      <c r="H277" s="13"/>
+      <c r="I277" s="5"/>
+      <c r="K277" s="4"/>
+      <c r="L277" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="M277" s="13"/>
+      <c r="N277" s="13"/>
+      <c r="O277" s="5"/>
+    </row>
+    <row r="278" spans="2:15">
+      <c r="B278" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C278" s="13"/>
+      <c r="D278" s="13"/>
+      <c r="E278" s="13"/>
+      <c r="F278" s="13"/>
+      <c r="G278" s="13"/>
+      <c r="H278" s="13"/>
+      <c r="I278" s="5"/>
+      <c r="K278" s="4"/>
+      <c r="L278" s="13" t="s">
+        <v>330</v>
+      </c>
+      <c r="M278" s="13"/>
+      <c r="N278" s="13"/>
+      <c r="O278" s="5"/>
+    </row>
+    <row r="279" spans="2:15">
+      <c r="B279" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="C279" s="13"/>
+      <c r="D279" s="13"/>
+      <c r="E279" s="13"/>
+      <c r="F279" s="13"/>
+      <c r="G279" s="13"/>
+      <c r="H279" s="13"/>
+      <c r="I279" s="5"/>
+      <c r="K279" s="4"/>
+      <c r="L279" s="13" t="s">
+        <v>331</v>
+      </c>
+      <c r="M279" s="13"/>
+      <c r="N279" s="13"/>
+      <c r="O279" s="5"/>
+    </row>
+    <row r="280" spans="2:15">
+      <c r="B280" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C280" s="13"/>
+      <c r="D280" s="13"/>
+      <c r="E280" s="13"/>
+      <c r="F280" s="13"/>
+      <c r="G280" s="13"/>
+      <c r="H280" s="13"/>
+      <c r="I280" s="5"/>
+      <c r="K280" s="7"/>
+      <c r="L280" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="M280" s="8"/>
+      <c r="N280" s="8"/>
+      <c r="O280" s="9"/>
+    </row>
+    <row r="281" spans="2:15">
+      <c r="B281" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="C281" s="13"/>
+      <c r="D281" s="13"/>
+      <c r="E281" s="13"/>
+      <c r="F281" s="13"/>
+      <c r="G281" s="13"/>
+      <c r="H281" s="13"/>
+      <c r="I281" s="5"/>
+      <c r="J281" t="s">
+        <v>17</v>
+      </c>
+      <c r="K281" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="282" spans="2:15">
+      <c r="B282" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="C282" s="13"/>
+      <c r="D282" s="13"/>
+      <c r="E282" s="13"/>
+      <c r="F282" s="13"/>
+      <c r="G282" s="13"/>
+      <c r="H282" s="13"/>
+      <c r="I282" s="5"/>
+      <c r="K282" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="283" spans="2:15">
+      <c r="B283" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="C283" s="13"/>
+      <c r="D283" s="13"/>
+      <c r="E283" s="13"/>
+      <c r="F283" s="13"/>
+      <c r="G283" s="13"/>
+      <c r="H283" s="13"/>
+      <c r="I283" s="5"/>
+    </row>
+    <row r="284" spans="2:15">
+      <c r="B284" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C284" s="13"/>
+      <c r="D284" s="13"/>
+      <c r="E284" s="13"/>
+      <c r="F284" s="13"/>
+      <c r="G284" s="13"/>
+      <c r="H284" s="13"/>
+      <c r="I284" s="5"/>
+    </row>
+    <row r="285" spans="2:15">
+      <c r="B285" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="C285" s="13"/>
+      <c r="D285" s="13"/>
+      <c r="E285" s="13"/>
+      <c r="F285" s="13"/>
+      <c r="G285" s="13"/>
+      <c r="H285" s="13"/>
+      <c r="I285" s="5"/>
+    </row>
+    <row r="286" spans="2:15">
+      <c r="B286" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C286" s="13"/>
+      <c r="D286" s="13"/>
+      <c r="E286" s="13"/>
+      <c r="F286" s="13"/>
+      <c r="G286" s="13"/>
+      <c r="H286" s="13"/>
+      <c r="I286" s="5"/>
+    </row>
+    <row r="287" spans="2:15">
+      <c r="B287" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="C287" s="13"/>
+      <c r="D287" s="13"/>
+      <c r="E287" s="13"/>
+      <c r="F287" s="13"/>
+      <c r="G287" s="13"/>
+      <c r="H287" s="13"/>
+      <c r="I287" s="5"/>
+    </row>
+    <row r="288" spans="2:15">
+      <c r="B288" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C288" s="13"/>
+      <c r="D288" s="13"/>
+      <c r="E288" s="13"/>
+      <c r="F288" s="13"/>
+      <c r="G288" s="13"/>
+      <c r="H288" s="13"/>
+      <c r="I288" s="5"/>
+    </row>
+    <row r="289" spans="1:18">
+      <c r="B289" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="C289" s="13"/>
+      <c r="D289" s="13"/>
+      <c r="E289" s="13"/>
+      <c r="F289" s="13"/>
+      <c r="G289" s="13"/>
+      <c r="H289" s="13"/>
+      <c r="I289" s="5"/>
+    </row>
+    <row r="290" spans="1:18">
+      <c r="B290" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C290" s="13"/>
+      <c r="D290" s="13"/>
+      <c r="E290" s="13"/>
+      <c r="F290" s="13"/>
+      <c r="G290" s="13"/>
+      <c r="H290" s="13"/>
+      <c r="I290" s="5"/>
+    </row>
+    <row r="291" spans="1:18">
+      <c r="B291" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="C291" s="13"/>
+      <c r="D291" s="13"/>
+      <c r="E291" s="13"/>
+      <c r="F291" s="13"/>
+      <c r="G291" s="13"/>
+      <c r="H291" s="13"/>
+      <c r="I291" s="5"/>
+    </row>
+    <row r="292" spans="1:18">
+      <c r="B292" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C292" s="13"/>
+      <c r="D292" s="13"/>
+      <c r="E292" s="13"/>
+      <c r="F292" s="13"/>
+      <c r="G292" s="13"/>
+      <c r="H292" s="13"/>
+      <c r="I292" s="5"/>
+    </row>
+    <row r="293" spans="1:18">
+      <c r="B293" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="C293" s="13"/>
+      <c r="D293" s="13"/>
+      <c r="E293" s="13"/>
+      <c r="F293" s="13"/>
+      <c r="G293" s="13"/>
+      <c r="H293" s="13"/>
+      <c r="I293" s="5"/>
+    </row>
+    <row r="294" spans="1:18">
+      <c r="B294" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C294" s="13"/>
+      <c r="D294" s="13"/>
+      <c r="E294" s="13"/>
+      <c r="F294" s="13"/>
+      <c r="G294" s="13"/>
+      <c r="H294" s="13"/>
+      <c r="I294" s="5"/>
+    </row>
+    <row r="295" spans="1:18">
+      <c r="B295" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="C295" s="13"/>
+      <c r="D295" s="13"/>
+      <c r="E295" s="13"/>
+      <c r="F295" s="13"/>
+      <c r="G295" s="13"/>
+      <c r="H295" s="13"/>
+      <c r="I295" s="5"/>
+    </row>
+    <row r="296" spans="1:18">
+      <c r="B296" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C296" s="13"/>
+      <c r="D296" s="13"/>
+      <c r="E296" s="13"/>
+      <c r="F296" s="13"/>
+      <c r="G296" s="13"/>
+      <c r="H296" s="13"/>
+      <c r="I296" s="5"/>
+    </row>
+    <row r="297" spans="1:18">
+      <c r="B297" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="C297" s="13"/>
+      <c r="D297" s="13"/>
+      <c r="E297" s="13"/>
+      <c r="F297" s="13"/>
+      <c r="G297" s="13"/>
+      <c r="H297" s="13"/>
+      <c r="I297" s="5"/>
+      <c r="J297" t="s">
+        <v>17</v>
+      </c>
+      <c r="K297" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="298" spans="1:18">
+      <c r="B298" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C298" s="13"/>
+      <c r="D298" s="13"/>
+      <c r="E298" s="13"/>
+      <c r="F298" s="13"/>
+      <c r="G298" s="13"/>
+      <c r="H298" s="13"/>
+      <c r="I298" s="5"/>
+      <c r="K298" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="299" spans="1:18">
+      <c r="B299" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="C299" s="8"/>
+      <c r="D299" s="8"/>
+      <c r="E299" s="8"/>
+      <c r="F299" s="8"/>
+      <c r="G299" s="8"/>
+      <c r="H299" s="8"/>
+      <c r="I299" s="9"/>
+    </row>
+    <row r="302" spans="1:18">
+      <c r="A302" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B302" s="2"/>
+      <c r="C302" s="2"/>
+      <c r="D302" s="2"/>
+      <c r="E302" s="2"/>
+      <c r="F302" s="2"/>
+      <c r="G302" s="2"/>
+      <c r="H302" s="2"/>
+      <c r="I302" s="2"/>
+      <c r="J302" s="2"/>
+      <c r="K302" s="2"/>
+      <c r="L302" s="2"/>
+      <c r="M302" s="2"/>
+      <c r="N302" s="2"/>
+      <c r="O302" s="2"/>
+      <c r="P302" s="2"/>
+      <c r="Q302" s="2"/>
+      <c r="R302" s="3"/>
+    </row>
+    <row r="303" spans="1:18">
+      <c r="A303" s="4"/>
+      <c r="B303" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="C303" s="13"/>
+      <c r="D303" s="13"/>
+      <c r="E303" s="13"/>
+      <c r="F303" s="13"/>
+      <c r="G303" s="13"/>
+      <c r="H303" s="13"/>
+      <c r="I303" s="13"/>
+      <c r="J303" s="13"/>
+      <c r="K303" s="13"/>
+      <c r="L303" s="13"/>
+      <c r="M303" s="13"/>
+      <c r="N303" s="13"/>
+      <c r="O303" s="13"/>
+      <c r="P303" s="13"/>
+      <c r="Q303" s="13"/>
+      <c r="R303" s="5"/>
+    </row>
+    <row r="304" spans="1:18">
+      <c r="A304" s="4"/>
+      <c r="B304" s="13"/>
+      <c r="C304" s="13"/>
+      <c r="D304" s="13"/>
+      <c r="E304" s="13"/>
+      <c r="F304" s="13"/>
+      <c r="G304" s="13"/>
+      <c r="H304" s="13"/>
+      <c r="I304" s="13"/>
+      <c r="J304" s="13"/>
+      <c r="K304" s="13"/>
+      <c r="L304" s="13"/>
+      <c r="M304" s="13"/>
+      <c r="N304" s="13"/>
+      <c r="O304" s="13"/>
+      <c r="P304" s="13"/>
+      <c r="Q304" s="13"/>
+      <c r="R304" s="5"/>
+    </row>
+    <row r="305" spans="1:18">
+      <c r="A305" s="4"/>
+      <c r="B305" s="13"/>
+      <c r="C305" s="13"/>
+      <c r="D305" s="13"/>
+      <c r="E305" s="13"/>
+      <c r="F305" s="13"/>
+      <c r="G305" s="13"/>
+      <c r="H305" s="13"/>
+      <c r="I305" s="13"/>
+      <c r="J305" s="13"/>
+      <c r="K305" s="13"/>
+      <c r="L305" s="13"/>
+      <c r="M305" s="13"/>
+      <c r="N305" s="13"/>
+      <c r="O305" s="13"/>
+      <c r="P305" s="13"/>
+      <c r="Q305" s="13"/>
+      <c r="R305" s="5"/>
+    </row>
+    <row r="306" spans="1:18">
+      <c r="A306" s="4"/>
+      <c r="B306" s="13"/>
+      <c r="C306" s="13"/>
+      <c r="D306" s="13"/>
+      <c r="E306" s="13"/>
+      <c r="F306" s="13"/>
+      <c r="G306" s="13"/>
+      <c r="H306" s="13"/>
+      <c r="I306" s="13"/>
+      <c r="J306" s="13"/>
+      <c r="K306" s="13"/>
+      <c r="L306" s="13"/>
+      <c r="M306" s="13"/>
+      <c r="N306" s="13"/>
+      <c r="O306" s="13"/>
+      <c r="P306" s="13"/>
+      <c r="Q306" s="13"/>
+      <c r="R306" s="5"/>
+    </row>
+    <row r="307" spans="1:18">
+      <c r="A307" s="4"/>
+      <c r="B307" s="13"/>
+      <c r="C307" s="13"/>
+      <c r="D307" s="13"/>
+      <c r="E307" s="13"/>
+      <c r="F307" s="13"/>
+      <c r="G307" s="13"/>
+      <c r="H307" s="13"/>
+      <c r="I307" s="13"/>
+      <c r="J307" s="13"/>
+      <c r="K307" s="13"/>
+      <c r="L307" s="13"/>
+      <c r="M307" s="13"/>
+      <c r="N307" s="13"/>
+      <c r="O307" s="13"/>
+      <c r="P307" s="13"/>
+      <c r="Q307" s="13"/>
+      <c r="R307" s="5"/>
+    </row>
+    <row r="308" spans="1:18">
+      <c r="A308" s="4"/>
+      <c r="B308" s="13"/>
+      <c r="C308" s="13"/>
+      <c r="D308" s="13"/>
+      <c r="E308" s="13"/>
+      <c r="F308" s="13"/>
+      <c r="G308" s="13"/>
+      <c r="H308" s="13"/>
+      <c r="I308" s="13"/>
+      <c r="J308" s="13"/>
+      <c r="K308" s="13"/>
+      <c r="L308" s="13"/>
+      <c r="M308" s="13"/>
+      <c r="N308" s="13"/>
+      <c r="O308" s="13"/>
+      <c r="P308" s="13"/>
+      <c r="Q308" s="13"/>
+      <c r="R308" s="5"/>
+    </row>
+    <row r="309" spans="1:18">
+      <c r="A309" s="4"/>
+      <c r="B309" s="13"/>
+      <c r="C309" s="13"/>
+      <c r="D309" s="13"/>
+      <c r="E309" s="13"/>
+      <c r="F309" s="13"/>
+      <c r="G309" s="13"/>
+      <c r="H309" s="13"/>
+      <c r="I309" s="13"/>
+      <c r="J309" s="13"/>
+      <c r="K309" s="13"/>
+      <c r="L309" s="13"/>
+      <c r="M309" s="13"/>
+      <c r="N309" s="13"/>
+      <c r="O309" s="13"/>
+      <c r="P309" s="13"/>
+      <c r="Q309" s="13"/>
+      <c r="R309" s="5"/>
+    </row>
+    <row r="310" spans="1:18">
+      <c r="A310" s="4"/>
+      <c r="B310" s="13"/>
+      <c r="C310" s="13"/>
+      <c r="D310" s="13"/>
+      <c r="E310" s="13"/>
+      <c r="F310" s="13"/>
+      <c r="G310" s="13"/>
+      <c r="H310" s="13"/>
+      <c r="I310" s="13"/>
+      <c r="J310" s="13"/>
+      <c r="K310" s="13"/>
+      <c r="L310" s="13"/>
+      <c r="M310" s="13"/>
+      <c r="N310" s="13"/>
+      <c r="O310" s="13"/>
+      <c r="P310" s="13"/>
+      <c r="Q310" s="13"/>
+      <c r="R310" s="5"/>
+    </row>
+    <row r="311" spans="1:18">
+      <c r="A311" s="4"/>
+      <c r="B311" s="13"/>
+      <c r="C311" s="13"/>
+      <c r="D311" s="13"/>
+      <c r="E311" s="13"/>
+      <c r="F311" s="13"/>
+      <c r="G311" s="13"/>
+      <c r="H311" s="13"/>
+      <c r="I311" s="13"/>
+      <c r="J311" s="13"/>
+      <c r="K311" s="13"/>
+      <c r="L311" s="13"/>
+      <c r="M311" s="13"/>
+      <c r="N311" s="13"/>
+      <c r="O311" s="13"/>
+      <c r="P311" s="13"/>
+      <c r="Q311" s="13"/>
+      <c r="R311" s="5"/>
+    </row>
+    <row r="312" spans="1:18">
+      <c r="A312" s="4"/>
+      <c r="B312" s="13"/>
+      <c r="C312" s="13"/>
+      <c r="D312" s="13"/>
+      <c r="E312" s="13"/>
+      <c r="F312" s="13"/>
+      <c r="G312" s="13"/>
+      <c r="H312" s="13"/>
+      <c r="I312" s="13"/>
+      <c r="J312" s="13"/>
+      <c r="K312" s="13"/>
+      <c r="L312" s="13"/>
+      <c r="M312" s="13"/>
+      <c r="N312" s="13"/>
+      <c r="O312" s="13"/>
+      <c r="P312" s="13"/>
+      <c r="Q312" s="13"/>
+      <c r="R312" s="5"/>
+    </row>
+    <row r="313" spans="1:18">
+      <c r="A313" s="4"/>
+      <c r="B313" s="13"/>
+      <c r="C313" s="13"/>
+      <c r="D313" s="13"/>
+      <c r="E313" s="13"/>
+      <c r="F313" s="13"/>
+      <c r="G313" s="13"/>
+      <c r="H313" s="13"/>
+      <c r="I313" s="13"/>
+      <c r="J313" s="13"/>
+      <c r="K313" s="13"/>
+      <c r="L313" s="13"/>
+      <c r="M313" s="13"/>
+      <c r="N313" s="13"/>
+      <c r="O313" s="13"/>
+      <c r="P313" s="13"/>
+      <c r="Q313" s="13"/>
+      <c r="R313" s="5"/>
+    </row>
+    <row r="314" spans="1:18">
+      <c r="A314" s="4"/>
+      <c r="B314" s="13"/>
+      <c r="C314" s="13"/>
+      <c r="D314" s="13"/>
+      <c r="E314" s="13"/>
+      <c r="F314" s="13"/>
+      <c r="G314" s="13"/>
+      <c r="H314" s="13"/>
+      <c r="I314" s="13"/>
+      <c r="J314" s="13"/>
+      <c r="K314" s="13"/>
+      <c r="L314" s="13"/>
+      <c r="M314" s="13"/>
+      <c r="N314" s="13"/>
+      <c r="O314" s="13"/>
+      <c r="P314" s="13"/>
+      <c r="Q314" s="13"/>
+      <c r="R314" s="5"/>
+    </row>
+    <row r="315" spans="1:18">
+      <c r="A315" s="4"/>
+      <c r="B315" s="13"/>
+      <c r="C315" s="13"/>
+      <c r="D315" s="13"/>
+      <c r="E315" s="13"/>
+      <c r="F315" s="13"/>
+      <c r="G315" s="13"/>
+      <c r="H315" s="13"/>
+      <c r="I315" s="13"/>
+      <c r="J315" s="13"/>
+      <c r="K315" s="13"/>
+      <c r="L315" s="13"/>
+      <c r="M315" s="13"/>
+      <c r="N315" s="13"/>
+      <c r="O315" s="13"/>
+      <c r="P315" s="13"/>
+      <c r="Q315" s="13"/>
+      <c r="R315" s="5"/>
+    </row>
+    <row r="316" spans="1:18">
+      <c r="A316" s="4"/>
+      <c r="B316" s="13"/>
+      <c r="C316" s="13"/>
+      <c r="D316" s="13"/>
+      <c r="E316" s="13"/>
+      <c r="F316" s="13"/>
+      <c r="G316" s="13"/>
+      <c r="H316" s="13"/>
+      <c r="I316" s="13"/>
+      <c r="J316" s="13"/>
+      <c r="K316" s="13"/>
+      <c r="L316" s="13"/>
+      <c r="M316" s="13"/>
+      <c r="N316" s="13"/>
+      <c r="O316" s="13"/>
+      <c r="P316" s="13"/>
+      <c r="Q316" s="13"/>
+      <c r="R316" s="5"/>
+    </row>
+    <row r="317" spans="1:18">
+      <c r="A317" s="4"/>
+      <c r="B317" s="13"/>
+      <c r="C317" s="13"/>
+      <c r="D317" s="13"/>
+      <c r="E317" s="13"/>
+      <c r="F317" s="13"/>
+      <c r="G317" s="13"/>
+      <c r="H317" s="13"/>
+      <c r="I317" s="13"/>
+      <c r="J317" s="13"/>
+      <c r="K317" s="13"/>
+      <c r="L317" s="13"/>
+      <c r="M317" s="13"/>
+      <c r="N317" s="13"/>
+      <c r="O317" s="13"/>
+      <c r="P317" s="13"/>
+      <c r="Q317" s="13"/>
+      <c r="R317" s="5"/>
+    </row>
+    <row r="318" spans="1:18">
+      <c r="A318" s="4"/>
+      <c r="B318" s="13"/>
+      <c r="C318" s="13"/>
+      <c r="D318" s="13"/>
+      <c r="E318" s="13"/>
+      <c r="F318" s="13"/>
+      <c r="G318" s="13"/>
+      <c r="H318" s="13"/>
+      <c r="I318" s="13"/>
+      <c r="J318" s="13"/>
+      <c r="K318" s="13"/>
+      <c r="L318" s="13"/>
+      <c r="M318" s="13"/>
+      <c r="N318" s="13"/>
+      <c r="O318" s="13"/>
+      <c r="P318" s="13"/>
+      <c r="Q318" s="13"/>
+      <c r="R318" s="5"/>
+    </row>
+    <row r="319" spans="1:18">
+      <c r="A319" s="4"/>
+      <c r="B319" s="13"/>
+      <c r="C319" s="13"/>
+      <c r="D319" s="13"/>
+      <c r="E319" s="13"/>
+      <c r="F319" s="13"/>
+      <c r="G319" s="13"/>
+      <c r="H319" s="13"/>
+      <c r="I319" s="13"/>
+      <c r="J319" s="13"/>
+      <c r="K319" s="13"/>
+      <c r="L319" s="13"/>
+      <c r="M319" s="13"/>
+      <c r="N319" s="13"/>
+      <c r="O319" s="13"/>
+      <c r="P319" s="13"/>
+      <c r="Q319" s="13"/>
+      <c r="R319" s="5"/>
+    </row>
+    <row r="320" spans="1:18">
+      <c r="A320" s="4"/>
+      <c r="B320" s="13"/>
+      <c r="C320" s="13"/>
+      <c r="D320" s="13"/>
+      <c r="E320" s="13"/>
+      <c r="F320" s="13"/>
+      <c r="G320" s="13"/>
+      <c r="H320" s="13"/>
+      <c r="I320" s="13"/>
+      <c r="J320" s="13"/>
+      <c r="K320" s="13"/>
+      <c r="L320" s="13"/>
+      <c r="M320" s="13"/>
+      <c r="N320" s="13"/>
+      <c r="O320" s="13"/>
+      <c r="P320" s="13"/>
+      <c r="Q320" s="13"/>
+      <c r="R320" s="5"/>
+    </row>
+    <row r="321" spans="1:18">
+      <c r="A321" s="4"/>
+      <c r="B321" s="13"/>
+      <c r="C321" s="13"/>
+      <c r="D321" s="13"/>
+      <c r="E321" s="13"/>
+      <c r="F321" s="13"/>
+      <c r="G321" s="13"/>
+      <c r="H321" s="13"/>
+      <c r="I321" s="13"/>
+      <c r="J321" s="13"/>
+      <c r="K321" s="13"/>
+      <c r="L321" s="13"/>
+      <c r="M321" s="13"/>
+      <c r="N321" s="13"/>
+      <c r="O321" s="13"/>
+      <c r="P321" s="13"/>
+      <c r="Q321" s="13"/>
+      <c r="R321" s="5"/>
+    </row>
+    <row r="322" spans="1:18">
+      <c r="A322" s="4"/>
+      <c r="B322" s="13"/>
+      <c r="C322" s="13"/>
+      <c r="D322" s="13"/>
+      <c r="E322" s="13"/>
+      <c r="F322" s="13"/>
+      <c r="G322" s="13"/>
+      <c r="H322" s="13"/>
+      <c r="I322" s="13"/>
+      <c r="J322" s="13"/>
+      <c r="K322" s="13"/>
+      <c r="L322" s="13"/>
+      <c r="M322" s="13"/>
+      <c r="N322" s="13"/>
+      <c r="O322" s="13"/>
+      <c r="P322" s="13"/>
+      <c r="Q322" s="13"/>
+      <c r="R322" s="5"/>
+    </row>
+    <row r="323" spans="1:18">
+      <c r="A323" s="4"/>
+      <c r="B323" s="13"/>
+      <c r="C323" s="13"/>
+      <c r="D323" s="13"/>
+      <c r="E323" s="13"/>
+      <c r="F323" s="13"/>
+      <c r="G323" s="13"/>
+      <c r="H323" s="13"/>
+      <c r="I323" s="13"/>
+      <c r="J323" s="13"/>
+      <c r="K323" s="13"/>
+      <c r="L323" s="13"/>
+      <c r="M323" s="13"/>
+      <c r="N323" s="13"/>
+      <c r="O323" s="13"/>
+      <c r="P323" s="13"/>
+      <c r="Q323" s="13"/>
+      <c r="R323" s="5"/>
+    </row>
+    <row r="324" spans="1:18">
+      <c r="A324" s="4"/>
+      <c r="B324" s="13"/>
+      <c r="C324" s="13"/>
+      <c r="D324" s="13"/>
+      <c r="E324" s="13"/>
+      <c r="F324" s="13"/>
+      <c r="G324" s="13"/>
+      <c r="H324" s="13"/>
+      <c r="I324" s="13"/>
+      <c r="J324" s="13"/>
+      <c r="K324" s="13"/>
+      <c r="L324" s="13"/>
+      <c r="M324" s="13"/>
+      <c r="N324" s="13"/>
+      <c r="O324" s="13"/>
+      <c r="P324" s="13"/>
+      <c r="Q324" s="13"/>
+      <c r="R324" s="5"/>
+    </row>
+    <row r="325" spans="1:18">
+      <c r="A325" s="4"/>
+      <c r="B325" s="13"/>
+      <c r="C325" s="13"/>
+      <c r="D325" s="13"/>
+      <c r="E325" s="13"/>
+      <c r="F325" s="13"/>
+      <c r="G325" s="13"/>
+      <c r="H325" s="13"/>
+      <c r="I325" s="13"/>
+      <c r="J325" s="13"/>
+      <c r="K325" s="13"/>
+      <c r="L325" s="13"/>
+      <c r="M325" s="13"/>
+      <c r="N325" s="13"/>
+      <c r="O325" s="13"/>
+      <c r="P325" s="13"/>
+      <c r="Q325" s="13"/>
+      <c r="R325" s="5"/>
+    </row>
+    <row r="326" spans="1:18">
+      <c r="A326" s="4"/>
+      <c r="B326" s="13"/>
+      <c r="C326" s="13"/>
+      <c r="D326" s="13"/>
+      <c r="E326" s="13"/>
+      <c r="F326" s="13"/>
+      <c r="G326" s="13"/>
+      <c r="H326" s="13"/>
+      <c r="I326" s="13"/>
+      <c r="J326" s="13"/>
+      <c r="K326" s="13"/>
+      <c r="L326" s="13"/>
+      <c r="M326" s="13"/>
+      <c r="N326" s="13"/>
+      <c r="O326" s="13"/>
+      <c r="P326" s="13"/>
+      <c r="Q326" s="13"/>
+      <c r="R326" s="5"/>
+    </row>
+    <row r="327" spans="1:18">
+      <c r="A327" s="4"/>
+      <c r="B327" s="13"/>
+      <c r="C327" s="13"/>
+      <c r="D327" s="13"/>
+      <c r="E327" s="13"/>
+      <c r="F327" s="13"/>
+      <c r="G327" s="13"/>
+      <c r="H327" s="13"/>
+      <c r="I327" s="13"/>
+      <c r="J327" s="13"/>
+      <c r="K327" s="13"/>
+      <c r="L327" s="13"/>
+      <c r="M327" s="13"/>
+      <c r="N327" s="13"/>
+      <c r="O327" s="13"/>
+      <c r="P327" s="13"/>
+      <c r="Q327" s="13"/>
+      <c r="R327" s="5"/>
+    </row>
+    <row r="328" spans="1:18">
+      <c r="A328" s="4"/>
+      <c r="B328" s="13"/>
+      <c r="C328" s="13"/>
+      <c r="D328" s="13"/>
+      <c r="E328" s="13"/>
+      <c r="F328" s="13"/>
+      <c r="G328" s="13"/>
+      <c r="H328" s="13"/>
+      <c r="I328" s="13"/>
+      <c r="J328" s="13"/>
+      <c r="K328" s="13"/>
+      <c r="L328" s="13"/>
+      <c r="M328" s="13"/>
+      <c r="N328" s="13"/>
+      <c r="O328" s="13"/>
+      <c r="P328" s="13"/>
+      <c r="Q328" s="13"/>
+      <c r="R328" s="5"/>
+    </row>
+    <row r="329" spans="1:18">
+      <c r="A329" s="4"/>
+      <c r="B329" s="13"/>
+      <c r="C329" s="13"/>
+      <c r="D329" s="13"/>
+      <c r="E329" s="13"/>
+      <c r="F329" s="13"/>
+      <c r="G329" s="13"/>
+      <c r="H329" s="13"/>
+      <c r="I329" s="13"/>
+      <c r="J329" s="13"/>
+      <c r="K329" s="13"/>
+      <c r="L329" s="13"/>
+      <c r="M329" s="13"/>
+      <c r="N329" s="13"/>
+      <c r="O329" s="13"/>
+      <c r="P329" s="13"/>
+      <c r="Q329" s="13"/>
+      <c r="R329" s="5"/>
+    </row>
+    <row r="330" spans="1:18">
+      <c r="A330" s="4"/>
+      <c r="B330" s="13"/>
+      <c r="C330" s="13"/>
+      <c r="D330" s="13"/>
+      <c r="E330" s="13"/>
+      <c r="F330" s="13"/>
+      <c r="G330" s="13"/>
+      <c r="H330" s="13"/>
+      <c r="I330" s="13"/>
+      <c r="J330" s="13"/>
+      <c r="K330" s="13"/>
+      <c r="L330" s="13"/>
+      <c r="M330" s="13"/>
+      <c r="N330" s="13"/>
+      <c r="O330" s="13"/>
+      <c r="P330" s="13"/>
+      <c r="Q330" s="13"/>
+      <c r="R330" s="5"/>
+    </row>
+    <row r="331" spans="1:18">
+      <c r="A331" s="4"/>
+      <c r="B331" s="13"/>
+      <c r="C331" s="13"/>
+      <c r="D331" s="13"/>
+      <c r="E331" s="13"/>
+      <c r="F331" s="13"/>
+      <c r="G331" s="13"/>
+      <c r="H331" s="13"/>
+      <c r="I331" s="13"/>
+      <c r="J331" s="13"/>
+      <c r="K331" s="13"/>
+      <c r="L331" s="13"/>
+      <c r="M331" s="13"/>
+      <c r="N331" s="13"/>
+      <c r="O331" s="13"/>
+      <c r="P331" s="13"/>
+      <c r="Q331" s="13"/>
+      <c r="R331" s="5"/>
+    </row>
+    <row r="332" spans="1:18">
+      <c r="A332" s="4"/>
+      <c r="B332" s="13"/>
+      <c r="C332" s="13"/>
+      <c r="D332" s="13"/>
+      <c r="E332" s="13"/>
+      <c r="F332" s="13"/>
+      <c r="G332" s="13"/>
+      <c r="H332" s="13"/>
+      <c r="I332" s="13"/>
+      <c r="J332" s="13"/>
+      <c r="K332" s="13"/>
+      <c r="L332" s="13"/>
+      <c r="M332" s="13"/>
+      <c r="N332" s="13"/>
+      <c r="O332" s="13"/>
+      <c r="P332" s="13"/>
+      <c r="Q332" s="13"/>
+      <c r="R332" s="5"/>
+    </row>
+    <row r="333" spans="1:18">
+      <c r="A333" s="4"/>
+      <c r="B333" s="13"/>
+      <c r="C333" s="13"/>
+      <c r="D333" s="13"/>
+      <c r="E333" s="13"/>
+      <c r="F333" s="13"/>
+      <c r="G333" s="13"/>
+      <c r="H333" s="13"/>
+      <c r="I333" s="13"/>
+      <c r="J333" s="13"/>
+      <c r="K333" s="13"/>
+      <c r="L333" s="13"/>
+      <c r="M333" s="13"/>
+      <c r="N333" s="13"/>
+      <c r="O333" s="13"/>
+      <c r="P333" s="13"/>
+      <c r="Q333" s="13"/>
+      <c r="R333" s="5"/>
+    </row>
+    <row r="334" spans="1:18">
+      <c r="A334" s="4"/>
+      <c r="B334" s="13"/>
+      <c r="C334" s="13"/>
+      <c r="D334" s="13"/>
+      <c r="E334" s="13"/>
+      <c r="F334" s="13"/>
+      <c r="G334" s="13"/>
+      <c r="H334" s="13"/>
+      <c r="I334" s="13"/>
+      <c r="J334" s="13"/>
+      <c r="K334" s="13"/>
+      <c r="L334" s="13"/>
+      <c r="M334" s="13"/>
+      <c r="N334" s="13"/>
+      <c r="O334" s="13"/>
+      <c r="P334" s="13"/>
+      <c r="Q334" s="13"/>
+      <c r="R334" s="5"/>
+    </row>
+    <row r="335" spans="1:18">
+      <c r="A335" s="4"/>
+      <c r="B335" s="13"/>
+      <c r="C335" s="13"/>
+      <c r="D335" s="13"/>
+      <c r="E335" s="13"/>
+      <c r="F335" s="13"/>
+      <c r="G335" s="13"/>
+      <c r="H335" s="13"/>
+      <c r="I335" s="13"/>
+      <c r="J335" s="13"/>
+      <c r="K335" s="13"/>
+      <c r="L335" s="13"/>
+      <c r="M335" s="13"/>
+      <c r="N335" s="13"/>
+      <c r="O335" s="13"/>
+      <c r="P335" s="13"/>
+      <c r="Q335" s="13"/>
+      <c r="R335" s="5"/>
+    </row>
+    <row r="336" spans="1:18">
+      <c r="A336" s="4"/>
+      <c r="B336" s="13"/>
+      <c r="C336" s="13"/>
+      <c r="D336" s="13"/>
+      <c r="E336" s="13"/>
+      <c r="F336" s="13"/>
+      <c r="G336" s="13"/>
+      <c r="H336" s="13"/>
+      <c r="I336" s="13"/>
+      <c r="J336" s="13"/>
+      <c r="K336" s="13"/>
+      <c r="L336" s="13"/>
+      <c r="M336" s="13"/>
+      <c r="N336" s="13"/>
+      <c r="O336" s="13"/>
+      <c r="P336" s="13"/>
+      <c r="Q336" s="13"/>
+      <c r="R336" s="5"/>
+    </row>
+    <row r="337" spans="1:18">
+      <c r="A337" s="4"/>
+      <c r="B337" s="13"/>
+      <c r="C337" s="13"/>
+      <c r="D337" s="13"/>
+      <c r="E337" s="13"/>
+      <c r="F337" s="13"/>
+      <c r="G337" s="13"/>
+      <c r="H337" s="13"/>
+      <c r="I337" s="13"/>
+      <c r="J337" s="13"/>
+      <c r="K337" s="13"/>
+      <c r="L337" s="13"/>
+      <c r="M337" s="13"/>
+      <c r="N337" s="13"/>
+      <c r="O337" s="13"/>
+      <c r="P337" s="13"/>
+      <c r="Q337" s="13"/>
+      <c r="R337" s="5"/>
+    </row>
+    <row r="338" spans="1:18">
+      <c r="A338" s="4"/>
+      <c r="B338" s="13"/>
+      <c r="C338" s="13"/>
+      <c r="D338" s="13"/>
+      <c r="E338" s="13"/>
+      <c r="F338" s="13"/>
+      <c r="G338" s="13"/>
+      <c r="H338" s="13"/>
+      <c r="I338" s="13"/>
+      <c r="J338" s="13"/>
+      <c r="K338" s="13"/>
+      <c r="L338" s="13"/>
+      <c r="M338" s="13"/>
+      <c r="N338" s="13"/>
+      <c r="O338" s="13"/>
+      <c r="P338" s="13"/>
+      <c r="Q338" s="13"/>
+      <c r="R338" s="5"/>
+    </row>
+    <row r="339" spans="1:18">
+      <c r="A339" s="4"/>
+      <c r="B339" s="13"/>
+      <c r="C339" s="13"/>
+      <c r="D339" s="13"/>
+      <c r="E339" s="13"/>
+      <c r="F339" s="13"/>
+      <c r="G339" s="13"/>
+      <c r="H339" s="13"/>
+      <c r="I339" s="13"/>
+      <c r="J339" s="13"/>
+      <c r="K339" s="13"/>
+      <c r="L339" s="13"/>
+      <c r="M339" s="13"/>
+      <c r="N339" s="13"/>
+      <c r="O339" s="13"/>
+      <c r="P339" s="13"/>
+      <c r="Q339" s="13"/>
+      <c r="R339" s="5"/>
+    </row>
+    <row r="340" spans="1:18">
+      <c r="A340" s="4"/>
+      <c r="B340" s="13"/>
+      <c r="C340" s="13"/>
+      <c r="D340" s="13"/>
+      <c r="E340" s="13"/>
+      <c r="F340" s="13"/>
+      <c r="G340" s="13"/>
+      <c r="H340" s="13"/>
+      <c r="I340" s="13"/>
+      <c r="J340" s="13"/>
+      <c r="K340" s="13"/>
+      <c r="L340" s="13"/>
+      <c r="M340" s="13"/>
+      <c r="N340" s="13"/>
+      <c r="O340" s="13"/>
+      <c r="P340" s="13"/>
+      <c r="Q340" s="13"/>
+      <c r="R340" s="5"/>
+    </row>
+    <row r="341" spans="1:18">
+      <c r="A341" s="4"/>
+      <c r="B341" s="13"/>
+      <c r="C341" s="13"/>
+      <c r="D341" s="13"/>
+      <c r="E341" s="13"/>
+      <c r="F341" s="13"/>
+      <c r="G341" s="13"/>
+      <c r="H341" s="13"/>
+      <c r="I341" s="13"/>
+      <c r="J341" s="13"/>
+      <c r="K341" s="13"/>
+      <c r="L341" s="13"/>
+      <c r="M341" s="13"/>
+      <c r="N341" s="13"/>
+      <c r="O341" s="13"/>
+      <c r="P341" s="13"/>
+      <c r="Q341" s="13"/>
+      <c r="R341" s="5"/>
+    </row>
+    <row r="342" spans="1:18">
+      <c r="A342" s="4"/>
+      <c r="B342" s="13"/>
+      <c r="C342" s="13"/>
+      <c r="D342" s="13"/>
+      <c r="E342" s="13"/>
+      <c r="F342" s="13"/>
+      <c r="G342" s="13"/>
+      <c r="H342" s="13"/>
+      <c r="I342" s="13"/>
+      <c r="J342" s="13"/>
+      <c r="K342" s="13"/>
+      <c r="L342" s="13"/>
+      <c r="M342" s="13"/>
+      <c r="N342" s="13"/>
+      <c r="O342" s="13"/>
+      <c r="P342" s="13"/>
+      <c r="Q342" s="13"/>
+      <c r="R342" s="5"/>
+    </row>
+    <row r="343" spans="1:18">
+      <c r="A343" s="4"/>
+      <c r="B343" s="13"/>
+      <c r="C343" s="13"/>
+      <c r="D343" s="13"/>
+      <c r="E343" s="13"/>
+      <c r="F343" s="13"/>
+      <c r="G343" s="13"/>
+      <c r="H343" s="13"/>
+      <c r="I343" s="13"/>
+      <c r="J343" s="13"/>
+      <c r="K343" s="13"/>
+      <c r="L343" s="13"/>
+      <c r="M343" s="13"/>
+      <c r="N343" s="13"/>
+      <c r="O343" s="13"/>
+      <c r="P343" s="13"/>
+      <c r="Q343" s="13"/>
+      <c r="R343" s="5"/>
+    </row>
+    <row r="344" spans="1:18">
+      <c r="A344" s="4"/>
+      <c r="B344" s="13"/>
+      <c r="C344" s="13"/>
+      <c r="D344" s="13"/>
+      <c r="E344" s="13"/>
+      <c r="F344" s="13"/>
+      <c r="G344" s="13"/>
+      <c r="H344" s="13"/>
+      <c r="I344" s="13"/>
+      <c r="J344" s="13"/>
+      <c r="K344" s="13"/>
+      <c r="L344" s="13"/>
+      <c r="M344" s="13"/>
+      <c r="N344" s="13" t="s">
+        <v>340</v>
+      </c>
+      <c r="O344" s="13"/>
+      <c r="P344" s="13"/>
+      <c r="Q344" s="13"/>
+      <c r="R344" s="5"/>
+    </row>
+    <row r="345" spans="1:18">
+      <c r="A345" s="4"/>
+      <c r="B345" s="13"/>
+      <c r="C345" s="13"/>
+      <c r="D345" s="13"/>
+      <c r="E345" s="13"/>
+      <c r="F345" s="13"/>
+      <c r="G345" s="13"/>
+      <c r="H345" s="13"/>
+      <c r="I345" s="13"/>
+      <c r="J345" s="13"/>
+      <c r="K345" s="13"/>
+      <c r="L345" s="13"/>
+      <c r="M345" s="13"/>
+      <c r="N345" s="13"/>
+      <c r="O345" s="13"/>
+      <c r="P345" s="13"/>
+      <c r="Q345" s="13"/>
+      <c r="R345" s="5"/>
+    </row>
+    <row r="346" spans="1:18">
+      <c r="A346" s="4"/>
+      <c r="B346" s="13"/>
+      <c r="C346" s="13"/>
+      <c r="D346" s="13"/>
+      <c r="E346" s="13"/>
+      <c r="F346" s="13"/>
+      <c r="G346" s="13"/>
+      <c r="H346" s="13"/>
+      <c r="I346" s="13"/>
+      <c r="J346" s="13"/>
+      <c r="K346" s="13"/>
+      <c r="L346" s="13"/>
+      <c r="M346" s="13"/>
+      <c r="N346" s="13"/>
+      <c r="O346" s="13"/>
+      <c r="P346" s="13"/>
+      <c r="Q346" s="13"/>
+      <c r="R346" s="5"/>
+    </row>
+    <row r="347" spans="1:18">
+      <c r="A347" s="4"/>
+      <c r="B347" s="13"/>
+      <c r="C347" s="13"/>
+      <c r="D347" s="13"/>
+      <c r="E347" s="13"/>
+      <c r="F347" s="13"/>
+      <c r="G347" s="13"/>
+      <c r="H347" s="13"/>
+      <c r="I347" s="13"/>
+      <c r="J347" s="13"/>
+      <c r="K347" s="13"/>
+      <c r="L347" s="13"/>
+      <c r="M347" s="13"/>
+      <c r="N347" s="13"/>
+      <c r="O347" s="13"/>
+      <c r="P347" s="13"/>
+      <c r="Q347" s="13"/>
+      <c r="R347" s="5"/>
+    </row>
+    <row r="348" spans="1:18">
+      <c r="A348" s="4"/>
+      <c r="B348" s="13"/>
+      <c r="C348" s="13"/>
+      <c r="D348" s="13"/>
+      <c r="E348" s="13"/>
+      <c r="F348" s="13"/>
+      <c r="G348" s="13"/>
+      <c r="H348" s="13"/>
+      <c r="I348" s="13"/>
+      <c r="J348" s="13"/>
+      <c r="K348" s="13"/>
+      <c r="L348" s="13"/>
+      <c r="M348" s="13"/>
+      <c r="N348" s="13"/>
+      <c r="O348" s="13"/>
+      <c r="P348" s="13"/>
+      <c r="Q348" s="13"/>
+      <c r="R348" s="5"/>
+    </row>
+    <row r="349" spans="1:18">
+      <c r="A349" s="4"/>
+      <c r="B349" s="13"/>
+      <c r="C349" s="13"/>
+      <c r="D349" s="13"/>
+      <c r="E349" s="13"/>
+      <c r="F349" s="13"/>
+      <c r="G349" s="13"/>
+      <c r="H349" s="13"/>
+      <c r="I349" s="13"/>
+      <c r="J349" s="13"/>
+      <c r="K349" s="13"/>
+      <c r="L349" s="13"/>
+      <c r="M349" s="13"/>
+      <c r="N349" s="13"/>
+      <c r="O349" s="13"/>
+      <c r="P349" s="13"/>
+      <c r="Q349" s="13"/>
+      <c r="R349" s="5"/>
+    </row>
+    <row r="350" spans="1:18">
+      <c r="A350" s="4"/>
+      <c r="B350" s="13"/>
+      <c r="C350" s="13"/>
+      <c r="D350" s="13"/>
+      <c r="E350" s="13"/>
+      <c r="F350" s="13"/>
+      <c r="G350" s="13"/>
+      <c r="H350" s="13"/>
+      <c r="I350" s="13"/>
+      <c r="J350" s="13"/>
+      <c r="K350" s="13"/>
+      <c r="L350" s="13"/>
+      <c r="M350" s="13"/>
+      <c r="N350" s="13"/>
+      <c r="O350" s="13"/>
+      <c r="P350" s="13"/>
+      <c r="Q350" s="13"/>
+      <c r="R350" s="5"/>
+    </row>
+    <row r="351" spans="1:18">
+      <c r="A351" s="4"/>
+      <c r="B351" s="13"/>
+      <c r="C351" s="13"/>
+      <c r="D351" s="13"/>
+      <c r="E351" s="13"/>
+      <c r="F351" s="13"/>
+      <c r="G351" s="13"/>
+      <c r="H351" s="13"/>
+      <c r="I351" s="13"/>
+      <c r="J351" s="13"/>
+      <c r="K351" s="13"/>
+      <c r="L351" s="13"/>
+      <c r="M351" s="13"/>
+      <c r="N351" s="13"/>
+      <c r="O351" s="13"/>
+      <c r="P351" s="13"/>
+      <c r="Q351" s="13"/>
+      <c r="R351" s="5"/>
+    </row>
+    <row r="352" spans="1:18">
+      <c r="A352" s="7"/>
+      <c r="B352" s="8"/>
+      <c r="C352" s="8"/>
+      <c r="D352" s="8"/>
+      <c r="E352" s="8"/>
+      <c r="F352" s="8"/>
+      <c r="G352" s="8"/>
+      <c r="H352" s="8"/>
+      <c r="I352" s="8"/>
+      <c r="J352" s="8"/>
+      <c r="K352" s="8"/>
+      <c r="L352" s="8"/>
+      <c r="M352" s="8"/>
+      <c r="N352" s="8"/>
+      <c r="O352" s="8"/>
+      <c r="P352" s="8"/>
+      <c r="Q352" s="8"/>
+      <c r="R352" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>